<commit_message>
Updated latest changes to master 071718
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -5,33 +5,33 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\TestAutomation\FrameworkBase\src\main\java\testdata\LoadPay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="1000" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="1000" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
     <sheet name="AdminLogin" sheetId="9" r:id="rId2"/>
     <sheet name="AdminSearchData" sheetId="26" r:id="rId3"/>
     <sheet name="AdminLoginshipperaccountmodule" sheetId="32" r:id="rId4"/>
-    <sheet name="ShipperCompleteAccModuleData" sheetId="31" r:id="rId5"/>
-    <sheet name="BrokerProcessedTabSearchData" sheetId="33" r:id="rId6"/>
-    <sheet name="BrokerDiscountsTabSearchData" sheetId="34" r:id="rId7"/>
-    <sheet name="BrokerSchedPaymentTabSearchData" sheetId="35" r:id="rId8"/>
-    <sheet name="BrokerLoginData" sheetId="1" r:id="rId9"/>
-    <sheet name="BrokerRegister" sheetId="4" r:id="rId10"/>
-    <sheet name="BrokerUpdatePaymentData" sheetId="24" r:id="rId11"/>
-    <sheet name="BrokerNewPaymentData" sheetId="7" r:id="rId12"/>
-    <sheet name="BrokerPaymentDataforUnmatchedCr" sheetId="10" r:id="rId13"/>
-    <sheet name="BrokerRegisterCanada" sheetId="11" r:id="rId14"/>
-    <sheet name="BrokerBankingData" sheetId="15" r:id="rId15"/>
-    <sheet name="BrokerPaymentHistorydata" sheetId="30" r:id="rId16"/>
-    <sheet name="BrokerChangePasswordData" sheetId="27" r:id="rId17"/>
-    <sheet name="CarrierChangePasswordData" sheetId="36" r:id="rId18"/>
-    <sheet name="BrokerForgotPassword" sheetId="28" r:id="rId19"/>
-    <sheet name="AdminforcepasswordData" sheetId="39" r:id="rId20"/>
+    <sheet name="AdminforcepasswordData" sheetId="39" r:id="rId5"/>
+    <sheet name="ShipperCompleteAccModuleData" sheetId="31" r:id="rId6"/>
+    <sheet name="BrokerProcessedTabSearchData" sheetId="33" r:id="rId7"/>
+    <sheet name="BrokerDiscountsTabSearchData" sheetId="34" r:id="rId8"/>
+    <sheet name="BrokerSchedPaymentTabSearchData" sheetId="35" r:id="rId9"/>
+    <sheet name="BrokerLoginData" sheetId="1" r:id="rId10"/>
+    <sheet name="BrokerRegister" sheetId="4" r:id="rId11"/>
+    <sheet name="BrokerUpdatePaymentData" sheetId="24" r:id="rId12"/>
+    <sheet name="BrokerNewPaymentData" sheetId="7" r:id="rId13"/>
+    <sheet name="BrokerPaymentDataforUnmatchedCr" sheetId="10" r:id="rId14"/>
+    <sheet name="BrokerRegisterCanada" sheetId="11" r:id="rId15"/>
+    <sheet name="BrokerBankingData" sheetId="15" r:id="rId16"/>
+    <sheet name="BrokerPaymentHistorydata" sheetId="30" r:id="rId17"/>
+    <sheet name="BrokerForgotPassword" sheetId="28" r:id="rId18"/>
+    <sheet name="BrokerChangePasswordData" sheetId="27" r:id="rId19"/>
+    <sheet name="CarrierChangePasswordData" sheetId="36" r:id="rId20"/>
     <sheet name="CarrierForgotPasswordData" sheetId="37" r:id="rId21"/>
     <sheet name="CarrierRegisterData" sheetId="6" r:id="rId22"/>
     <sheet name="CarrierLoginData" sheetId="5" r:id="rId23"/>
@@ -675,7 +675,7 @@
     <t>carrierNewFramework4@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>brokerNewFramework2@loadpaytest.truckstop.com</t>
+    <t>brokerCVK071618A4@loadpaytest.truckstop.com</t>
   </si>
 </sst>
 </file>
@@ -1345,9 +1345,49 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1483,7 +1523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC2"/>
   <sheetViews>
@@ -1682,7 +1722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1731,7 +1771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1814,7 +1854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -1968,7 +2008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2017,7 +2057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -2080,7 +2120,63 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.25" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
+    <col min="4" max="4" width="25.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2130,116 +2226,6 @@
     <hyperlink ref="C2" r:id="rId2"/>
     <hyperlink ref="D2" r:id="rId3"/>
     <hyperlink ref="A2" r:id="rId4"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.25" customWidth="1"/>
-    <col min="3" max="3" width="20.75" customWidth="1"/>
-    <col min="4" max="4" width="25.25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -2289,28 +2275,29 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="C1" s="36" t="s">
+      <c r="A1" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>15</v>
+      <c r="D1" s="34" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2318,19 +2305,20 @@
         <v>139</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>139</v>
+        <v>197</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3933,6 +3921,58 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4017,7 +4057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4077,7 +4117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4137,7 +4177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4195,43 +4235,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Rest Assured jars and reduced Sonar warnings
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="1000" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="1000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -675,7 +675,7 @@
     <t>carrierNewFramework4@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>brokerCVK071618A4@loadpaytest.truckstop.com</t>
+    <t>brokerCVK071718A2@loadpaytest.truckstop.com</t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2828,8 +2828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2888,7 +2888,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="33">
-        <v>32002</v>
+        <v>149737</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>

</xml_diff>

<commit_message>
Added new wait objects to each class
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -1,55 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6F78832C-2174-4DB9-BA7C-6E97338B8800}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="1000" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" tabRatio="1000" firstSheet="31" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
-    <sheet name="AdminLogin" sheetId="9" r:id="rId2"/>
-    <sheet name="AdminSearchData" sheetId="26" r:id="rId3"/>
-    <sheet name="AdminLoginshipperaccountmodule" sheetId="32" r:id="rId4"/>
-    <sheet name="AdminforcepasswordData" sheetId="39" r:id="rId5"/>
+    <sheet name="AdminforcepasswordData" sheetId="39" r:id="rId2"/>
+    <sheet name="AdminLogin" sheetId="9" r:id="rId3"/>
+    <sheet name="AdminSearchData" sheetId="26" r:id="rId4"/>
+    <sheet name="AdminLoginshipperaccountmodule" sheetId="32" r:id="rId5"/>
     <sheet name="ShipperCompleteAccModuleData" sheetId="31" r:id="rId6"/>
     <sheet name="BrokerProcessedTabSearchData" sheetId="33" r:id="rId7"/>
     <sheet name="BrokerDiscountsTabSearchData" sheetId="34" r:id="rId8"/>
     <sheet name="BrokerSchedPaymentTabSearchData" sheetId="35" r:id="rId9"/>
     <sheet name="BrokerLoginData" sheetId="1" r:id="rId10"/>
     <sheet name="BrokerRegister" sheetId="4" r:id="rId11"/>
-    <sheet name="BrokerUpdatePaymentData" sheetId="24" r:id="rId12"/>
-    <sheet name="BrokerNewPaymentData" sheetId="7" r:id="rId13"/>
-    <sheet name="BrokerPaymentDataforUnmatchedCr" sheetId="10" r:id="rId14"/>
-    <sheet name="BrokerRegisterCanada" sheetId="11" r:id="rId15"/>
-    <sheet name="BrokerBankingData" sheetId="15" r:id="rId16"/>
-    <sheet name="BrokerPaymentHistorydata" sheetId="30" r:id="rId17"/>
+    <sheet name="BrokerDuplicateEmail" sheetId="47" r:id="rId12"/>
+    <sheet name="BrokerUpdatePaymentData" sheetId="24" r:id="rId13"/>
+    <sheet name="BrokerNewPaymentData" sheetId="7" r:id="rId14"/>
+    <sheet name="BrokerPaymentDataforUnmatchedCr" sheetId="10" r:id="rId15"/>
+    <sheet name="BrokerRegisterCanada" sheetId="11" r:id="rId16"/>
+    <sheet name="BrokerBankingData" sheetId="15" r:id="rId17"/>
     <sheet name="BrokerForgotPassword" sheetId="28" r:id="rId18"/>
-    <sheet name="BrokerChangePasswordData" sheetId="27" r:id="rId19"/>
-    <sheet name="CarrierChangePasswordData" sheetId="36" r:id="rId20"/>
-    <sheet name="CarrierForgotPasswordData" sheetId="37" r:id="rId21"/>
-    <sheet name="CarrierRegisterData" sheetId="6" r:id="rId22"/>
-    <sheet name="CarrierLoginData" sheetId="5" r:id="rId23"/>
-    <sheet name="CarrierLoginAccountModuleData" sheetId="38" r:id="rId24"/>
-    <sheet name="CarrierlockedaccountAdminUnlock" sheetId="19" r:id="rId25"/>
-    <sheet name="carrierparentchilddata" sheetId="20" r:id="rId26"/>
-    <sheet name="carrierresetpassworddata" sheetId="21" r:id="rId27"/>
-    <sheet name="CarrierFuelcardaccountNumbers" sheetId="13" r:id="rId28"/>
-    <sheet name="BulkUploadPaymentsmatched" sheetId="22" r:id="rId29"/>
-    <sheet name="BulkUploadPaymentsUnmatched" sheetId="23" r:id="rId30"/>
-    <sheet name="CcarrierMatchedPayByCheckPayMNW" sheetId="14" r:id="rId31"/>
-    <sheet name="CarrierRegisterCanada" sheetId="12" r:id="rId32"/>
-    <sheet name="CarrierPaidTabData" sheetId="17" r:id="rId33"/>
-    <sheet name="CarrierBankingData" sheetId="16" r:id="rId34"/>
-    <sheet name="CarrierPaymentHistorydata" sheetId="29" r:id="rId35"/>
-    <sheet name="CarrierSchedulePaymentTabData" sheetId="25" r:id="rId36"/>
-    <sheet name="Verificare" sheetId="2" state="hidden" r:id="rId37"/>
-    <sheet name="tasks" sheetId="3" state="hidden" r:id="rId38"/>
+    <sheet name="BrokerPaymentHistorydata" sheetId="30" r:id="rId19"/>
+    <sheet name="BrokerChangePasswordData" sheetId="27" r:id="rId20"/>
+    <sheet name="CarrierDuplicateEmail" sheetId="46" r:id="rId21"/>
+    <sheet name="CarrierChangePasswordData" sheetId="36" r:id="rId22"/>
+    <sheet name="CarrierForgotPasswordData" sheetId="37" r:id="rId23"/>
+    <sheet name="CarrierLoginData" sheetId="5" r:id="rId24"/>
+    <sheet name="CarrierRegisterData" sheetId="6" r:id="rId25"/>
+    <sheet name="LoginHandshakewithRTF_CarrierDa" sheetId="43" r:id="rId26"/>
+    <sheet name="RTFLogindata" sheetId="41" state="hidden" r:id="rId27"/>
+    <sheet name="CarrierLoginAccountModuleData" sheetId="38" r:id="rId28"/>
+    <sheet name="CarrierlockedaccountAdminUnlock" sheetId="19" r:id="rId29"/>
+    <sheet name="carrierparentchilddata" sheetId="20" r:id="rId30"/>
+    <sheet name="carrierresetpassworddata" sheetId="21" r:id="rId31"/>
+    <sheet name="CarrierFuelcardaccountNumbers" sheetId="13" r:id="rId32"/>
+    <sheet name="BulkUploadPaymentsmatched" sheetId="22" r:id="rId33"/>
+    <sheet name="BulkUploadPaymentsUnmatched" sheetId="23" r:id="rId34"/>
+    <sheet name="CcarrierMatchedPayByCheckPayMNW" sheetId="14" r:id="rId35"/>
+    <sheet name="CarrierRegisterCanada" sheetId="12" r:id="rId36"/>
+    <sheet name="CarrierPaidTabData" sheetId="17" r:id="rId37"/>
+    <sheet name="CarrierBankingData" sheetId="16" r:id="rId38"/>
+    <sheet name="CarrierPaymentHistorydata" sheetId="29" r:id="rId39"/>
+    <sheet name="CarrierSchedulePaymentTabData" sheetId="25" r:id="rId40"/>
+    <sheet name="BankAccountDetailsForCopyPaste" sheetId="40" r:id="rId41"/>
+    <sheet name="CreditAmount" sheetId="42" r:id="rId42"/>
+    <sheet name="RTFLogin" sheetId="45" r:id="rId43"/>
+    <sheet name="Verificare" sheetId="2" state="hidden" r:id="rId44"/>
+    <sheet name="tasks" sheetId="3" state="hidden" r:id="rId45"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -63,8 +71,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Yurii Merviak</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{44300FB3-8245-4534-9071-F06903D54E19}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yurii Merviak:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="216">
   <si>
     <t>Username</t>
   </si>
@@ -261,9 +303,6 @@
     <t>Password@1</t>
   </si>
   <si>
-    <t>brcanada1395@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>crcanada1416@loadpaytest.truckstop.com</t>
   </si>
   <si>
@@ -633,9 +672,6 @@
     <t>unmatched99CVK@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>unmatched90CVK@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>Jason Is Cool</t>
   </si>
   <si>
@@ -669,23 +705,65 @@
     <t>Password@91</t>
   </si>
   <si>
-    <t>Password@5</t>
-  </si>
-  <si>
-    <t>carrierNewFramework4@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>brokerCVK071718A2@loadpaytest.truckstop.com</t>
+    <t>brcanada139545@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>EmailId</t>
+  </si>
+  <si>
+    <t>AccountName</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>ConfirmAccountNumber</t>
+  </si>
+  <si>
+    <t>BrokerAccount</t>
+  </si>
+  <si>
+    <t>BrokerQANoBankAccount@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jasong </t>
+  </si>
+  <si>
+    <t>CreditAmount</t>
+  </si>
+  <si>
+    <t>jcglaser@yahoo.com</t>
+  </si>
+  <si>
+    <t>jg718242broker@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>jasong</t>
+  </si>
+  <si>
+    <t>yuriicarrierstage@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>carrierCVK072518A1@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>071218NP03</t>
+  </si>
+  <si>
+    <t>carrierCVK071118A7@loadpaytest.truckstop.com </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -728,6 +806,36 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF172B4D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Open Sans"/>
     </font>
   </fonts>
   <fills count="10">
@@ -959,7 +1067,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1024,6 +1132,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1306,20 +1425,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="14.75" customWidth="1"/>
     <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1327,7 +1446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -1337,27 +1456,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1365,33 +1484,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>203</v>
+    <row r="2" spans="1:2">
+      <c r="A2" s="15" t="s">
+        <v>172</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="14.25" customWidth="1"/>
     <col min="2" max="2" width="16.125" customWidth="1"/>
@@ -1410,7 +1528,7 @@
     <col min="17" max="17" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1463,7 +1581,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="4" customFormat="1">
       <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1471,10 +1589,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -1515,8 +1633,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1524,19 +1642,58 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B1083F-2C63-4FCE-9825-F3543005262F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="39.625" customWidth="1"/>
+    <col min="2" max="2" width="44.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29">
       <c r="A1" s="3" t="s">
         <v>62</v>
       </c>
@@ -1544,90 +1701,90 @@
         <v>37</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="AC1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" s="2" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>29</v>
@@ -1636,108 +1793,108 @@
         <v>456789</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="H2" s="16" t="s">
+      <c r="I2" s="16" t="s">
         <v>117</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>118</v>
       </c>
       <c r="J2" s="16" t="b">
         <v>1</v>
       </c>
       <c r="K2" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="L2" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="M2" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="N2" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="O2" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="O2" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="P2" s="16" t="s">
+      <c r="Q2" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="R2" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="S2" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="T2" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="U2" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="V2" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="W2" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="X2" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="Y2" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="Y2" s="16" t="s">
+      <c r="Z2" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA2" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="Z2" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="AA2" s="16" t="s">
+      <c r="AB2" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="AB2" s="16" t="s">
+      <c r="AC2" s="16" t="s">
         <v>134</v>
-      </c>
-      <c r="AC2" s="16" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="35.875" customWidth="1"/>
+    <col min="1" max="1" width="45.5" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="7" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -1751,41 +1908,44 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>173</v>
+    <row r="2" spans="1:4">
+      <c r="A2" s="49" t="s">
+        <v>209</v>
       </c>
       <c r="B2" s="4">
-        <v>2221</v>
+        <v>718237</v>
       </c>
       <c r="C2" s="4">
-        <v>2221</v>
+        <v>718237</v>
       </c>
       <c r="D2" s="4">
-        <v>1000</v>
+        <v>930</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="35.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -1805,9 +1965,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="4">
         <v>10041598</v>
@@ -1825,44 +1985,23 @@
         <v>295676689</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B3" s="4">
-        <v>10041599</v>
-      </c>
-      <c r="C3" s="4">
-        <v>10041599</v>
-      </c>
-      <c r="D3" s="4">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="10">
-        <v>295676689</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
@@ -1871,7 +2010,7 @@
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1936,7 +2075,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>20</v>
@@ -1945,10 +2084,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>65</v>
+        <v>199</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>65</v>
+        <v>199</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>44</v>
@@ -2001,22 +2140,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
@@ -2024,7 +2163,7 @@
     <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -2038,7 +2177,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
         <v>60</v>
       </c>
@@ -2057,15 +2196,71 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="39.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.25" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
+    <col min="4" max="4" width="25.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-1200-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-1200-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-1200-000003000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13.125" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -2074,44 +2269,44 @@
     <col min="5" max="6" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="41" t="s">
-        <v>68</v>
-      </c>
       <c r="D1" s="41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E1" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="41" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="41" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="A2" s="42">
         <v>100</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C2" s="4">
         <v>8564</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E2" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" s="43" t="s">
         <v>169</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2120,71 +2315,67 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="39.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.25" customWidth="1"/>
-    <col min="3" max="3" width="20.75" customWidth="1"/>
-    <col min="4" max="4" width="25.25" customWidth="1"/>
+    <col min="1" max="2" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-1300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
@@ -2192,93 +2383,96 @@
     <col min="4" max="4" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="D1" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="34" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-1000-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-1000-000002000000}"/>
+    <hyperlink ref="A2" r:id="rId4" xr:uid="{00000000-0004-0000-1000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8498A2-173A-4149-92D9-3958E39CAEBC}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5" customWidth="1"/>
+    <col min="2" max="2" width="40.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>34</v>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{154F057B-201F-4E7E-8E4E-91C54C91AB1E}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{02EE2114-EFD0-40CF-9F8B-F22941B577D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
@@ -2286,105 +2480,144 @@
     <col min="4" max="4" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="D1" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="34" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-1100-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-1100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="38.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-1400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="7" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{8EBDED6C-07C8-4E79-A462-166389A445A3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="13.75" customWidth="1"/>
@@ -2399,7 +2632,7 @@
     <col min="17" max="17" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2452,7 +2685,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="4" customFormat="1">
       <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
@@ -2460,10 +2693,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -2504,60 +2737,89 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{FF194B88-B472-4A0A-A310-2F323C81799B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16.5">
+      <c r="A2" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="36.125" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="2" max="2" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>155</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>197</v>
+    <row r="2" spans="1:2" ht="16.5">
+      <c r="A2" s="47" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
@@ -2565,7 +2827,7 @@
     <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -2573,18 +2835,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C2" s="4">
         <v>8085</v>
@@ -2595,65 +2857,103 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>139</v>
+      <c r="B1" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.875" customWidth="1"/>
@@ -2661,7 +2961,7 @@
     <col min="4" max="4" width="39.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -2669,44 +2969,44 @@
         <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-1A00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
@@ -2714,60 +3014,60 @@
     <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="B2" r:id="rId3"/>
-    <hyperlink ref="D2" r:id="rId4"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-1B00-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{00000000-0004-0000-1B00-000002000000}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{00000000-0004-0000-1B00-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>50</v>
       </c>
@@ -2775,7 +3075,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="4">
         <v>6542988</v>
       </c>
@@ -2789,29 +3089,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="4">
         <v>100</v>
       </c>
@@ -2824,15 +3124,425 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4">
+        <v>500</v>
+      </c>
+      <c r="B2" s="4">
+        <v>501</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="12">
+        <v>374657000000</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="4">
+        <v>102101645</v>
+      </c>
+      <c r="T2" s="12">
+        <v>456457000000</v>
+      </c>
+      <c r="U2" s="12">
+        <v>456457000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-2100-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-2100-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="4">
+        <v>333.33</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="51" t="s">
+        <v>214</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{52FAD71A-44A8-4EF0-BA56-799A9566A000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="4">
+        <v>101000187</v>
+      </c>
+      <c r="C2" s="4">
+        <v>123456789</v>
+      </c>
+      <c r="D2" s="4">
+        <v>123456789</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="38">
+        <v>100</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="39">
+        <v>241</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:L17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
@@ -2848,75 +3558,75 @@
     <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="16.5" thickBot="1">
       <c r="A1" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="C1" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="F1" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="J1" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="K1" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="L1" s="32" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="33">
-        <v>149737</v>
+        <v>32002</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="F2" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="25"/>
       <c r="B3" s="18">
         <v>100</v>
@@ -2927,256 +3637,256 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L3" s="26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="25"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>155</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L4" s="26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="25"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L5" s="26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="25"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G6" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="G6" s="18" t="s">
-        <v>153</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L6" s="26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="25"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>153</v>
-      </c>
       <c r="I7" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L7" s="26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="25"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I8" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>153</v>
-      </c>
       <c r="J8" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L8" s="26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="25"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>153</v>
-      </c>
       <c r="K9" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="25"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="K10" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>153</v>
-      </c>
       <c r="L10" s="26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="16.5" thickBot="1">
       <c r="A11" s="25"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="L11" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="L11" s="27" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="20">
         <v>33343</v>
       </c>
@@ -3185,28 +3895,28 @@
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="G12" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="G12" s="23" t="s">
-        <v>153</v>
-      </c>
       <c r="H12" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L12" s="24" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="25">
         <v>33310</v>
       </c>
@@ -3215,28 +3925,28 @@
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H13" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>153</v>
-      </c>
       <c r="I13" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L13" s="26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="25">
         <v>33558</v>
       </c>
@@ -3245,28 +3955,28 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I14" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>153</v>
-      </c>
       <c r="J14" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L14" s="26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="25">
         <v>33280</v>
       </c>
@@ -3275,28 +3985,28 @@
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="J15" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>153</v>
-      </c>
       <c r="K15" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L15" s="26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="25">
         <v>33307</v>
       </c>
@@ -3305,28 +4015,28 @@
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="K16" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="K16" s="18" t="s">
-        <v>153</v>
-      </c>
       <c r="L16" s="26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="16.5" thickBot="1">
       <c r="A17" s="28">
         <v>8140</v>
       </c>
@@ -3335,25 +4045,25 @@
       <c r="D17" s="30"/>
       <c r="E17" s="30"/>
       <c r="F17" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="I17" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="L17" s="31" t="s">
         <v>152</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="I17" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="J17" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="K17" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="L17" s="31" t="s">
-        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3362,425 +4072,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>500</v>
-      </c>
-      <c r="B2" s="4">
-        <v>501</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="34.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="12">
-        <v>374657000000</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="4">
-        <v>102101645</v>
-      </c>
-      <c r="T2" s="12">
-        <v>456457000000</v>
-      </c>
-      <c r="U2" s="12">
-        <v>456457000000</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1234.56</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="4">
-        <v>101000187</v>
-      </c>
-      <c r="C2" s="4">
-        <v>123456789</v>
-      </c>
-      <c r="D2" s="4">
-        <v>123456789</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>167</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="38">
-        <v>100</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="39">
-        <v>241</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" s="40" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>170</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="31.625" customWidth="1"/>
     <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
@@ -3790,7 +4090,7 @@
     <col min="6" max="6" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>62</v>
       </c>
@@ -3798,62 +4098,190 @@
         <v>63</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D2" s="4">
         <v>1234.56</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-2500-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-2500-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" customHeight="1">
+      <c r="A2" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="46">
+        <v>122105155</v>
+      </c>
+      <c r="E2" s="46">
+        <v>123456789</v>
+      </c>
+      <c r="F2" s="46">
+        <v>123456789</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="15.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="48" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="35.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3861,7 +4289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3871,45 +4299,45 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="mailto:Admin1@calpion.com"/>
-    <hyperlink ref="A2" r:id="rId2" display="mailto:Admin1@calpion.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="mailto:Admin1@calpion.com" xr:uid="{00000000-0004-0000-2900-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" display="mailto:Admin1@calpion.com" xr:uid="{00000000-0004-0000-2900-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="44" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" s="13">
         <v>1000</v>
       </c>
@@ -3919,67 +4347,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="38.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
@@ -3991,7 +4367,7 @@
     <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3999,42 +4375,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="F2" s="4">
         <v>1111111111</v>
@@ -4051,21 +4427,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="33.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
@@ -4074,29 +4450,29 @@
     <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -4110,7 +4486,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -4118,14 +4494,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
@@ -4134,29 +4510,29 @@
     <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -4170,7 +4546,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -4178,14 +4554,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
@@ -4194,29 +4570,29 @@
     <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -4230,7 +4606,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Migrated new test data input sheet
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,57 +8,57 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3E3AE3AE-13F8-4D0B-9636-C86B78D495E8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CA031FDB-7E64-42CB-AF79-8135FDF844E1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" tabRatio="1000" firstSheet="25" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" tabRatio="1000" firstSheet="37" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
     <sheet name="ITSDispatchLoginData" sheetId="48" r:id="rId2"/>
-    <sheet name="RTFLogin" sheetId="45" r:id="rId3"/>
+    <sheet name="AdminforcepasswordData" sheetId="39" r:id="rId3"/>
     <sheet name="AdminLogin" sheetId="9" r:id="rId4"/>
     <sheet name="AdminSearchData" sheetId="26" r:id="rId5"/>
-    <sheet name="AdminforcepasswordData" sheetId="39" r:id="rId6"/>
-    <sheet name="AdminLoginshipperaccountmodule" sheetId="32" r:id="rId7"/>
-    <sheet name="ShipperCompleteAccModuleData" sheetId="31" r:id="rId8"/>
-    <sheet name="BrokerProcessedTabSearchData" sheetId="33" r:id="rId9"/>
-    <sheet name="BrokerDiscountsTabSearchData" sheetId="34" r:id="rId10"/>
-    <sheet name="BrokerSchedPaymentTabSearchData" sheetId="35" r:id="rId11"/>
-    <sheet name="BrokerLoginData" sheetId="1" r:id="rId12"/>
-    <sheet name="BrokerRegister" sheetId="4" r:id="rId13"/>
-    <sheet name="BrokerDuplicateEmail" sheetId="47" r:id="rId14"/>
-    <sheet name="BrokerUpdatePaymentData" sheetId="24" r:id="rId15"/>
-    <sheet name="BrokerUpdatedPaymentData" sheetId="49" r:id="rId16"/>
-    <sheet name="BrokerNewPaymentData" sheetId="7" r:id="rId17"/>
-    <sheet name="BrokerPaymentDataforUnmatchedCr" sheetId="10" r:id="rId18"/>
-    <sheet name="BrokerRegisterCanada" sheetId="11" r:id="rId19"/>
-    <sheet name="BrokerBankingData" sheetId="15" r:id="rId20"/>
-    <sheet name="BrokerForgotPassword" sheetId="28" r:id="rId21"/>
-    <sheet name="BrokerPaymentHistorydata" sheetId="30" r:id="rId22"/>
-    <sheet name="BrokerChangePasswordData" sheetId="27" r:id="rId23"/>
-    <sheet name="BankAccountDetailsForCopyPaste" sheetId="40" r:id="rId24"/>
-    <sheet name="CarrierDuplicateEmail" sheetId="46" r:id="rId25"/>
-    <sheet name="CarrierChangePasswordData" sheetId="36" r:id="rId26"/>
-    <sheet name="CarrierForgotPasswordData" sheetId="37" r:id="rId27"/>
-    <sheet name="CarrierLoginData" sheetId="5" r:id="rId28"/>
-    <sheet name="CarrierRegisterData" sheetId="6" r:id="rId29"/>
-    <sheet name="CarrierUpdatePaymentData" sheetId="50" r:id="rId30"/>
-    <sheet name="LoginHandshakewithRTF_CarrierDa" sheetId="43" r:id="rId31"/>
-    <sheet name="RTFLogindata" sheetId="41" state="hidden" r:id="rId32"/>
-    <sheet name="CarrierLoginAccountModuleData" sheetId="38" r:id="rId33"/>
-    <sheet name="CarrierlockedaccountAdminUnlock" sheetId="19" r:id="rId34"/>
-    <sheet name="carrierparentchilddata" sheetId="20" r:id="rId35"/>
-    <sheet name="carrierresetpassworddata" sheetId="21" r:id="rId36"/>
-    <sheet name="CarrierFuelcardaccountNumbers" sheetId="13" r:id="rId37"/>
-    <sheet name="BulkUploadPaymentsmatched" sheetId="22" r:id="rId38"/>
-    <sheet name="BulkUploadPaymentsUnmatched" sheetId="23" r:id="rId39"/>
-    <sheet name="CcarrierMatchedPayByCheckPayMNW" sheetId="14" r:id="rId40"/>
-    <sheet name="CarrierRegisterCanada" sheetId="12" r:id="rId41"/>
-    <sheet name="CarrierPaidTabData" sheetId="17" r:id="rId42"/>
-    <sheet name="CarrierBankingData" sheetId="16" r:id="rId43"/>
-    <sheet name="CarrierPaymentHistorydata" sheetId="29" r:id="rId44"/>
-    <sheet name="CarrierSchedulePaymentTabData" sheetId="25" r:id="rId45"/>
-    <sheet name="CreditAmount" sheetId="42" r:id="rId46"/>
+    <sheet name="AdminLoginshipperaccountmodule" sheetId="32" r:id="rId6"/>
+    <sheet name="ShipperCompleteAccModuleData" sheetId="31" r:id="rId7"/>
+    <sheet name="BrokerProcessedTabSearchData" sheetId="33" r:id="rId8"/>
+    <sheet name="BrokerDiscountsTabSearchData" sheetId="34" r:id="rId9"/>
+    <sheet name="BrokerSchedPaymentTabSearchData" sheetId="35" r:id="rId10"/>
+    <sheet name="BrokerLoginData" sheetId="1" r:id="rId11"/>
+    <sheet name="BrokerRegister" sheetId="4" r:id="rId12"/>
+    <sheet name="BrokerDuplicateEmail" sheetId="47" r:id="rId13"/>
+    <sheet name="BrokerUpdatePaymentData" sheetId="24" r:id="rId14"/>
+    <sheet name="BrokerUpdatedPaymentData" sheetId="49" r:id="rId15"/>
+    <sheet name="BrokerNewPaymentData" sheetId="7" r:id="rId16"/>
+    <sheet name="BrokerPaymentDataforUnmatchedCr" sheetId="10" r:id="rId17"/>
+    <sheet name="BrokerRegisterCanada" sheetId="11" r:id="rId18"/>
+    <sheet name="BrokerBankingData" sheetId="15" r:id="rId19"/>
+    <sheet name="BrokerForgotPassword" sheetId="28" r:id="rId20"/>
+    <sheet name="BrokerPaymentHistorydata" sheetId="30" r:id="rId21"/>
+    <sheet name="BrokerChangePasswordData" sheetId="27" r:id="rId22"/>
+    <sheet name="CarrierDuplicateEmail" sheetId="46" r:id="rId23"/>
+    <sheet name="CarrierChangePasswordData" sheetId="36" r:id="rId24"/>
+    <sheet name="CarrierForgotPasswordData" sheetId="37" r:id="rId25"/>
+    <sheet name="CarrierLoginData" sheetId="5" r:id="rId26"/>
+    <sheet name="CarrierRegisterData" sheetId="6" r:id="rId27"/>
+    <sheet name="CarrierUpdatePaymentData" sheetId="50" r:id="rId28"/>
+    <sheet name="LoginHandshakewithRTF_CarrierDa" sheetId="43" r:id="rId29"/>
+    <sheet name="RTFLogindata" sheetId="41" state="hidden" r:id="rId30"/>
+    <sheet name="CarrierLoginAccountModuleData" sheetId="38" r:id="rId31"/>
+    <sheet name="CarrierlockedaccountAdminUnlock" sheetId="19" r:id="rId32"/>
+    <sheet name="carrierparentchilddata" sheetId="20" r:id="rId33"/>
+    <sheet name="carrierresetpassworddata" sheetId="21" r:id="rId34"/>
+    <sheet name="CarrierFuelcardaccountNumbers" sheetId="13" r:id="rId35"/>
+    <sheet name="BulkUploadPaymentsmatched" sheetId="22" r:id="rId36"/>
+    <sheet name="BulkUploadPaymentsUnmatched" sheetId="23" r:id="rId37"/>
+    <sheet name="CcarrierMatchedPayByCheckPayMNW" sheetId="14" r:id="rId38"/>
+    <sheet name="CarrierRegisterCanada" sheetId="12" r:id="rId39"/>
+    <sheet name="CarrierPaidTabData" sheetId="17" r:id="rId40"/>
+    <sheet name="CarrierBankingData" sheetId="16" r:id="rId41"/>
+    <sheet name="CarrierPaymentHistorydata" sheetId="29" r:id="rId42"/>
+    <sheet name="CarrierSchedulePaymentTabData" sheetId="25" r:id="rId43"/>
+    <sheet name="BankAccountDetailsForCopyPaste" sheetId="40" r:id="rId44"/>
+    <sheet name="CreditAmount" sheetId="42" r:id="rId45"/>
+    <sheet name="RTFLogin" sheetId="45" r:id="rId46"/>
     <sheet name="Verificare" sheetId="2" state="hidden" r:id="rId47"/>
     <sheet name="tasks" sheetId="3" state="hidden" r:id="rId48"/>
   </sheets>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="224">
   <si>
     <t>Username</t>
   </si>
@@ -705,6 +705,9 @@
     <t>Password@91</t>
   </si>
   <si>
+    <t>brcanada139545@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
     <t>EmailId</t>
   </si>
   <si>
@@ -762,34 +765,22 @@
     <t>321456</t>
   </si>
   <si>
-    <t>brCanadaCVK01@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>carrierCVK073018X03@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>080118X03</t>
-  </si>
-  <si>
-    <t>080118X04</t>
-  </si>
-  <si>
-    <t>carrierCVK080118X03@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>brokerCVK080118X03@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>brokerCVK080118X05@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>unmatchedCVK080118@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>80118Z01</t>
-  </si>
-  <si>
-    <t>carrierCVK080118X05@loadpaytest.truckstop.com</t>
+    <t>unmatched01AK@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>carrierAK01@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>jg718242broker125@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>jcglaser@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -1168,8 +1159,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1490,66 +1483,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="4">
-        <v>110</v>
-      </c>
-      <c r="E2" s="4">
-        <v>230</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1609,12 +1542,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1632,24 +1565,24 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>222</v>
+      <c r="A2" s="15" t="s">
+        <v>172</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{A2CC20E9-3DA4-44BF-A2F2-EE2A2BF6BE17}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{B62A179D-BC10-4F8A-81D5-C80430FC8A99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -1737,10 +1670,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -1781,15 +1714,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{117DB727-8BB8-4590-8484-378A16B21942}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{40D4F1D4-B52F-45C8-B39B-457540DC6C82}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{55440022-35C2-4C46-A0B1-CCB9FB423F6A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B1083F-2C63-4FCE-9825-F3543005262F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1807,7 +1740,7 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1828,7 +1761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
@@ -2030,12 +1963,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F80A14-7D04-448E-8D00-2F385D5F98CA}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2049,7 +1982,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>89</v>
@@ -2067,7 +2000,7 @@
         <v>87</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>91</v>
@@ -2075,16 +2008,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E2" s="4">
         <v>1234587</v>
@@ -2107,17 +2040,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.5" customWidth="1"/>
+    <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
@@ -2137,49 +2070,45 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>218</v>
+      <c r="A2" s="49" t="s">
+        <v>223</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D2" s="4">
-        <v>456</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
-        <v>218</v>
+      <c r="A3" s="49" t="s">
+        <v>223</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D3" s="4">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{D8987F63-9E63-4056-8EA2-008B70352B1E}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{E91DD1BB-216D-4DAD-A771-F23511D32A73}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2210,16 +2139,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>225</v>
+        <v>218</v>
+      </c>
+      <c r="B2" s="4">
+        <v>10041515</v>
+      </c>
+      <c r="C2" s="4">
+        <v>10041515</v>
       </c>
       <c r="D2" s="4">
-        <v>789</v>
+        <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>38</v>
@@ -2236,12 +2165,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2327,10 +2256,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>44</v>
@@ -2384,56 +2313,13 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{45BD0E3E-08B7-44E5-8CCF-965C56D3B272}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59E68DCD-E1C6-4AD9-B92C-49D8D397AE38}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2482,7 +2368,50 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59E68DCD-E1C6-4AD9-B92C-49D8D397AE38}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2538,7 +2467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -2601,7 +2530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2657,71 +2586,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>199</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>200</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>202</v>
-      </c>
-      <c r="D2" s="46">
-        <v>122105155</v>
-      </c>
-      <c r="E2" s="46">
-        <v>123456789</v>
-      </c>
-      <c r="F2" s="46">
-        <v>123456789</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8498A2-173A-4149-92D9-3958E39CAEBC}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2745,10 +2610,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2762,7 +2627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2816,7 +2681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2868,12 +2733,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2891,23 +2756,22 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>221</v>
+      <c r="A2" s="49" t="s">
+        <v>223</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{5D14EB07-44AB-47D1-BB5C-B6FF68B313E6}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{DF5E700E-7839-4D46-8BFA-3F24C340437E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -2984,9 +2848,6 @@
       </c>
     </row>
     <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1234567</v>
-      </c>
       <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
@@ -2994,10 +2855,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -3039,49 +2900,13 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{DFF619DA-CFF9-4B15-B42A-F7A91033B0DE}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{1E74D2BC-3532-4C14-8C5E-7ABF9A3D7EC0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B750627-6F23-4CDD-9F53-6ABD7DC947B5}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -3100,7 +2925,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>89</v>
@@ -3118,7 +2943,7 @@
         <v>87</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>91</v>
@@ -3126,16 +2951,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E2" s="4">
         <v>1234587</v>
@@ -3158,7 +2983,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3178,10 +3003,10 @@
     </row>
     <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3189,7 +3014,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-1300-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3213,10 +3090,10 @@
     </row>
     <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3225,7 +3102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3277,7 +3154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3321,7 +3198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3374,7 +3251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3429,7 +3306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3465,7 +3342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3500,7 +3377,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3535,45 +3412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3610,7 +3449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -3767,7 +3606,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3835,7 +3712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3884,7 +3761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3948,7 +3825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -4015,7 +3892,71 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" s="46">
+        <v>122105155</v>
+      </c>
+      <c r="E2" s="46">
+        <v>123456789</v>
+      </c>
+      <c r="F2" s="46">
+        <v>123456789</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -4030,7 +3971,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -4040,6 +3981,42 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4634,58 +4611,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="38.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-1300-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -4713,7 +4638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -4799,7 +4724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4857,4 +4782,64 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="4">
+        <v>110</v>
+      </c>
+      <c r="E2" s="4">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
XML updates and smart wait added
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3E27D42A-BB21-43AC-98A0-40CFF2AB41F5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EC71C98C-1B20-4A55-8A12-63490377DE04}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" tabRatio="1000" firstSheet="14" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" tabRatio="1000" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -27,8 +27,8 @@
     <sheet name="BrokerRegister" sheetId="4" r:id="rId12"/>
     <sheet name="BrokerDuplicateEmail" sheetId="47" r:id="rId13"/>
     <sheet name="BrokerUpdatePaymentData" sheetId="24" r:id="rId14"/>
-    <sheet name="BrokerUpdatedPaymentData" sheetId="49" r:id="rId15"/>
-    <sheet name="BrokerNewPaymentData" sheetId="7" r:id="rId16"/>
+    <sheet name="BrokerNewPaymentData" sheetId="7" r:id="rId15"/>
+    <sheet name="BrokerUpdatedPaymentData" sheetId="49" r:id="rId16"/>
     <sheet name="BrokerPaymentDataforUnmatchedCr" sheetId="10" r:id="rId17"/>
     <sheet name="BrokerRegisterCanada" sheetId="11" r:id="rId18"/>
     <sheet name="BrokerBankingData" sheetId="15" r:id="rId19"/>
@@ -774,16 +774,16 @@
     <t>jcglaser@yahoo.com</t>
   </si>
   <si>
-    <t>umCVK080618A01@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>080618A01UM</t>
-  </si>
-  <si>
-    <t>080618A01</t>
-  </si>
-  <si>
-    <t>080618A02</t>
+    <t>080718A01UM</t>
+  </si>
+  <si>
+    <t>umCVK080718A01@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>080718A07</t>
+  </si>
+  <si>
+    <t>080718A08</t>
   </si>
 </sst>
 </file>
@@ -1967,6 +1967,69 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" s="4">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F80A14-7D04-448E-8D00-2F385D5F98CA}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -2043,75 +2106,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>220</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="D2" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
-        <v>220</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="D3" s="4">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2142,13 +2142,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>222</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D2" s="4">
         <v>123.45</v>

</xml_diff>

<commit_message>
O Sprint Updates 080818
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EC71C98C-1B20-4A55-8A12-63490377DE04}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E6105A8B-4594-4548-A17D-7185518AABE5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" tabRatio="1000" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="229">
   <si>
     <t>Username</t>
   </si>
@@ -705,9 +705,6 @@
     <t>Password@91</t>
   </si>
   <si>
-    <t>brcanada139545@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>EmailId</t>
   </si>
   <si>
@@ -765,25 +762,40 @@
     <t>321456</t>
   </si>
   <si>
-    <t>carrierAK01@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>jg718242broker125@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>jcglaser@yahoo.com</t>
-  </si>
-  <si>
-    <t>080718A01UM</t>
-  </si>
-  <si>
-    <t>umCVK080718A01@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>080718A07</t>
-  </si>
-  <si>
-    <t>080718A08</t>
+    <t>brokerCaCVK080718A02@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>Password@5</t>
+  </si>
+  <si>
+    <t>carrierCVK080818CC01@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>carrierCVK080818CC02@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>brokerCVK080818BB01@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>umCarrierCVK080818U03@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>080818UM07</t>
+  </si>
+  <si>
+    <t>080818UM08</t>
+  </si>
+  <si>
+    <t>carrierCVK080818CC03@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>080818CC09</t>
+  </si>
+  <si>
+    <t>080818CC10</t>
+  </si>
+  <si>
+    <t>brokerCVK080818AK12@loadpaytest.truckstop.com</t>
   </si>
 </sst>
 </file>
@@ -1162,10 +1174,8 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1550,7 +1560,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1568,17 +1578,17 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>172</v>
+      <c r="A2" s="2" t="s">
+        <v>221</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{B62A179D-BC10-4F8A-81D5-C80430FC8A99}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{56E72764-36AC-4EBC-8D3A-0A59E2F99D22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1589,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1673,10 +1683,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -1717,8 +1727,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{55440022-35C2-4C46-A0B1-CCB9FB423F6A}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{03A1FFB6-0600-4511-A735-BCFC5DFB1015}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{1C3F2681-4CEE-45F6-9627-5EC68BE74A5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1743,7 +1753,7 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="49" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1970,13 +1980,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
@@ -1996,36 +2006,40 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>220</v>
+      <c r="A2" s="2" t="s">
+        <v>219</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D2" s="4">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
-        <v>220</v>
+      <c r="A3" s="2" t="s">
+        <v>219</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D3" s="4">
         <v>200</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E0AF94C3-9F3B-4AA1-8DE8-E5C6B400BE18}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{565D9B7D-90DD-4D44-B6D0-456658EF1252}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2048,7 +2062,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>89</v>
@@ -2066,7 +2080,7 @@
         <v>87</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>91</v>
@@ -2074,16 +2088,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>215</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>216</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E2" s="4">
         <v>1234587</v>
@@ -2108,15 +2122,16 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2145,10 +2160,10 @@
         <v>222</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D2" s="4">
         <v>123.45</v>
@@ -2160,9 +2175,30 @@
         <v>295676689</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" s="4">
+        <v>456.78</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="10">
+        <v>295676689</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{17ECB252-F6A9-4FD4-9508-2EC92DCF0622}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{BFB88CDD-BC03-4DFD-9A20-381D943B636F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2173,7 +2209,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2259,10 +2295,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>44</v>
@@ -2315,8 +2351,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{B252F9C7-03C1-4E9A-A8E9-AF276250EA75}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{BFF31301-BAE2-40D4-B6A4-33364DA2AC30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2388,7 +2424,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>155</v>
@@ -2399,13 +2435,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -2613,10 +2649,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2741,7 +2777,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2759,16 +2795,17 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DF5E700E-7839-4D46-8BFA-3F24C340437E}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{25236D84-96CB-4CC1-9812-532B4A593D4F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2779,7 +2816,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2858,10 +2895,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -2902,8 +2939,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{1E74D2BC-3532-4C14-8C5E-7ABF9A3D7EC0}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{F80E385F-FAF1-4F90-A236-2F28AFA509E0}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{8E5655BA-F6C9-4F12-AD5A-F92673770305}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2928,7 +2965,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>89</v>
@@ -2946,7 +2983,7 @@
         <v>87</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>91</v>
@@ -2954,16 +2991,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E2" s="4">
         <v>1234587</v>
@@ -3006,10 +3043,10 @@
     </row>
     <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3093,10 +3130,10 @@
     </row>
     <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3636,7 +3673,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -3900,12 +3937,12 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
@@ -3915,33 +3952,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D1" s="37" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="F1" s="37" t="s">
-        <v>202</v>
-      </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>204</v>
+      <c r="A2" s="50" t="s">
+        <v>203</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D2" s="46">
         <v>122105155</v>
@@ -3954,8 +3991,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6CC7F1F0-F045-4027-9BDD-7D1CDE871892}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3974,7 +4014,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -4011,10 +4051,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated test data spread sheet with payments greater than 45 days tab
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChristopherVonKaenel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{798DE15D-7136-45BD-B08A-BE0AAB8B158E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F90AA31D-BE1A-4DC6-9DDB-AC0756A4DE2D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="1000" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -19,48 +19,50 @@
     <sheet name="AdminLogin" sheetId="9" r:id="rId4"/>
     <sheet name="AdminSearchData" sheetId="26" r:id="rId5"/>
     <sheet name="AdminLoginshipperaccountmodule" sheetId="32" r:id="rId6"/>
-    <sheet name="ShipperCompleteAccModuleData" sheetId="31" r:id="rId7"/>
-    <sheet name="BrokerProcessedTabSearchData" sheetId="33" r:id="rId8"/>
-    <sheet name="BrokerDiscountsTabSearchData" sheetId="34" r:id="rId9"/>
-    <sheet name="BrokerSchedPaymentTabSearchData" sheetId="35" r:id="rId10"/>
-    <sheet name="BrokerLoginData" sheetId="1" r:id="rId11"/>
-    <sheet name="BrokerRegister" sheetId="4" r:id="rId12"/>
-    <sheet name="BrokerDuplicateEmail" sheetId="47" r:id="rId13"/>
-    <sheet name="BrokerUpdatePaymentData" sheetId="24" r:id="rId14"/>
-    <sheet name="BrokerNewPaymentData" sheetId="7" r:id="rId15"/>
-    <sheet name="BrokerUpdatedPaymentData" sheetId="49" r:id="rId16"/>
-    <sheet name="BrokerPaymentDataforUnmatchedCr" sheetId="10" r:id="rId17"/>
-    <sheet name="BrokerRegisterCanada" sheetId="11" r:id="rId18"/>
-    <sheet name="BrokerBankingData" sheetId="15" r:id="rId19"/>
-    <sheet name="BrokerForgotPassword" sheetId="28" r:id="rId20"/>
-    <sheet name="BrokerPaymentHistorydata" sheetId="30" r:id="rId21"/>
-    <sheet name="BrokerChangePasswordData" sheetId="27" r:id="rId22"/>
-    <sheet name="CarrierDuplicateEmail" sheetId="46" r:id="rId23"/>
-    <sheet name="CarrierChangePasswordData" sheetId="36" r:id="rId24"/>
-    <sheet name="CarrierForgotPasswordData" sheetId="37" r:id="rId25"/>
-    <sheet name="CarrierLoginData" sheetId="5" r:id="rId26"/>
-    <sheet name="CarrierRegisterData" sheetId="6" r:id="rId27"/>
-    <sheet name="CarrierUpdatePaymentData" sheetId="50" r:id="rId28"/>
-    <sheet name="LoginHandshakewithRTF_CarrierDa" sheetId="43" r:id="rId29"/>
-    <sheet name="RTFLogindata" sheetId="41" state="hidden" r:id="rId30"/>
-    <sheet name="CarrierLoginAccountModuleData" sheetId="38" r:id="rId31"/>
-    <sheet name="CarrierlockedaccountAdminUnlock" sheetId="19" r:id="rId32"/>
-    <sheet name="carrierparentchilddata" sheetId="20" r:id="rId33"/>
-    <sheet name="carrierresetpassworddata" sheetId="21" r:id="rId34"/>
-    <sheet name="CarrierFuelcardaccountNumbers" sheetId="13" r:id="rId35"/>
-    <sheet name="BulkUploadPaymentsmatched" sheetId="22" r:id="rId36"/>
-    <sheet name="BulkUploadPaymentsUnmatched" sheetId="23" r:id="rId37"/>
-    <sheet name="CcarrierMatchedPayByCheckPayMNW" sheetId="14" r:id="rId38"/>
-    <sheet name="CarrierRegisterCanada" sheetId="12" r:id="rId39"/>
-    <sheet name="CarrierPaidTabData" sheetId="17" r:id="rId40"/>
-    <sheet name="CarrierBankingData" sheetId="16" r:id="rId41"/>
-    <sheet name="CarrierPaymentHistorydata" sheetId="29" r:id="rId42"/>
-    <sheet name="CarrierSchedulePaymentTabData" sheetId="25" r:id="rId43"/>
-    <sheet name="BankAccountDetailsForCopyPaste" sheetId="40" r:id="rId44"/>
-    <sheet name="CreditAmount" sheetId="42" r:id="rId45"/>
-    <sheet name="RTFLogin" sheetId="45" r:id="rId46"/>
-    <sheet name="Verificare" sheetId="2" state="hidden" r:id="rId47"/>
-    <sheet name="tasks" sheetId="3" state="hidden" r:id="rId48"/>
+    <sheet name="AdminPaymentsGreaterthan45Days" sheetId="51" r:id="rId7"/>
+    <sheet name="ShipperCompleteAccModuleData" sheetId="31" r:id="rId8"/>
+    <sheet name="BrokerProcessedTabSearchData" sheetId="33" r:id="rId9"/>
+    <sheet name="BrokerDiscountsTabSearchData" sheetId="34" r:id="rId10"/>
+    <sheet name="BrokerSchedPaymentTabSearchData" sheetId="35" r:id="rId11"/>
+    <sheet name="BrokerLoginData" sheetId="1" r:id="rId12"/>
+    <sheet name="BrokerRegister" sheetId="4" r:id="rId13"/>
+    <sheet name="BrokerDuplicateEmail" sheetId="47" r:id="rId14"/>
+    <sheet name="BrokerUpdatePaymentData" sheetId="24" r:id="rId15"/>
+    <sheet name="BrokerNewPaymentData" sheetId="7" r:id="rId16"/>
+    <sheet name="payementmorethan45daysData" sheetId="52" r:id="rId17"/>
+    <sheet name="BrokerUpdatedPaymentData" sheetId="49" r:id="rId18"/>
+    <sheet name="BrokerPaymentDataforUnmatchedCr" sheetId="10" r:id="rId19"/>
+    <sheet name="BrokerRegisterCanada" sheetId="11" r:id="rId20"/>
+    <sheet name="BrokerBankingData" sheetId="15" r:id="rId21"/>
+    <sheet name="BrokerForgotPassword" sheetId="28" r:id="rId22"/>
+    <sheet name="BrokerPaymentHistorydata" sheetId="30" r:id="rId23"/>
+    <sheet name="BrokerChangePasswordData" sheetId="27" r:id="rId24"/>
+    <sheet name="CarrierDuplicateEmail" sheetId="46" r:id="rId25"/>
+    <sheet name="CarrierChangePasswordData" sheetId="36" r:id="rId26"/>
+    <sheet name="CarrierForgotPasswordData" sheetId="37" r:id="rId27"/>
+    <sheet name="CarrierLoginData" sheetId="5" r:id="rId28"/>
+    <sheet name="CarrierRegisterData" sheetId="6" r:id="rId29"/>
+    <sheet name="CarrierUpdatePaymentData" sheetId="50" r:id="rId30"/>
+    <sheet name="LoginHandshakewithRTF_CarrierDa" sheetId="43" r:id="rId31"/>
+    <sheet name="RTFLogindata" sheetId="41" state="hidden" r:id="rId32"/>
+    <sheet name="CarrierLoginAccountModuleData" sheetId="38" r:id="rId33"/>
+    <sheet name="CarrierlockedaccountAdminUnlock" sheetId="19" r:id="rId34"/>
+    <sheet name="carrierparentchilddata" sheetId="20" r:id="rId35"/>
+    <sheet name="carrierresetpassworddata" sheetId="21" r:id="rId36"/>
+    <sheet name="CarrierFuelcardaccountNumbers" sheetId="13" r:id="rId37"/>
+    <sheet name="BulkUploadPaymentsmatched" sheetId="22" r:id="rId38"/>
+    <sheet name="BulkUploadPaymentsUnmatched" sheetId="23" r:id="rId39"/>
+    <sheet name="CcarrierMatchedPayByCheckPayMNW" sheetId="14" r:id="rId40"/>
+    <sheet name="CarrierRegisterCanada" sheetId="12" r:id="rId41"/>
+    <sheet name="CarrierPaidTabData" sheetId="17" r:id="rId42"/>
+    <sheet name="CarrierBankingData" sheetId="16" r:id="rId43"/>
+    <sheet name="CarrierPaymentHistorydata" sheetId="29" r:id="rId44"/>
+    <sheet name="CarrierSchedulePaymentTabData" sheetId="25" r:id="rId45"/>
+    <sheet name="BankAccountDetailsForCopyPaste" sheetId="40" r:id="rId46"/>
+    <sheet name="CreditAmount" sheetId="42" r:id="rId47"/>
+    <sheet name="RTFLogin" sheetId="45" r:id="rId48"/>
+    <sheet name="Verificare" sheetId="2" state="hidden" r:id="rId49"/>
+    <sheet name="tasks" sheetId="3" state="hidden" r:id="rId50"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -109,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="232">
   <si>
     <t>Username</t>
   </si>
@@ -264,9 +266,6 @@
     <t>fleet_accountnbr</t>
   </si>
   <si>
-    <t>Cgihrms@1234</t>
-  </si>
-  <si>
     <t>Anilkumar</t>
   </si>
   <si>
@@ -765,15 +764,9 @@
     <t>brokerCaCVK080718A02@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>Password@5</t>
-  </si>
-  <si>
     <t>carrierCVK080818CC01@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>brokerCVK080818BB01@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>umCarrierCVK080818U03@loadpaytest.truckstop.com</t>
   </si>
   <si>
@@ -793,6 +786,27 @@
   </si>
   <si>
     <t>080918CC18</t>
+  </si>
+  <si>
+    <t>scheduledate</t>
+  </si>
+  <si>
+    <t>10/27/2018</t>
+  </si>
+  <si>
+    <t>carrierregister62@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>Cgihrms@12345</t>
+  </si>
+  <si>
+    <t>080918ak36</t>
+  </si>
+  <si>
+    <t>080918ak37</t>
+  </si>
+  <si>
+    <t>08/20/2019</t>
   </si>
 </sst>
 </file>
@@ -1459,13 +1473,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" customWidth="1"/>
-    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1481,7 +1495,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -1493,6 +1507,66 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="4">
+        <v>110</v>
+      </c>
+      <c r="E2" s="4">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1511,27 +1585,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="45" t="s">
         <v>191</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>192</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -1552,12 +1626,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1576,23 +1650,22 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>220</v>
+        <v>171</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{56E72764-36AC-4EBC-8D3A-0A59E2F99D22}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{36D1AB56-994A-4224-85CB-F76B2C177D99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -1680,10 +1753,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -1732,7 +1805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B1083F-2C63-4FCE-9825-F3543005262F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1756,10 +1829,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1771,7 +1844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
@@ -1789,96 +1862,96 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>29</v>
@@ -1887,82 +1960,82 @@
         <v>456789</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="H2" s="16" t="s">
+      <c r="I2" s="16" t="s">
         <v>116</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>117</v>
       </c>
       <c r="J2" s="16" t="b">
         <v>1</v>
       </c>
       <c r="K2" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="M2" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="N2" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="O2" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="O2" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="P2" s="16" t="s">
+      <c r="Q2" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="R2" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="S2" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="T2" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="U2" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="V2" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="W2" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="X2" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="Y2" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="Y2" s="16" t="s">
+      <c r="Z2" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA2" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="Z2" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="AA2" s="16" t="s">
+      <c r="AB2" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="AB2" s="16" t="s">
+      <c r="AC2" s="16" t="s">
         <v>133</v>
-      </c>
-      <c r="AC2" s="16" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1973,12 +2046,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2004,13 +2077,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D2" s="4">
         <v>100</v>
@@ -2018,13 +2091,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D3" s="4">
         <v>200</v>
@@ -2036,7 +2109,62 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D59054-07F3-4D98-89C6-3D3B72291E7D}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.5" customWidth="1"/>
+    <col min="2" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F80A14-7D04-448E-8D00-2F385D5F98CA}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -2055,10 +2183,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>37</v>
@@ -2067,42 +2195,42 @@
         <v>31</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>214</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>215</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E2" s="4">
         <v>1234587</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2113,12 +2241,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2150,13 +2278,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D2" s="4">
         <v>123.45</v>
@@ -2170,13 +2298,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D3" s="4">
         <v>456.78</v>
@@ -2197,7 +2325,50 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59E68DCD-E1C6-4AD9-B92C-49D8D397AE38}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -2288,10 +2459,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>44</v>
@@ -2351,7 +2522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2369,21 +2540,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4">
         <v>101200453</v>
@@ -2400,50 +2571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59E68DCD-E1C6-4AD9-B92C-49D8D397AE38}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2464,10 +2592,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>15</v>
@@ -2475,16 +2603,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2499,7 +2627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -2518,22 +2646,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="41" t="s">
-        <v>67</v>
-      </c>
       <c r="D1" s="41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E1" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="41" t="s">
         <v>166</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2541,19 +2669,19 @@
         <v>100</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C2" s="4">
         <v>8564</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E2" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="43" t="s">
         <v>168</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2562,7 +2690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2580,30 +2708,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="D1" s="34" t="s">
         <v>157</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2618,7 +2746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8498A2-173A-4149-92D9-3958E39CAEBC}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2642,10 +2770,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2659,7 +2787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2677,30 +2805,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="D1" s="34" t="s">
         <v>157</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2713,7 +2841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2733,10 +2861,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>15</v>
@@ -2744,16 +2872,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2765,12 +2893,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2789,7 +2917,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
@@ -2798,13 +2926,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DF5E700E-7839-4D46-8BFA-3F24C340437E}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{25236D84-96CB-4CC1-9812-532B4A593D4F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -2888,10 +3015,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -2939,7 +3066,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-1300-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B750627-6F23-4CDD-9F53-6ABD7DC947B5}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -2958,10 +3137,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>37</v>
@@ -2970,42 +3149,42 @@
         <v>31</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E2" s="4">
         <v>1234587</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -3016,7 +3195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3036,10 +3215,10 @@
     </row>
     <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3047,59 +3226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="38.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-1300-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3115,7 +3242,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3123,10 +3250,10 @@
     </row>
     <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3135,7 +3262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3159,7 +3286,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>39</v>
@@ -3167,10 +3294,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C2" s="4">
         <v>8085</v>
@@ -3187,7 +3314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3209,18 +3336,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3231,7 +3358,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3255,10 +3382,10 @@
         <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3266,13 +3393,13 @@
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3284,7 +3411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3302,30 +3429,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3339,7 +3466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3375,7 +3502,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3391,10 +3518,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3410,7 +3537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3426,10 +3553,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3445,7 +3572,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3463,18 +3628,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3482,7 +3647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -3576,10 +3741,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>44</v>
@@ -3639,45 +3804,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3697,42 +3824,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" s="4">
         <v>1234.56</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3745,7 +3872,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3763,21 +3890,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="4">
         <v>101000187</v>
@@ -3794,7 +3921,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3814,22 +3941,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="37" t="s">
-        <v>67</v>
-      </c>
       <c r="D1" s="37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E1" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>166</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3837,19 +3964,19 @@
         <v>100</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" s="39">
         <v>241</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E2" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="40" t="s">
         <v>168</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3858,7 +3985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3878,42 +4005,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D2" s="4">
         <v>1234.56</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3925,7 +4052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3945,33 +4072,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D1" s="37" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>200</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D2" s="46">
         <v>122105155</v>
@@ -3992,7 +4119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -4007,7 +4134,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -4020,7 +4147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -4036,7 +4163,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -4044,10 +4171,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -4056,7 +4183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -4093,18 +4220,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4134,40 +4249,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="C1" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="F1" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="J1" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="K1" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>149</v>
-      </c>
-      <c r="L1" s="32" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4179,25 +4294,25 @@
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="F2" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4211,25 +4326,25 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L3" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -4237,31 +4352,31 @@
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>154</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L4" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -4271,25 +4386,25 @@
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L5" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -4299,25 +4414,25 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G6" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="G6" s="18" t="s">
-        <v>152</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L6" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -4327,25 +4442,25 @@
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>152</v>
-      </c>
       <c r="I7" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L7" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -4355,25 +4470,25 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I8" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>152</v>
-      </c>
       <c r="J8" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L8" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -4383,25 +4498,25 @@
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>152</v>
-      </c>
       <c r="K9" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -4411,25 +4526,25 @@
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K10" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>152</v>
-      </c>
       <c r="L10" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4439,25 +4554,25 @@
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L11" s="27" t="s">
         <v>151</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="L11" s="27" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -4469,25 +4584,25 @@
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="G12" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="G12" s="23" t="s">
-        <v>152</v>
-      </c>
       <c r="H12" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L12" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -4499,25 +4614,25 @@
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H13" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>152</v>
-      </c>
       <c r="I13" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L13" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -4529,25 +4644,25 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I14" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>152</v>
-      </c>
       <c r="J14" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L14" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -4559,25 +4674,25 @@
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J15" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>152</v>
-      </c>
       <c r="K15" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L15" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -4589,25 +4704,25 @@
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K16" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="K16" s="18" t="s">
-        <v>152</v>
-      </c>
       <c r="L16" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4619,30 +4734,42 @@
       <c r="D17" s="30"/>
       <c r="E17" s="30"/>
       <c r="F17" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="I17" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="L17" s="31" t="s">
         <v>151</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="I17" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="J17" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="K17" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="L17" s="31" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4661,7 +4788,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -4675,6 +4802,61 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C3BC51-A396-415F-9233-1E72E8DB73EF}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.625" customWidth="1"/>
+    <col min="2" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -4702,42 +4884,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="F2" s="4">
         <v>1111111111</v>
@@ -4760,7 +4942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4779,27 +4961,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -4818,64 +5000,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="4">
-        <v>110</v>
-      </c>
-      <c r="E2" s="4">
-        <v>230</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated Psprint.xml and Test Data
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A19D4A54-6C55-4009-B06A-039FC0362F80}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{528B5818-DA4F-4B31-B663-84B802AAD0D9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="43" activeTab="48" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="23" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -2753,7 +2753,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2899,8 +2899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2919,10 +2919,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>227</v>
+        <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -4189,8 +4189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE248A60-C3BD-412F-B50B-074B69CAE368}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated master with Admin Customers Side Menu Search tests
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -5,73 +5,71 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{528B5818-DA4F-4B31-B663-84B802AAD0D9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{02673BDB-BBEB-40EA-B64F-90DE27B3FC57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="23" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="1000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
     <sheet name="ITSDispatchLoginData" sheetId="48" r:id="rId2"/>
     <sheet name="AdminforcepasswordData" sheetId="39" r:id="rId3"/>
     <sheet name="AdminLogin" sheetId="9" r:id="rId4"/>
-    <sheet name="AdminSearchData" sheetId="26" r:id="rId5"/>
-    <sheet name="AdminLoginshipperaccountmodule" sheetId="32" r:id="rId6"/>
-    <sheet name="ShipperCompleteAccModuleData" sheetId="31" r:id="rId7"/>
-    <sheet name="BrokerProcessedTabSearchData" sheetId="33" r:id="rId8"/>
-    <sheet name="BrokerDiscountsTabSearchData" sheetId="34" r:id="rId9"/>
-    <sheet name="BrokerSchedPaymentTabSearchData" sheetId="35" r:id="rId10"/>
-    <sheet name="BrokerLoginData" sheetId="1" r:id="rId11"/>
-    <sheet name="BrokerRegister" sheetId="4" r:id="rId12"/>
-    <sheet name="BrokerDuplicateEmail" sheetId="47" r:id="rId13"/>
-    <sheet name="BrokerUpdatePaymentData" sheetId="24" r:id="rId14"/>
-    <sheet name="BrokerNewPaymentData" sheetId="7" r:id="rId15"/>
-    <sheet name="AdminPaymentsGreaterthan45Days" sheetId="51" r:id="rId16"/>
-    <sheet name="payementmorethan45daysData" sheetId="52" r:id="rId17"/>
-    <sheet name="BrokerUpdatedPaymentData" sheetId="49" r:id="rId18"/>
-    <sheet name="BrokerPaymentDataforUnmatchedCr" sheetId="10" r:id="rId19"/>
-    <sheet name="BrokerRegisterCanada" sheetId="11" r:id="rId20"/>
-    <sheet name="BrokerBankingData" sheetId="15" r:id="rId21"/>
-    <sheet name="BrokerForgotPassword" sheetId="28" r:id="rId22"/>
-    <sheet name="BrokerPaymentHistorydata" sheetId="30" r:id="rId23"/>
-    <sheet name="BrokerChangePasswordData" sheetId="27" r:id="rId24"/>
-    <sheet name="CarrierDuplicateEmail" sheetId="46" r:id="rId25"/>
-    <sheet name="CarrierChangePasswordData" sheetId="36" r:id="rId26"/>
-    <sheet name="CarrierForgotPasswordData" sheetId="37" r:id="rId27"/>
-    <sheet name="CarrierLoginData" sheetId="5" r:id="rId28"/>
-    <sheet name="CarrierRegisterData" sheetId="6" r:id="rId29"/>
-    <sheet name="CarrierUpdatePaymentData" sheetId="50" r:id="rId30"/>
-    <sheet name="LoginHandshakewithRTF_CarrierDa" sheetId="43" r:id="rId31"/>
-    <sheet name="RTFLogindata" sheetId="41" state="hidden" r:id="rId32"/>
-    <sheet name="CarrierLoginAccountModuleData" sheetId="38" r:id="rId33"/>
-    <sheet name="CarrierlockedaccountAdminUnlock" sheetId="19" r:id="rId34"/>
-    <sheet name="carrierparentchilddata" sheetId="20" r:id="rId35"/>
-    <sheet name="carrierresetpassworddata" sheetId="21" r:id="rId36"/>
-    <sheet name="CarrierFuelcardaccountNumbers" sheetId="13" r:id="rId37"/>
-    <sheet name="BulkUploadPaymentsmatched" sheetId="22" r:id="rId38"/>
-    <sheet name="BulkUploadPaymentsUnmatched" sheetId="23" r:id="rId39"/>
-    <sheet name="CcarrierMatchedPayByCheckPayMNW" sheetId="14" r:id="rId40"/>
-    <sheet name="CarrierRegisterCanada" sheetId="12" r:id="rId41"/>
-    <sheet name="CarrierPaidTabData" sheetId="17" r:id="rId42"/>
-    <sheet name="CarrierBankingData" sheetId="16" r:id="rId43"/>
-    <sheet name="CarrierPaymentHistorydata" sheetId="29" r:id="rId44"/>
-    <sheet name="CarrierSchedulePaymentTabData" sheetId="25" r:id="rId45"/>
-    <sheet name="BankAccountDetailsForCopyPaste" sheetId="40" r:id="rId46"/>
-    <sheet name="CreditAmount" sheetId="42" r:id="rId47"/>
-    <sheet name="RTFLogin" sheetId="45" r:id="rId48"/>
-    <sheet name="CarrierBankAccountDetails" sheetId="53" r:id="rId49"/>
-    <sheet name="Verificare" sheetId="2" state="hidden" r:id="rId50"/>
-    <sheet name="tasks" sheetId="3" state="hidden" r:id="rId51"/>
+    <sheet name="AdminCustomersSideMenSearchData" sheetId="54" r:id="rId5"/>
+    <sheet name="AdminSearchData" sheetId="26" r:id="rId6"/>
+    <sheet name="AdminLoginshipperaccountmodule" sheetId="32" r:id="rId7"/>
+    <sheet name="ShipperCompleteAccModuleData" sheetId="31" r:id="rId8"/>
+    <sheet name="BrokerProcessedTabSearchData" sheetId="33" r:id="rId9"/>
+    <sheet name="BrokerDiscountsTabSearchData" sheetId="34" r:id="rId10"/>
+    <sheet name="BrokerSchedPaymentTabSearchData" sheetId="35" r:id="rId11"/>
+    <sheet name="BrokerLoginData" sheetId="1" r:id="rId12"/>
+    <sheet name="BrokerRegister" sheetId="4" r:id="rId13"/>
+    <sheet name="BrokerDuplicateEmail" sheetId="47" r:id="rId14"/>
+    <sheet name="BrokerUpdatePaymentData" sheetId="24" r:id="rId15"/>
+    <sheet name="BrokerNewPaymentData" sheetId="7" r:id="rId16"/>
+    <sheet name="AdminPaymentsGreaterthan45Days" sheetId="51" r:id="rId17"/>
+    <sheet name="payementmorethan45daysData" sheetId="52" r:id="rId18"/>
+    <sheet name="BrokerUpdatedPaymentData" sheetId="49" r:id="rId19"/>
+    <sheet name="BrokerPaymentDataforUnmatchedCr" sheetId="10" r:id="rId20"/>
+    <sheet name="BrokerRegisterCanada" sheetId="11" r:id="rId21"/>
+    <sheet name="BrokerBankingData" sheetId="15" r:id="rId22"/>
+    <sheet name="BrokerForgotPassword" sheetId="28" r:id="rId23"/>
+    <sheet name="BrokerPaymentHistorydata" sheetId="30" r:id="rId24"/>
+    <sheet name="BrokerChangePasswordData" sheetId="27" r:id="rId25"/>
+    <sheet name="CarrierDuplicateEmail" sheetId="46" r:id="rId26"/>
+    <sheet name="CarrierChangePasswordData" sheetId="36" r:id="rId27"/>
+    <sheet name="CarrierForgotPasswordData" sheetId="37" r:id="rId28"/>
+    <sheet name="CarrierLoginData" sheetId="5" r:id="rId29"/>
+    <sheet name="CarrierRegisterData" sheetId="6" r:id="rId30"/>
+    <sheet name="CarrierUpdatePaymentData" sheetId="50" r:id="rId31"/>
+    <sheet name="LoginHandshakewithRTF_CarrierDa" sheetId="43" r:id="rId32"/>
+    <sheet name="RTFLogindata" sheetId="41" state="hidden" r:id="rId33"/>
+    <sheet name="CarrierLoginAccountModuleData" sheetId="38" r:id="rId34"/>
+    <sheet name="CarrierlockedaccountAdminUnlock" sheetId="19" r:id="rId35"/>
+    <sheet name="carrierparentchilddata" sheetId="20" r:id="rId36"/>
+    <sheet name="carrierresetpassworddata" sheetId="21" r:id="rId37"/>
+    <sheet name="CarrierFuelcardaccountNumbers" sheetId="13" r:id="rId38"/>
+    <sheet name="BulkUploadPaymentsmatched" sheetId="22" r:id="rId39"/>
+    <sheet name="BulkUploadPaymentsUnmatched" sheetId="23" r:id="rId40"/>
+    <sheet name="CcarrierMatchedPayByCheckPayMNW" sheetId="14" r:id="rId41"/>
+    <sheet name="CarrierRegisterCanada" sheetId="12" r:id="rId42"/>
+    <sheet name="CarrierPaidTabData" sheetId="17" r:id="rId43"/>
+    <sheet name="CarrierBankingData" sheetId="16" r:id="rId44"/>
+    <sheet name="CarrierPaymentHistorydata" sheetId="29" r:id="rId45"/>
+    <sheet name="CarrierSchedulePaymentTabData" sheetId="25" r:id="rId46"/>
+    <sheet name="BankAccountDetailsForCopyPaste" sheetId="40" r:id="rId47"/>
+    <sheet name="CreditAmount" sheetId="42" r:id="rId48"/>
+    <sheet name="RTFLogin" sheetId="45" r:id="rId49"/>
+    <sheet name="CarrierBankAccountDetails" sheetId="53" r:id="rId50"/>
+    <sheet name="Verificare" sheetId="2" state="hidden" r:id="rId51"/>
+    <sheet name="tasks" sheetId="3" state="hidden" r:id="rId52"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -112,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="239">
   <si>
     <t>Username</t>
   </si>
@@ -814,6 +812,21 @@
   </si>
   <si>
     <t>CarrierAccount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Company Name</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email </t>
+  </si>
+  <si>
+    <t>shantesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brokerym123456@loadpaytest.truckstop.com </t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1135,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1194,6 +1207,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1483,13 +1500,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.75" customWidth="1"/>
-    <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.69921875" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1497,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -1514,6 +1531,66 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="4">
+        <v>110</v>
+      </c>
+      <c r="E2" s="4">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1521,16 +1598,16 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>183</v>
       </c>
@@ -1547,7 +1624,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>190</v>
       </c>
@@ -1573,7 +1650,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1581,13 +1658,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1595,7 +1672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>171</v>
       </c>
@@ -1612,7 +1689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -1620,26 +1697,26 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.25" customWidth="1"/>
-    <col min="2" max="2" width="16.125" customWidth="1"/>
-    <col min="3" max="3" width="17.875" customWidth="1"/>
-    <col min="4" max="4" width="35.75" customWidth="1"/>
-    <col min="5" max="5" width="36.375" customWidth="1"/>
-    <col min="6" max="6" width="12.875" customWidth="1"/>
-    <col min="9" max="9" width="11.875" customWidth="1"/>
-    <col min="10" max="10" width="12.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="15.25" customWidth="1"/>
-    <col min="13" max="13" width="14.75" customWidth="1"/>
-    <col min="14" max="14" width="15.875" customWidth="1"/>
-    <col min="15" max="15" width="15.25" customWidth="1"/>
-    <col min="16" max="16" width="16.25" customWidth="1"/>
+    <col min="1" max="1" width="14.19921875" customWidth="1"/>
+    <col min="2" max="2" width="16.09765625" customWidth="1"/>
+    <col min="3" max="3" width="17.8984375" customWidth="1"/>
+    <col min="4" max="4" width="35.69921875" customWidth="1"/>
+    <col min="5" max="5" width="36.3984375" customWidth="1"/>
+    <col min="6" max="6" width="12.8984375" customWidth="1"/>
+    <col min="9" max="9" width="11.8984375" customWidth="1"/>
+    <col min="10" max="10" width="12.09765625" customWidth="1"/>
+    <col min="11" max="11" width="14.3984375" customWidth="1"/>
+    <col min="12" max="12" width="15.19921875" customWidth="1"/>
+    <col min="13" max="13" width="14.69921875" customWidth="1"/>
+    <col min="14" max="14" width="15.8984375" customWidth="1"/>
+    <col min="15" max="15" width="15.19921875" customWidth="1"/>
+    <col min="16" max="16" width="16.19921875" customWidth="1"/>
     <col min="17" max="17" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1692,7 +1769,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1752,7 +1829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B1083F-2C63-4FCE-9825-F3543005262F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1760,13 +1837,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.625" customWidth="1"/>
-    <col min="2" max="2" width="44.25" customWidth="1"/>
+    <col min="1" max="1" width="39.59765625" customWidth="1"/>
+    <col min="2" max="2" width="44.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1774,7 +1851,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>158</v>
       </c>
@@ -1791,7 +1868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
@@ -1799,15 +1876,15 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>61</v>
       </c>
@@ -1896,7 +1973,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>111</v>
       </c>
@@ -1993,7 +2070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2001,14 +2078,14 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.69921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -2022,7 +2099,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>217</v>
       </c>
@@ -2036,7 +2113,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>217</v>
       </c>
@@ -2056,7 +2133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C3BC51-A396-415F-9233-1E72E8DB73EF}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2064,15 +2141,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.625" customWidth="1"/>
-    <col min="2" max="3" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.59765625" customWidth="1"/>
+    <col min="2" max="3" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -2089,7 +2166,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>227</v>
       </c>
@@ -2111,7 +2188,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D59054-07F3-4D98-89C6-3D3B72291E7D}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2119,15 +2196,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.5" customWidth="1"/>
-    <col min="2" max="3" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -2144,7 +2221,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>227</v>
       </c>
@@ -2166,7 +2243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F80A14-7D04-448E-8D00-2F385D5F98CA}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -2174,16 +2251,16 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>197</v>
       </c>
@@ -2209,7 +2286,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>213</v>
       </c>
@@ -2238,90 +2315,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{74225089-1083-4CA4-873D-523BC11F8FAF}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="D2" s="4">
-        <v>123.45</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="10">
-        <v>295676689</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="D3" s="4">
-        <v>456.78</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="10">
-        <v>295676689</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{17ECB252-F6A9-4FD4-9508-2EC92DCF0622}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{BFB88CDD-BC03-4DFD-9A20-381D943B636F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2335,14 +2328,14 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>208</v>
       </c>
@@ -2353,7 +2346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>209</v>
       </c>
@@ -2371,6 +2364,90 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="39.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.8984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D2" s="4">
+        <v>123.45</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="10">
+        <v>295676689</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="4">
+        <v>456.78</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="10">
+        <v>295676689</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{17ECB252-F6A9-4FD4-9508-2EC92DCF0622}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{BFB88CDD-BC03-4DFD-9A20-381D943B636F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -2378,16 +2455,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="35.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="35.19921875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2452,7 +2529,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>20</v>
@@ -2524,7 +2601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2532,15 +2609,15 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>55</v>
       </c>
@@ -2554,7 +2631,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>59</v>
       </c>
@@ -2573,7 +2650,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2581,15 +2658,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.25" customWidth="1"/>
-    <col min="3" max="3" width="20.75" customWidth="1"/>
-    <col min="4" max="4" width="25.25" customWidth="1"/>
+    <col min="1" max="1" width="39.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.19921875" customWidth="1"/>
+    <col min="3" max="3" width="20.69921875" customWidth="1"/>
+    <col min="4" max="4" width="25.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -2603,7 +2680,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>160</v>
       </c>
@@ -2629,7 +2706,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -2637,16 +2714,16 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.125" customWidth="1"/>
+    <col min="1" max="1" width="13.09765625" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
         <v>69</v>
       </c>
@@ -2666,7 +2743,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="42">
         <v>100</v>
       </c>
@@ -2692,7 +2769,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2700,15 +2777,15 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.625" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" customWidth="1"/>
+    <col min="4" max="4" width="17.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
         <v>154</v>
       </c>
@@ -2722,7 +2799,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>158</v>
       </c>
@@ -2748,7 +2825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8498A2-173A-4149-92D9-3958E39CAEBC}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2756,13 +2833,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.5" customWidth="1"/>
-    <col min="2" max="2" width="40.75" customWidth="1"/>
+    <col min="2" max="2" width="40.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -2770,7 +2847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>207</v>
       </c>
@@ -2789,7 +2866,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2797,15 +2874,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
         <v>154</v>
       </c>
@@ -2819,7 +2896,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>137</v>
       </c>
@@ -2843,7 +2920,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2851,14 +2928,14 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -2872,7 +2949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>137</v>
       </c>
@@ -2895,21 +2972,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -2917,7 +2994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>76</v>
       </c>
@@ -2928,141 +3005,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DF5E700E-7839-4D46-8BFA-3F24C340437E}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
-  <dimension ref="A1:Q2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="13.75" customWidth="1"/>
-    <col min="3" max="3" width="10.25" customWidth="1"/>
-    <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="35.875" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="11" max="12" width="14.625" customWidth="1"/>
-    <col min="13" max="13" width="15.5" customWidth="1"/>
-    <col min="15" max="15" width="13.75" customWidth="1"/>
-    <col min="16" max="16" width="12.625" customWidth="1"/>
-    <col min="17" max="17" width="13" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="5">
-        <v>374657342938</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="4">
-        <v>102101645</v>
-      </c>
-      <c r="P2" s="5">
-        <v>456456567567</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>456456567567</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{F80E385F-FAF1-4F90-A236-2F28AFA509E0}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{8E5655BA-F6C9-4F12-AD5A-F92673770305}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3076,14 +3018,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="38.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -3097,7 +3039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>137</v>
       </c>
@@ -3121,6 +3063,141 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="13.69921875" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" customWidth="1"/>
+    <col min="4" max="4" width="36" customWidth="1"/>
+    <col min="5" max="5" width="35.8984375" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="11" max="12" width="14.59765625" customWidth="1"/>
+    <col min="13" max="13" width="15.5" customWidth="1"/>
+    <col min="15" max="15" width="13.69921875" customWidth="1"/>
+    <col min="16" max="16" width="12.59765625" customWidth="1"/>
+    <col min="17" max="17" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="5">
+        <v>374657342938</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="4">
+        <v>102101645</v>
+      </c>
+      <c r="P2" s="5">
+        <v>456456567567</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>456456567567</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{F80E385F-FAF1-4F90-A236-2F28AFA509E0}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{8E5655BA-F6C9-4F12-AD5A-F92673770305}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B750627-6F23-4CDD-9F53-6ABD7DC947B5}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -3128,16 +3205,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>197</v>
       </c>
@@ -3163,7 +3240,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>213</v>
       </c>
@@ -3197,7 +3274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3205,9 +3282,9 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3215,7 +3292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A2" s="47" t="s">
         <v>206</v>
       </c>
@@ -3228,7 +3305,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3236,13 +3313,13 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
+    <col min="2" max="2" width="15.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>154</v>
       </c>
@@ -3250,7 +3327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A2" s="47" t="s">
         <v>204</v>
       </c>
@@ -3264,7 +3341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3272,15 +3349,15 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -3294,7 +3371,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>137</v>
       </c>
@@ -3316,7 +3393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3324,13 +3401,13 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -3341,7 +3418,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>137</v>
       </c>
@@ -3360,7 +3437,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3368,15 +3445,15 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="1" max="1" width="9.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.8984375" customWidth="1"/>
     <col min="3" max="3" width="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -3390,7 +3467,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
@@ -3413,7 +3490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3421,15 +3498,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>77</v>
       </c>
@@ -3443,7 +3520,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>83</v>
       </c>
@@ -3468,7 +3545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3476,13 +3553,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>50</v>
       </c>
@@ -3490,7 +3567,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>6542988</v>
       </c>
@@ -3504,7 +3581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3512,13 +3589,13 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>81</v>
       </c>
@@ -3526,47 +3603,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>100</v>
       </c>
       <c r="B2" s="4">
         <v>101</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>500</v>
-      </c>
-      <c r="B2" s="4">
-        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -3582,13 +3624,13 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
@@ -3596,7 +3638,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
@@ -3613,6 +3655,41 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>500</v>
+      </c>
+      <c r="B2" s="4">
+        <v>501</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3620,15 +3697,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>52</v>
       </c>
@@ -3636,7 +3713,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>54</v>
       </c>
@@ -3649,7 +3726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -3657,19 +3734,19 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="34.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="34.09765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.8984375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -3734,7 +3811,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>48</v>
@@ -3806,7 +3883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3814,17 +3891,17 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>61</v>
       </c>
@@ -3844,7 +3921,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>187</v>
       </c>
@@ -3874,7 +3951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3882,15 +3959,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>55</v>
       </c>
@@ -3904,7 +3981,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>60</v>
       </c>
@@ -3923,7 +4000,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3931,17 +4008,17 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.69921875" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>69</v>
       </c>
@@ -3961,7 +4038,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="38">
         <v>100</v>
       </c>
@@ -3987,7 +4064,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3995,17 +4072,17 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.625" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.59765625" customWidth="1"/>
+    <col min="2" max="2" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>61</v>
       </c>
@@ -4025,7 +4102,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>187</v>
       </c>
@@ -4054,7 +4131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -4062,17 +4139,17 @@
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>197</v>
       </c>
@@ -4092,7 +4169,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
         <v>202</v>
       </c>
@@ -4121,7 +4198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -4129,17 +4206,17 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.25" customWidth="1"/>
+    <col min="1" max="1" width="15.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -4149,7 +4226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -4157,13 +4234,13 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>154</v>
       </c>
@@ -4171,7 +4248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>206</v>
       </c>
@@ -4185,7 +4262,52 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40E438A-E780-41FE-A9D6-473CFD9403B6}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>238</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{16E02862-1747-4D6C-8003-E89E09C31896}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE248A60-C3BD-412F-B50B-074B69CAE368}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -4193,17 +4315,17 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.625" customWidth="1"/>
-    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" customWidth="1"/>
-    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.09765625" customWidth="1"/>
+    <col min="6" max="6" width="20.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>197</v>
       </c>
@@ -4223,7 +4345,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
         <v>232</v>
       </c>
@@ -4251,545 +4373,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="G1" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="H1" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="I1" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="K1" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="L1" s="32" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="33">
-        <v>32002</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="K2" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="L2" s="24" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="18">
-        <v>100</v>
-      </c>
-      <c r="C3" s="18">
-        <v>1000</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="L3" s="26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="L4" s="26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="L5" s="26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="L6" s="26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="L7" s="26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="L8" s="26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="L9" s="26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="L10" s="26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="L11" s="27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="20">
-        <v>33343</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="J12" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="25">
-        <v>33310</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="L13" s="26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="25">
-        <v>33558</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="L14" s="26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="25">
-        <v>33280</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="L15" s="26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="25">
-        <v>33307</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K16" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="L16" s="26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28">
-        <v>8140</v>
-      </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="I17" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="J17" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="K17" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="L17" s="31" t="s">
-        <v>151</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -4797,13 +4381,13 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4811,7 +4395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -4829,19 +4413,557 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:L17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="33">
+        <v>32002</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="25"/>
+      <c r="B3" s="18">
+        <v>100</v>
+      </c>
+      <c r="C3" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="25"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L4" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="25"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L6" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="25"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L8" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="25"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L9" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="L10" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="25"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L11" s="27" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="20">
+        <v>33343</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <v>33310</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L13" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <v>33558</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L14" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
+        <v>33280</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L15" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <v>33307</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="L16" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="28">
+        <v>8140</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="I17" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="L17" s="31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -4849,17 +4971,17 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>1000</v>
       </c>
@@ -4869,7 +4991,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -4877,19 +4999,19 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4918,7 +5040,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>171</v>
       </c>
@@ -4955,7 +5077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4963,16 +5085,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>183</v>
       </c>
@@ -4989,7 +5111,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>190</v>
       </c>
@@ -5013,64 +5135,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="4">
-        <v>110</v>
-      </c>
-      <c r="E2" s="4">
-        <v>230</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
"LP-5427 Admin - Delay Debit" commit
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\SeleniumFramework\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0571CE36-0976-43C7-B8B3-FAB3057A2A96}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8464459A-0C8B-4607-AF30-53813C23C3AC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -823,10 +823,10 @@
     <t>ak30broker11@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>080918C16</t>
-  </si>
-  <si>
-    <t>080918C17</t>
+    <t>080918C77</t>
+  </si>
+  <si>
+    <t>080918C78</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated LP-5427 and unmatched tests
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8464459A-0C8B-4607-AF30-53813C23C3AC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{43D38DE9-C7AC-4A9E-8621-F4FD8280E60E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -20,17 +20,17 @@
     <sheet name="AdminCustomersSideMenSearchData" sheetId="54" r:id="rId5"/>
     <sheet name="AdminSearchData" sheetId="26" r:id="rId6"/>
     <sheet name="AdminLoginshipperaccountmodule" sheetId="32" r:id="rId7"/>
-    <sheet name="ShipperCompleteAccModuleData" sheetId="31" r:id="rId8"/>
-    <sheet name="BrokerProcessedTabSearchData" sheetId="33" r:id="rId9"/>
-    <sheet name="BrokerDiscountsTabSearchData" sheetId="34" r:id="rId10"/>
-    <sheet name="BrokerSchedPaymentTabSearchData" sheetId="35" r:id="rId11"/>
-    <sheet name="BrokerLoginData" sheetId="1" r:id="rId12"/>
-    <sheet name="BrokerRegister" sheetId="4" r:id="rId13"/>
-    <sheet name="BrokerDuplicateEmail" sheetId="47" r:id="rId14"/>
-    <sheet name="BrokerUpdatePaymentData" sheetId="24" r:id="rId15"/>
-    <sheet name="BrokerNewPaymentData" sheetId="7" r:id="rId16"/>
-    <sheet name="AdminPaymentsGreaterthan45Days" sheetId="51" r:id="rId17"/>
-    <sheet name="payementmorethan45daysData" sheetId="52" r:id="rId18"/>
+    <sheet name="AdminPaymentsGreaterthan45Days" sheetId="51" r:id="rId8"/>
+    <sheet name="payementmorethan45daysData" sheetId="52" r:id="rId9"/>
+    <sheet name="ShipperCompleteAccModuleData" sheetId="31" r:id="rId10"/>
+    <sheet name="BrokerProcessedTabSearchData" sheetId="33" r:id="rId11"/>
+    <sheet name="BrokerDiscountsTabSearchData" sheetId="34" r:id="rId12"/>
+    <sheet name="BrokerSchedPaymentTabSearchData" sheetId="35" r:id="rId13"/>
+    <sheet name="BrokerLoginData" sheetId="1" r:id="rId14"/>
+    <sheet name="BrokerRegister" sheetId="4" r:id="rId15"/>
+    <sheet name="BrokerDuplicateEmail" sheetId="47" r:id="rId16"/>
+    <sheet name="BrokerUpdatePaymentData" sheetId="24" r:id="rId17"/>
+    <sheet name="BrokerNewPaymentData" sheetId="7" r:id="rId18"/>
     <sheet name="BrokerUpdatedPaymentData" sheetId="49" r:id="rId19"/>
     <sheet name="BrokerPaymentDataforUnmatchedCr" sheetId="10" r:id="rId20"/>
     <sheet name="BrokerRegisterCanada" sheetId="11" r:id="rId21"/>
@@ -44,25 +44,25 @@
     <sheet name="CarrierLoginData" sheetId="5" r:id="rId29"/>
     <sheet name="CarrierRegisterData" sheetId="6" r:id="rId30"/>
     <sheet name="CarrierUpdatePaymentData" sheetId="50" r:id="rId31"/>
-    <sheet name="LoginHandshakewithRTF_CarrierDa" sheetId="43" r:id="rId32"/>
-    <sheet name="RTFLogindata" sheetId="41" state="hidden" r:id="rId33"/>
-    <sheet name="CarrierLoginAccountModuleData" sheetId="38" r:id="rId34"/>
-    <sheet name="CarrierlockedaccountAdminUnlock" sheetId="19" r:id="rId35"/>
-    <sheet name="carrierparentchilddata" sheetId="20" r:id="rId36"/>
-    <sheet name="carrierresetpassworddata" sheetId="21" r:id="rId37"/>
-    <sheet name="CarrierFuelcardaccountNumbers" sheetId="13" r:id="rId38"/>
-    <sheet name="BulkUploadPaymentsmatched" sheetId="22" r:id="rId39"/>
-    <sheet name="BulkUploadPaymentsUnmatched" sheetId="23" r:id="rId40"/>
-    <sheet name="CcarrierMatchedPayByCheckPayMNW" sheetId="14" r:id="rId41"/>
-    <sheet name="CarrierRegisterCanada" sheetId="12" r:id="rId42"/>
-    <sheet name="CarrierPaidTabData" sheetId="17" r:id="rId43"/>
-    <sheet name="CarrierBankingData" sheetId="16" r:id="rId44"/>
-    <sheet name="CarrierPaymentHistorydata" sheetId="29" r:id="rId45"/>
-    <sheet name="CarrierSchedulePaymentTabData" sheetId="25" r:id="rId46"/>
+    <sheet name="RTFLogindata" sheetId="41" state="hidden" r:id="rId32"/>
+    <sheet name="CarrierLoginAccountModuleData" sheetId="38" r:id="rId33"/>
+    <sheet name="CarrierlockedaccountAdminUnlock" sheetId="19" r:id="rId34"/>
+    <sheet name="carrierparentchilddata" sheetId="20" r:id="rId35"/>
+    <sheet name="carrierresetpassworddata" sheetId="21" r:id="rId36"/>
+    <sheet name="CarrierFuelcardaccountNumbers" sheetId="13" r:id="rId37"/>
+    <sheet name="BulkUploadPaymentsmatched" sheetId="22" r:id="rId38"/>
+    <sheet name="BulkUploadPaymentsUnmatched" sheetId="23" r:id="rId39"/>
+    <sheet name="CcarrierMatchedPayByCheckPayMNW" sheetId="14" r:id="rId40"/>
+    <sheet name="CarrierRegisterCanada" sheetId="12" r:id="rId41"/>
+    <sheet name="CarrierPaidTabData" sheetId="17" r:id="rId42"/>
+    <sheet name="CarrierBankingData" sheetId="16" r:id="rId43"/>
+    <sheet name="CarrierPaymentHistorydata" sheetId="29" r:id="rId44"/>
+    <sheet name="CarrierSchedulePaymentTabData" sheetId="25" r:id="rId45"/>
+    <sheet name="CarrierBankAccountDetails" sheetId="53" r:id="rId46"/>
     <sheet name="BankAccountDetailsForCopyPaste" sheetId="40" r:id="rId47"/>
     <sheet name="CreditAmount" sheetId="42" r:id="rId48"/>
     <sheet name="RTFLogin" sheetId="45" r:id="rId49"/>
-    <sheet name="CarrierBankAccountDetails" sheetId="53" r:id="rId50"/>
+    <sheet name="LoginHandshakewithRTF_CarrierDa" sheetId="43" r:id="rId50"/>
     <sheet name="Verificare" sheetId="2" state="hidden" r:id="rId51"/>
     <sheet name="tasks" sheetId="3" state="hidden" r:id="rId52"/>
   </sheets>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="239">
   <si>
     <t>Username</t>
   </si>
@@ -217,9 +217,6 @@
     <t>jasonglaser@truckstop.com</t>
   </si>
   <si>
-    <t>w2k/anilkumar</t>
-  </si>
-  <si>
     <t>CarrierEmail</t>
   </si>
   <si>
@@ -763,21 +760,6 @@
     <t>brokerCaCVK080718A02@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>umCarrierCVK080818U03@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>080818UM07</t>
-  </si>
-  <si>
-    <t>080818UM08</t>
-  </si>
-  <si>
-    <t>carrierCVK080818CC03@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>brokerCVK080818AK12@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>scheduledate</t>
   </si>
   <si>
@@ -787,9 +769,6 @@
     <t>carrierregister62@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>Cgihrms@12345</t>
-  </si>
-  <si>
     <t>08/20/2019</t>
   </si>
   <si>
@@ -820,13 +799,34 @@
     <t xml:space="preserve">brokerym123456@loadpaytest.truckstop.com </t>
   </si>
   <si>
-    <t>ak30broker11@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>080918C77</t>
-  </si>
-  <si>
-    <t>080918C78</t>
+    <t>082218UM001</t>
+  </si>
+  <si>
+    <t>082218UM002</t>
+  </si>
+  <si>
+    <t>carrierCVK082218C001@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>Password@5</t>
+  </si>
+  <si>
+    <t>brokerCVK082218B002@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>brokerCVK082218B003@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>umCVK082218U002@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>082218C001043</t>
+  </si>
+  <si>
+    <t>082218C001044</t>
+  </si>
+  <si>
+    <t>w2k/</t>
   </si>
 </sst>
 </file>
@@ -834,7 +834,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1132,7 +1132,7 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="55">
@@ -1496,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1516,21 +1516,162 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>238</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>225</v>
+        <v>62</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1111111111</v>
+      </c>
+      <c r="G2" s="4">
+        <v>11111</v>
+      </c>
+      <c r="H2" s="4">
+        <v>9999999999</v>
+      </c>
+      <c r="I2" s="4">
+        <v>3333333333</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="4">
+        <v>110</v>
+      </c>
+      <c r="E2" s="4">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1549,27 +1690,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>185</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -1590,7 +1731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1609,27 +1750,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>185</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="45" t="s">
         <v>190</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>191</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -1650,17 +1791,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1673,25 +1814,28 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>236</v>
+      <c r="A2" s="51" t="s">
+        <v>233</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{61090CE0-F74F-49B2-8F1A-92B790668C6A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1773,11 +1917,11 @@
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>221</v>
+      <c r="D2" s="51" t="s">
+        <v>234</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>234</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -1818,15 +1962,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{03A1FFB6-0600-4511-A735-BCFC5DFB1015}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{1C3F2681-4CEE-45F6-9627-5EC68BE74A5E}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{BF32865C-83F9-456C-BB24-2770DD351266}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{7326B572-57D0-4586-97F0-83E487BC8C1C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B1083F-2C63-4FCE-9825-F3543005262F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1850,10 +1994,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1865,7 +2009,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
@@ -1883,96 +2027,96 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>29</v>
@@ -1981,82 +2125,82 @@
         <v>456789</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H2" s="16" t="s">
+      <c r="I2" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>116</v>
       </c>
       <c r="J2" s="16" t="b">
         <v>1</v>
       </c>
       <c r="K2" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="M2" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="N2" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="O2" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="O2" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="P2" s="16" t="s">
+      <c r="Q2" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="R2" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="S2" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="T2" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="U2" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="V2" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="W2" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="X2" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="Y2" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="Y2" s="16" t="s">
+      <c r="Z2" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA2" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="Z2" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="AA2" s="16" t="s">
+      <c r="AB2" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="AB2" s="16" t="s">
+      <c r="AC2" s="16" t="s">
         <v>132</v>
-      </c>
-      <c r="AC2" s="16" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2067,11 +2211,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2079,7 +2223,7 @@
   <cols>
     <col min="1" max="1" width="44.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2097,146 +2241,40 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>224</v>
+      <c r="A2" s="51" t="s">
+        <v>231</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="D2" s="4">
-        <v>100</v>
+        <v>236</v>
+      </c>
+      <c r="D2" s="53">
+        <v>123.45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D3" s="53">
-        <v>100</v>
+        <v>123.46</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E2042960-FB20-4512-9FAF-4EE12E7FB798}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{E04B1E78-ADE4-4EC4-BDF2-23FAAB049F6A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C3BC51-A396-415F-9233-1E72E8DB73EF}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.625" customWidth="1"/>
-    <col min="2" max="3" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="D2" s="4">
-        <v>100</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D59054-07F3-4D98-89C6-3D3B72291E7D}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.5" customWidth="1"/>
-    <col min="2" max="3" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="D2" s="4">
-        <v>100</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2259,54 +2297,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>214</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E2" s="4">
         <v>1234587</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2334,10 +2372,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -2345,13 +2383,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2362,22 +2400,22 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>30</v>
@@ -2389,56 +2427,68 @@
         <v>32</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>217</v>
+      <c r="A2" s="51" t="s">
+        <v>235</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>218</v>
+        <v>229</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>229</v>
       </c>
       <c r="D2" s="4">
         <v>123.45</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" s="10">
         <v>295676689</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>219</v>
+      <c r="A3" s="51" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>230</v>
       </c>
       <c r="D3" s="4">
-        <v>456.78</v>
+        <v>123.67</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="10">
         <v>295676689</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="51" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="51" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{17ECB252-F6A9-4FD4-9508-2EC92DCF0622}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{BFB88CDD-BC03-4DFD-9A20-381D943B636F}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{DEABAF50-8E89-454B-8309-977F10130EFF}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{8416977C-9C53-4398-8C91-D905A88438B5}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{DB16F9B9-BCA6-4B23-9B34-D97B49A50748}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2478,10 +2528,10 @@
         <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>9</v>
@@ -2493,10 +2543,10 @@
         <v>11</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>12</v>
@@ -2535,19 +2585,19 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>23</v>
@@ -2556,10 +2606,10 @@
         <v>23</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>24</v>
@@ -2616,21 +2666,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="4">
         <v>101200453</v>
@@ -2668,10 +2718,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>15</v>
@@ -2679,16 +2729,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2722,22 +2772,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="41" t="s">
-        <v>66</v>
-      </c>
       <c r="D1" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E1" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="41" t="s">
         <v>165</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2745,19 +2795,19 @@
         <v>100</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="4">
         <v>8564</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E2" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="43" t="s">
         <v>167</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2784,30 +2834,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="D1" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2846,10 +2896,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -2881,30 +2931,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="D1" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2937,10 +2987,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>15</v>
@@ -2948,16 +2998,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2974,12 +3024,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2992,16 +3042,17 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>63</v>
+      <c r="A2" s="51" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DF5E700E-7839-4D46-8BFA-3F24C340437E}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{F45599BF-D923-4AC0-8295-499B237CEC00}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3027,10 +3078,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>15</v>
@@ -3038,16 +3089,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -3064,7 +3115,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3142,11 +3193,11 @@
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>220</v>
+      <c r="D2" s="51" t="s">
+        <v>231</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>231</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -3187,10 +3238,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{F80E385F-FAF1-4F90-A236-2F28AFA509E0}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{8E5655BA-F6C9-4F12-AD5A-F92673770305}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{0885AFC8-EB7F-43C6-90C3-615D238358AA}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{B69B1785-DD2A-479E-AB7C-EA61F509A86D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3213,54 +3265,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E2" s="4">
         <v>1234587</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3272,37 +3324,6 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
-        <v>206</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>203</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3318,7 +3339,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3326,10 +3347,10 @@
     </row>
     <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3338,7 +3359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3362,18 +3383,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C2" s="4">
         <v>8085</v>
@@ -3390,7 +3411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3412,18 +3433,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -3434,7 +3455,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3458,24 +3479,24 @@
         <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3487,7 +3508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3505,30 +3526,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -3542,7 +3563,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3558,10 +3579,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3578,7 +3599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3594,10 +3615,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3613,42 +3634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3664,10 +3650,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3683,7 +3669,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F490F69F-7B3C-4806-B078-17DFBA41A6FD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3701,18 +3725,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -3720,7 +3744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -3757,10 +3781,10 @@
         <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>9</v>
@@ -3772,10 +3796,10 @@
         <v>11</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>12</v>
@@ -3808,25 +3832,25 @@
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>23</v>
@@ -3835,10 +3859,10 @@
         <v>23</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>24</v>
@@ -3877,7 +3901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3897,42 +3921,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" s="4">
         <v>1234.56</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3945,7 +3969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3963,21 +3987,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4">
         <v>101000187</v>
@@ -3994,7 +4018,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -4014,22 +4038,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="37" t="s">
-        <v>66</v>
-      </c>
       <c r="D1" s="37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E1" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>165</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4037,19 +4061,19 @@
         <v>100</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" s="39">
         <v>241</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E2" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="40" t="s">
         <v>167</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -4058,7 +4082,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -4078,48 +4102,114 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D2" s="4">
         <v>1234.56</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-2500-000000000000}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-2500-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE248A60-C3BD-412F-B50B-074B69CAE368}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
+    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.125" customWidth="1"/>
+    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2" s="46">
+        <v>122105155</v>
+      </c>
+      <c r="E2" s="46">
+        <v>123456789</v>
+      </c>
+      <c r="F2" s="46">
+        <v>123456789</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F5CE9E67-00B3-4280-9EA7-BCF711537E2A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4145,33 +4235,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D1" s="37" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>199</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D2" s="46">
         <v>122105155</v>
@@ -4197,7 +4287,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4207,12 +4297,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1000</v>
+        <v>999999</v>
       </c>
     </row>
   </sheetData>
@@ -4236,7 +4326,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -4244,10 +4334,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -4273,24 +4363,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="C1" s="52" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -4302,67 +4392,32 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE248A60-C3BD-412F-B50B-074B69CAE368}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.625" customWidth="1"/>
-    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" customWidth="1"/>
-    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>197</v>
-      </c>
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>199</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>229</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>230</v>
-      </c>
-      <c r="D2" s="46">
-        <v>122105155</v>
-      </c>
-      <c r="E2" s="46">
-        <v>123456789</v>
-      </c>
-      <c r="F2" s="46">
-        <v>123456789</v>
+    </row>
+    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{F5CE9E67-00B3-4280-9EA7-BCF711537E2A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4445,40 +4500,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="C1" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="F1" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="J1" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="K1" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>148</v>
-      </c>
-      <c r="L1" s="32" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4490,25 +4545,25 @@
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="F2" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4522,25 +4577,25 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L3" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -4548,31 +4603,31 @@
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>153</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L4" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -4582,25 +4637,25 @@
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L5" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -4610,25 +4665,25 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="G6" s="18" t="s">
-        <v>151</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L6" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -4638,25 +4693,25 @@
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>151</v>
-      </c>
       <c r="I7" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L7" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -4666,25 +4721,25 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I8" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>151</v>
-      </c>
       <c r="J8" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L8" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -4694,25 +4749,25 @@
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>151</v>
-      </c>
       <c r="K9" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -4722,25 +4777,25 @@
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="K10" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>151</v>
-      </c>
       <c r="L10" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4750,25 +4805,25 @@
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="L11" s="27" t="s">
         <v>150</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="L11" s="27" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -4780,25 +4835,25 @@
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="G12" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="G12" s="23" t="s">
-        <v>151</v>
-      </c>
       <c r="H12" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L12" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -4810,25 +4865,25 @@
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H13" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>151</v>
-      </c>
       <c r="I13" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L13" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -4840,25 +4895,25 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I14" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>151</v>
-      </c>
       <c r="J14" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L14" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -4870,25 +4925,25 @@
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="J15" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>151</v>
-      </c>
       <c r="K15" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L15" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -4900,25 +4955,25 @@
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="K16" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K16" s="18" t="s">
-        <v>151</v>
-      </c>
       <c r="L16" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4930,25 +4985,25 @@
       <c r="D17" s="30"/>
       <c r="E17" s="30"/>
       <c r="F17" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="I17" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="L17" s="31" t="s">
         <v>150</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="I17" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="J17" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="K17" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="L17" s="31" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -4972,7 +5027,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -4986,147 +5041,111 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C3BC51-A396-415F-9233-1E72E8DB73EF}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.625" customWidth="1"/>
+    <col min="2" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>172</v>
+        <v>31</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>173</v>
+        <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1111111111</v>
-      </c>
-      <c r="G2" s="4">
-        <v>11111</v>
-      </c>
-      <c r="H2" s="4">
-        <v>9999999999</v>
-      </c>
-      <c r="I2" s="4">
-        <v>3333333333</v>
+        <v>218</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D59054-07F3-4D98-89C6-3D3B72291E7D}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5" customWidth="1"/>
+    <col min="2" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>183</v>
+        <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>184</v>
+        <v>30</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>185</v>
+        <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>66</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1000</v>
+      <c r="A2" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>221</v>
       </c>
       <c r="D2" s="4">
-        <v>110</v>
-      </c>
-      <c r="E2" s="4">
-        <v>230</v>
+        <v>100</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit "LP-5427Admin - DelayDebit" changes
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{43D38DE9-C7AC-4A9E-8621-F4FD8280E60E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B5EA822F-2783-4275-B1D0-EED2A7687BE0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="239">
   <si>
     <t>Username</t>
   </si>
@@ -808,25 +808,25 @@
     <t>carrierCVK082218C001@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>Password@5</t>
-  </si>
-  <si>
-    <t>brokerCVK082218B002@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>brokerCVK082218B003@loadpaytest.truckstop.com</t>
   </si>
   <si>
     <t>umCVK082218U002@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>082218C001043</t>
-  </si>
-  <si>
-    <t>082218C001044</t>
-  </si>
-  <si>
-    <t>w2k/</t>
+    <t>w2k/anilkumar</t>
+  </si>
+  <si>
+    <t>Cgihrms@12345</t>
+  </si>
+  <si>
+    <t>ak30broker11@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>082218C1114</t>
+  </si>
+  <si>
+    <t>082218C1115</t>
   </si>
 </sst>
 </file>
@@ -834,7 +834,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1132,7 +1132,7 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="55">
@@ -1496,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1516,11 +1516,16 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>235</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{FBE12775-733D-491E-8CC8-50689B08152E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1796,12 +1801,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1815,18 +1820,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{61090CE0-F74F-49B2-8F1A-92B790668C6A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1918,10 +1920,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -2215,7 +2217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2242,39 +2244,35 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D2" s="53">
-        <v>123.45</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D3" s="53">
-        <v>123.46</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{E2042960-FB20-4512-9FAF-4EE12E7FB798}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{E04B1E78-ADE4-4EC4-BDF2-23FAAB049F6A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2360,7 +2358,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2435,7 +2433,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>229</v>
@@ -2455,7 +2453,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B3" s="53" t="s">
         <v>230</v>
@@ -2475,12 +2473,12 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="51" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3024,7 +3022,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3043,7 +3041,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="B2" s="51" t="s">
         <v>26</v>
@@ -3052,7 +3050,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DF5E700E-7839-4D46-8BFA-3F24C340437E}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{F45599BF-D923-4AC0-8295-499B237CEC00}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3674,7 +3671,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3696,7 +3693,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>232</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated regression test suite
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C9F4E813-FEF3-4D3A-8371-7E299F2D2BAB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F20BFD23-05C0-47F2-AE42-0E86CE514116}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="13" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="24" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -757,9 +757,6 @@
     <t>321456</t>
   </si>
   <si>
-    <t>brokerCaCVK080718A02@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>scheduledate</t>
   </si>
   <si>
@@ -784,24 +781,12 @@
     <t xml:space="preserve">brokerym123456@loadpaytest.truckstop.com </t>
   </si>
   <si>
-    <t>umCVK082218U002@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>w2k/anilkumar</t>
   </si>
   <si>
     <t>Cgihrms@12345</t>
   </si>
   <si>
-    <t>082218UM037</t>
-  </si>
-  <si>
-    <t>082218UM039</t>
-  </si>
-  <si>
-    <t>brokerCVK082218B0033@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>carrierCVK082218C089(@loadpaytest.truckstop.com</t>
   </si>
   <si>
@@ -817,10 +802,25 @@
     <t>080918POUTUO</t>
   </si>
   <si>
-    <t>082218C1XYZ</t>
-  </si>
-  <si>
-    <t>082218CPOT</t>
+    <t>umCVK082218U072@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>822133AEDOP</t>
+  </si>
+  <si>
+    <t>82290087TQHOP</t>
+  </si>
+  <si>
+    <t>brokerCaCVK080718A099@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>082218JK</t>
+  </si>
+  <si>
+    <t>082218PT</t>
+  </si>
+  <si>
+    <t>brokerCVK082218B00336@loadpaytest.truckstop.com</t>
   </si>
 </sst>
 </file>
@@ -1510,10 +1510,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -1794,7 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1917,10 +1917,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -1962,7 +1962,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{BF32865C-83F9-456C-BB24-2770DD351266}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{7B8E1D49-38B7-4CF2-A45C-D38465443A0D}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{A58F144F-B2B5-4543-9FC0-0946C64797DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2215,7 +2215,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2244,13 +2244,13 @@
         <v>75</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D2" s="53">
-        <v>100</v>
+        <v>930</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2258,13 +2258,13 @@
         <v>75</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D3" s="53">
-        <v>100</v>
+        <v>930</v>
       </c>
     </row>
   </sheetData>
@@ -2434,13 +2434,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C2" s="53" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D2" s="4">
         <v>123.45</v>
@@ -2454,13 +2454,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B3" s="53" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D3" s="4">
         <v>123.67</v>
@@ -2475,7 +2475,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{17ECB252-F6A9-4FD4-9508-2EC92DCF0622}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{DEABAF50-8E89-454B-8309-977F10130EFF}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{4BCAE993-317A-4009-849A-10DCAAB7D60C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2486,7 +2486,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2571,11 +2571,11 @@
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>215</v>
+      <c r="D2" s="51" t="s">
+        <v>233</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>233</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>43</v>
@@ -2628,8 +2628,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{B252F9C7-03C1-4E9A-A8E9-AF276250EA75}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{BFF31301-BAE2-40D4-B6A4-33364DA2AC30}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{BFF31301-BAE2-40D4-B6A4-33364DA2AC30}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{EAE151DA-9EBF-45BD-9511-881F6C029360}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3010,7 +3010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3181,10 +3181,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -4176,13 +4176,13 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D2" s="46">
         <v>122105155</v>
@@ -4350,13 +4350,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="C1" s="52" t="s">
         <v>220</v>
-      </c>
-      <c r="C1" s="52" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4364,10 +4364,10 @@
         <v>135</v>
       </c>
       <c r="B2" s="53" t="s">
+        <v>221</v>
+      </c>
+      <c r="C2" s="51" t="s">
         <v>222</v>
-      </c>
-      <c r="C2" s="51" t="s">
-        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -5058,7 +5058,7 @@
         <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5066,16 +5066,16 @@
         <v>75</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D2" s="4">
         <v>100</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -5117,7 +5117,7 @@
         <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5125,16 +5125,16 @@
         <v>75</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D2" s="4">
         <v>100</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Test Data spreadsheet with no outlook credentials and base users
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F37D40D8-F008-4397-A794-659E9D86C73F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9A1B6F88-203A-4736-8114-75171B0E2BEC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="14" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="242">
   <si>
     <t>Username</t>
   </si>
@@ -781,15 +781,6 @@
     <t xml:space="preserve">brokerym123456@loadpaytest.truckstop.com </t>
   </si>
   <si>
-    <t>w2k/anilkumar</t>
-  </si>
-  <si>
-    <t>Cgihrms@12345</t>
-  </si>
-  <si>
-    <t>carrierCVK082218C089(@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>08/27/2019</t>
   </si>
   <si>
@@ -803,12 +794,6 @@
   </si>
   <si>
     <t>brokerCaCVK080718A099@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>brokerstage44783@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>unmatched01AK@loadpaytest.truckstop.com</t>
   </si>
   <si>
     <t>jcglaser@yahoo.com</t>
@@ -824,10 +809,34 @@
 824811 </t>
   </si>
   <si>
-    <t>01249</t>
-  </si>
-  <si>
-    <t>01250</t>
+    <t>broker@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>carrier@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>Password@5</t>
+  </si>
+  <si>
+    <t>082918NP001</t>
+  </si>
+  <si>
+    <t>082918NP002</t>
+  </si>
+  <si>
+    <t>umCarrier@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>082918UM001</t>
+  </si>
+  <si>
+    <t>082918UM002</t>
+  </si>
+  <si>
+    <t>082918NP003</t>
+  </si>
+  <si>
+    <t>w2k/</t>
   </si>
 </sst>
 </file>
@@ -835,7 +844,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1133,7 +1142,7 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="57">
@@ -1503,8 +1512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1523,16 +1532,11 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B2" s="51" t="s">
-        <v>224</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="B2" s="51"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{FBE12775-733D-491E-8CC8-50689B08152E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1827,7 +1831,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B2" s="51" t="s">
         <v>26</v>
@@ -1930,10 +1934,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -1976,7 +1980,7 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{BF32865C-83F9-456C-BB24-2770DD351266}"/>
     <hyperlink ref="L2" r:id="rId2" xr:uid="{A3731620-4590-43DF-9EBB-DC731876BFEB}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{D8B918EA-A59E-409D-AFBC-D9A9BEFAE07E}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{77346034-8AA3-4B39-9E11-3322673E28C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -2226,17 +2230,16 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.25" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="2" max="3" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2255,39 +2258,54 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D2" s="53">
-        <v>100</v>
+        <v>123.45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D3" s="53">
-        <v>100</v>
+        <v>123.67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="55" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" s="53">
+        <v>123.89</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="carrierregisterstage1@loadpaytest.truckstop.com" xr:uid="{B36CCD42-7380-4430-BCBD-00915AA61D67}"/>
     <hyperlink ref="A2" r:id="rId2" display="carrierregisterstage1@loadpaytest.truckstop.com" xr:uid="{6C7EA479-467D-4A9A-B890-6EAA20A00491}"/>
+    <hyperlink ref="A4" r:id="rId3" display="carrierregisterstage1@loadpaytest.truckstop.com" xr:uid="{43479387-9ABC-463F-A9E2-65A687B1061F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2448,16 +2466,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>232</v>
-      </c>
-      <c r="B2" s="53">
-        <v>10041565</v>
-      </c>
-      <c r="C2" s="53">
-        <v>10041565</v>
+        <v>237</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>238</v>
       </c>
       <c r="D2" s="53">
-        <v>10</v>
+        <v>123.45</v>
       </c>
       <c r="E2" s="53" t="s">
         <v>37</v>
@@ -2468,16 +2486,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
-        <v>232</v>
-      </c>
-      <c r="B3" s="53">
-        <v>10041566</v>
-      </c>
-      <c r="C3" s="53">
-        <v>10041566</v>
+        <v>237</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>239</v>
       </c>
       <c r="D3" s="53">
-        <v>10</v>
+        <v>123.67</v>
       </c>
       <c r="E3" s="53" t="s">
         <v>37</v>
@@ -2489,7 +2507,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{8AC65AD8-4A8D-4D4F-9C74-FE1190EF53D3}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{5404F43B-A22E-486E-AAAF-0D1E20796900}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{038C0CB3-B3C2-4829-AA36-ADB1F1C29FFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2586,10 +2604,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>43</v>
@@ -3044,7 +3062,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B2" s="51" t="s">
         <v>69</v>
@@ -3191,10 +3209,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -3235,8 +3253,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="carrierCVK082218C001@loadpaytest.truckstop.com" xr:uid="{0885AFC8-EB7F-43C6-90C3-615D238358AA}"/>
-    <hyperlink ref="E2" r:id="rId2" display="carrierCVK082218C001@loadpaytest.truckstop.com" xr:uid="{FCF40D41-4A6C-4981-BE06-22AB971BB89B}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{0885AFC8-EB7F-43C6-90C3-615D238358AA}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{B67FB339-084F-4B71-B304-38EF6C152D26}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -3671,7 +3689,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3693,7 +3711,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>62</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3938,7 +3956,7 @@
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B2" s="51" t="s">
         <v>69</v>
@@ -3950,10 +3968,10 @@
         <v>967.1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F2" s="56" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -5076,16 +5094,16 @@
         <v>75</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D2" s="4">
         <v>100</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -5135,16 +5153,16 @@
         <v>75</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D2" s="4">
         <v>100</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated J sprint stability
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{60D39915-EDA5-4C34-B364-F98850EA4A77}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DA43277C-2A18-45C1-B9A6-02DDC99971A7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="16" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="235">
   <si>
     <t>Username</t>
   </si>
@@ -301,9 +301,6 @@
     <t>Password@1</t>
   </si>
   <si>
-    <t>crcanada1416@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>Search Payer</t>
   </si>
   <si>
@@ -667,9 +664,6 @@
     <t>Jason Is Cool</t>
   </si>
   <si>
-    <t>carrierCVK070618X5@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>070818X5</t>
   </si>
   <si>
@@ -782,9 +776,6 @@
   </si>
   <si>
     <t>080918POUTUO</t>
-  </si>
-  <si>
-    <t>brokerCaCVK080718A099@loadpaytest.truckstop.com</t>
   </si>
   <si>
     <t>jcglaser@yahoo.com</t>
@@ -809,19 +800,22 @@
     <t>umCarrier@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>w2k/anilkumar</t>
-  </si>
-  <si>
-    <t>Cgihrms@12345</t>
-  </si>
-  <si>
     <t>AbcCal@126</t>
   </si>
   <si>
-    <t>12AB44</t>
-  </si>
-  <si>
-    <t>12AB45</t>
+    <t>Password@5</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>brokerCa@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>carrierCa@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>w2k/</t>
   </si>
 </sst>
 </file>
@@ -829,7 +823,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1127,7 +1121,7 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="57">
@@ -1497,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1517,16 +1511,11 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B2" s="51" t="s">
-        <v>233</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="B2" s="51"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{CCC2E108-2960-4708-BCC0-2AA393EE4822}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1559,42 +1548,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="F2" s="4">
         <v>1111111111</v>
@@ -1636,27 +1625,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -1696,27 +1685,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -1756,27 +1745,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -1802,7 +1791,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1821,7 +1810,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B2" s="51" t="s">
         <v>26</v>
@@ -1924,10 +1913,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -2001,10 +1990,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2040,90 +2029,90 @@
         <v>36</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>29</v>
@@ -2132,82 +2121,82 @@
         <v>456789</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="16" t="s">
+      <c r="I2" s="16" t="s">
         <v>113</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>114</v>
       </c>
       <c r="J2" s="16" t="b">
         <v>1</v>
       </c>
       <c r="K2" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="L2" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="M2" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="N2" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="O2" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="O2" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="P2" s="16" t="s">
+      <c r="Q2" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="R2" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="S2" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="T2" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="U2" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="V2" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="W2" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="X2" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="Y2" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="Y2" s="16" t="s">
+      <c r="Z2" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA2" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="Z2" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA2" s="16" t="s">
+      <c r="AB2" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="AB2" s="16" t="s">
+      <c r="AC2" s="16" t="s">
         <v>130</v>
-      </c>
-      <c r="AC2" s="16" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2220,10 +2209,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2248,13 +2237,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D2" s="53">
         <v>100</v>
@@ -2262,16 +2251,30 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D3" s="53">
-        <v>100</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="D4" s="53">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -2299,10 +2302,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>36</v>
@@ -2311,42 +2314,42 @@
         <v>31</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E2" s="4">
         <v>1234587</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2374,10 +2377,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -2385,13 +2388,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2405,7 +2408,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2437,16 +2440,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="53" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="53">
-        <v>82918025</v>
-      </c>
-      <c r="C2" s="53">
-        <v>82918025</v>
+      <c r="C2" s="53" t="s">
+        <v>231</v>
       </c>
       <c r="D2" s="53">
-        <v>100</v>
+        <v>123.45</v>
       </c>
       <c r="E2" s="53" t="s">
         <v>37</v>
@@ -2457,16 +2460,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" s="53" t="s">
         <v>231</v>
       </c>
-      <c r="B3" s="53">
-        <v>82918026</v>
-      </c>
-      <c r="C3" s="53">
-        <v>82918026</v>
+      <c r="C3" s="53" t="s">
+        <v>231</v>
       </c>
       <c r="D3" s="53">
-        <v>100</v>
+        <v>123.67</v>
       </c>
       <c r="E3" s="53" t="s">
         <v>37</v>
@@ -2489,7 +2492,7 @@
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2575,10 +2578,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>43</v>
@@ -2632,7 +2635,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{BFF31301-BAE2-40D4-B6A4-33364DA2AC30}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{EAE151DA-9EBF-45BD-9511-881F6C029360}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{CF124DBF-1F89-49C1-B243-1F53286525EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2708,10 +2711,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>15</v>
@@ -2719,16 +2722,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2762,22 +2765,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="41" t="s">
-        <v>65</v>
-      </c>
       <c r="D1" s="41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E1" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" s="41" t="s">
         <v>163</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2785,19 +2788,19 @@
         <v>100</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C2" s="4">
         <v>8564</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E2" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="43" t="s">
         <v>165</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2824,30 +2827,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="D1" s="34" t="s">
         <v>154</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2886,10 +2889,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2921,30 +2924,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="D1" s="34" t="s">
         <v>154</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2977,10 +2980,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>15</v>
@@ -2988,16 +2991,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -3033,10 +3036,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3064,10 +3067,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>15</v>
@@ -3075,16 +3078,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -3180,10 +3183,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -3251,10 +3254,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>36</v>
@@ -3263,42 +3266,42 @@
         <v>31</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>209</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>211</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E2" s="4">
         <v>1234587</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3325,7 +3328,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3333,10 +3336,10 @@
     </row>
     <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -3369,7 +3372,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>38</v>
@@ -3377,10 +3380,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C2" s="4">
         <v>8085</v>
@@ -3419,18 +3422,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3465,10 +3468,10 @@
         <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3476,13 +3479,13 @@
         <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3512,30 +3515,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3601,10 +3604,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3636,10 +3639,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3660,7 +3663,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3682,7 +3685,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>62</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3823,11 +3826,11 @@
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>63</v>
+      <c r="D2" s="51" t="s">
+        <v>233</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>233</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>43</v>
@@ -3881,7 +3884,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-2100-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-2100-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{0AE2CE27-A309-4157-9D40-7F852063D5A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3913,36 +3916,36 @@
         <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="4">
         <v>967.1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F2" s="56" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -4024,22 +4027,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="37" t="s">
-        <v>65</v>
-      </c>
       <c r="D1" s="37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E1" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>163</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4047,19 +4050,19 @@
         <v>100</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C2" s="39">
         <v>241</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E2" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="40" t="s">
         <v>165</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -4073,7 +4076,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4094,36 +4097,36 @@
         <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>185</v>
+      <c r="A2" s="51" t="s">
+        <v>227</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D2" s="4">
         <v>1234.56</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -4155,33 +4158,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D1" s="37" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D2" s="46">
         <v>122105155</v>
@@ -4221,33 +4224,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D1" s="37" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D2" s="46">
         <v>122105155</v>
@@ -4283,7 +4286,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -4312,7 +4315,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -4320,10 +4323,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -4349,24 +4352,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1" s="52" t="s">
         <v>215</v>
-      </c>
-      <c r="B1" s="52" t="s">
-        <v>216</v>
-      </c>
-      <c r="C1" s="52" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -4397,10 +4400,10 @@
     </row>
     <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -4486,40 +4489,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="C1" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="F1" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="J1" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="K1" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>146</v>
-      </c>
-      <c r="L1" s="32" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4531,25 +4534,25 @@
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="F2" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4563,25 +4566,25 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L3" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -4589,31 +4592,31 @@
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>151</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L4" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -4623,25 +4626,25 @@
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L5" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -4651,25 +4654,25 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="G6" s="18" t="s">
-        <v>149</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L6" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -4679,25 +4682,25 @@
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>149</v>
-      </c>
       <c r="I7" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L7" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -4707,25 +4710,25 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I8" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>149</v>
-      </c>
       <c r="J8" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L8" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -4735,25 +4738,25 @@
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>149</v>
-      </c>
       <c r="K9" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -4763,25 +4766,25 @@
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="K10" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>149</v>
-      </c>
       <c r="L10" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4791,25 +4794,25 @@
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="L11" s="27" t="s">
         <v>148</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="L11" s="27" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -4821,25 +4824,25 @@
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="G12" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="G12" s="23" t="s">
-        <v>149</v>
-      </c>
       <c r="H12" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L12" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -4851,25 +4854,25 @@
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H13" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>149</v>
-      </c>
       <c r="I13" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L13" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -4881,25 +4884,25 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I14" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>149</v>
-      </c>
       <c r="J14" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L14" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -4911,25 +4914,25 @@
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J15" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>149</v>
-      </c>
       <c r="K15" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L15" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -4941,25 +4944,25 @@
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="K16" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="K16" s="18" t="s">
-        <v>149</v>
-      </c>
       <c r="L16" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4971,25 +4974,25 @@
       <c r="D17" s="30"/>
       <c r="E17" s="30"/>
       <c r="F17" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="I17" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="L17" s="31" t="s">
         <v>148</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="I17" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="J17" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="K17" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="L17" s="31" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -5013,7 +5016,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -5057,24 +5060,24 @@
         <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D2" s="4">
         <v>100</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -5116,24 +5119,24 @@
         <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D2" s="4">
         <v>100</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I sprint Updates - 090618
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{55A03FF5-81A6-4201-8BCE-5BEDA4E11F4E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D09EE084-923E-4427-901C-879271F919C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="13" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -26,9 +26,9 @@
     <sheet name="BrokerProcessedTabSearchData" sheetId="33" r:id="rId11"/>
     <sheet name="BrokerDiscountsTabSearchData" sheetId="34" r:id="rId12"/>
     <sheet name="BrokerSchedPaymentTabSearchData" sheetId="35" r:id="rId13"/>
-    <sheet name="BrokerLoginData" sheetId="1" r:id="rId14"/>
-    <sheet name="HandshakeCarrierLogindata" sheetId="56" r:id="rId15"/>
-    <sheet name="HandshakeBrokerLogindata" sheetId="57" r:id="rId16"/>
+    <sheet name="HandshakeCarrierLogindata" sheetId="56" r:id="rId14"/>
+    <sheet name="HandshakeBrokerLogindata" sheetId="57" r:id="rId15"/>
+    <sheet name="BrokerLoginData" sheetId="1" r:id="rId16"/>
     <sheet name="BrokerRegister" sheetId="4" r:id="rId17"/>
     <sheet name="BrokerDuplicateEmail" sheetId="47" r:id="rId18"/>
     <sheet name="BrokerUpdatePaymentData" sheetId="24" r:id="rId19"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="238">
   <si>
     <t>Username</t>
   </si>
@@ -770,12 +770,6 @@
     <t>carrierCa@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>w2k\anilkumar</t>
-  </si>
-  <si>
-    <t>Cgihrms@12345</t>
-  </si>
-  <si>
     <t>IL54295</t>
   </si>
   <si>
@@ -815,12 +809,6 @@
     <t>AbcCal12@126</t>
   </si>
   <si>
-    <t>broker66889@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>umCarrier6661@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
     <t>123NJ7671S</t>
   </si>
   <si>
@@ -830,10 +818,16 @@
     <t>080918TTRKPW</t>
   </si>
   <si>
-    <t>897MMN</t>
-  </si>
-  <si>
-    <t>174LKO</t>
+    <t>broker@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>umCarrier@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>w2k\</t>
   </si>
 </sst>
 </file>
@@ -1509,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1529,16 +1523,11 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>219</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{99DDA902-DB9B-4916-8263-8594FCB3BE4A}"/>
-  </hyperlinks>
+        <v>237</v>
+      </c>
+      <c r="B2" s="50"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1810,6 +1799,84 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED729B66-0A87-4107-B23B-33252E36BD91}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4781DA1A-6424-483A-878E-C1124701B26A}"/>
+    <hyperlink ref="B1" r:id="rId2" xr:uid="{1435F2DD-1D47-4254-9ADA-2479914646F9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92269024-4481-400C-8D7F-BC60F056B751}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{DA813998-C10E-45EC-AD16-E22F40C0C23F}"/>
+    <hyperlink ref="B1" r:id="rId2" xr:uid="{31EA81E1-CB98-4D4D-B0F6-4724E540AD60}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1833,7 +1900,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B2" s="50" t="s">
         <v>62</v>
@@ -1845,84 +1912,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED729B66-0A87-4107-B23B-33252E36BD91}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>225</v>
-      </c>
-      <c r="B1" s="56" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{4781DA1A-6424-483A-878E-C1124701B26A}"/>
-    <hyperlink ref="B1" r:id="rId2" xr:uid="{1435F2DD-1D47-4254-9ADA-2479914646F9}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92269024-4481-400C-8D7F-BC60F056B751}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>225</v>
-      </c>
-      <c r="B1" s="56" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
-        <v>226</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{DA813998-C10E-45EC-AD16-E22F40C0C23F}"/>
-    <hyperlink ref="B1" r:id="rId2" xr:uid="{31EA81E1-CB98-4D4D-B0F6-4724E540AD60}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2014,10 +2003,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="50" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -2060,7 +2049,7 @@
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" xr:uid="{A3731620-4590-43DF-9EBB-DC731876BFEB}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{596D9BCA-E019-4DB7-B99D-31B571C319D2}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{189603D0-D765-4C83-9558-4001C97E00C9}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{DA09774B-9E23-4CAE-A9D4-911A665E0A4F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -2091,10 +2080,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2336,7 +2325,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>201</v>
@@ -2353,10 +2342,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2381,13 +2370,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D2" s="52">
         <v>930</v>
@@ -2395,21 +2384,70 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D3" s="52">
         <v>930</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="54" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="54" t="s">
+        <v>215</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D5">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="54" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D6">
+        <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6BD736EF-0A9A-4295-8C91-8829EF333F40}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{E95E0960-C996-46E2-9866-0BD7AB7CC179}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{EA87CDFC-A308-4C4B-ADBB-77FC9FB1D4AD}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{C76142B8-E5A1-4F5B-88EB-33862AB73FCC}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{013B6E89-69D3-4071-AC99-48B34CDE2EBB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -2418,7 +2456,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2495,7 +2533,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2527,13 +2565,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D2" s="52">
         <v>123.45</v>
@@ -2547,13 +2585,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D3" s="52">
         <v>123.67</v>
@@ -2568,7 +2606,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{8AC65AD8-4A8D-4D4F-9C74-FE1190EF53D3}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{67B40FB9-5A30-44D8-813F-216547A438C1}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{DE157CF1-E748-45D1-850E-D0400BA4C740}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2976,10 +3014,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -3175,7 +3213,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B2" s="50" t="s">
         <v>62</v>
@@ -3619,10 +3657,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>81</v>
@@ -3705,7 +3743,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -4268,7 +4306,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>62</v>
@@ -4334,7 +4372,7 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>62</v>
@@ -4392,7 +4430,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -4420,7 +4458,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="52">
-        <v>1000</v>
+        <v>999999</v>
       </c>
     </row>
   </sheetData>
@@ -4443,7 +4481,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -5178,19 +5216,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D2" s="4">
         <v>100</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -5236,19 +5274,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D2" s="4">
         <v>100</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated K Sprint tests - still in progress
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7F298B62-6855-4F44-B78F-B0A8A3739B0C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2D4ADE3D-6EF3-4908-A840-48C46B255E4A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="250">
   <si>
     <t>Username</t>
   </si>
@@ -263,18 +263,6 @@
   </si>
   <si>
     <t>fleet_accountnbr</t>
-  </si>
-  <si>
-    <t>Anilkumar</t>
-  </si>
-  <si>
-    <t>EnterDOTNnumber</t>
-  </si>
-  <si>
-    <t>ContactName</t>
-  </si>
-  <si>
-    <t>800832</t>
   </si>
   <si>
     <t>Account Name</t>
@@ -770,9 +758,6 @@
     <t>NewCreditAmount</t>
   </si>
   <si>
-    <t>Password@5</t>
-  </si>
-  <si>
     <t>carriershantu@loadpaytest.truckstop.com</t>
   </si>
   <si>
@@ -828,6 +813,54 @@
   </si>
   <si>
     <t>broker[uniqueID]@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>DOT Number</t>
+  </si>
+  <si>
+    <t>Street Address</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Contact Name</t>
+  </si>
+  <si>
+    <t>TestCompany1</t>
+  </si>
+  <si>
+    <t>TestCompany2</t>
+  </si>
+  <si>
+    <t>123 Main St</t>
+  </si>
+  <si>
+    <t>Addison</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>456 North Ave</t>
+  </si>
+  <si>
+    <t>Lombard</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
   </si>
   <si>
     <t>w2k\</t>
@@ -910,7 +943,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -961,6 +994,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1139,7 +1178,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1155,9 +1194,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1221,6 +1257,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1507,7 +1548,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1526,9 +1567,9 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B2" s="50"/>
+        <v>249</v>
+      </c>
+      <c r="B2" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1563,42 +1604,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F2" s="4">
         <v>1111111111</v>
@@ -1640,27 +1681,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>181</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>185</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -1700,27 +1741,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>181</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>185</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -1760,27 +1801,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>187</v>
+      <c r="B2" s="44" t="s">
+        <v>183</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -1816,19 +1857,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>221</v>
-      </c>
-      <c r="B1" s="56" t="s">
-        <v>62</v>
+      <c r="A1" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>62</v>
+      <c r="A2" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1855,18 +1896,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>221</v>
-      </c>
-      <c r="B1" s="56" t="s">
-        <v>62</v>
+      <c r="A1" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
-        <v>222</v>
-      </c>
-      <c r="B2" s="50" t="s">
+      <c r="A2" s="51" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="49" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1902,11 +1943,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>220</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>62</v>
+      <c r="A2" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2005,11 +2046,11 @@
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="E2" s="50" t="s">
-        <v>237</v>
+      <c r="D2" s="49" t="s">
+        <v>232</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>232</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -2029,7 +2070,7 @@
       <c r="K2" s="5">
         <v>374657342938</v>
       </c>
-      <c r="L2" s="50" t="s">
+      <c r="L2" s="49" t="s">
         <v>26</v>
       </c>
       <c r="M2" s="4" t="s">
@@ -2077,16 +2118,16 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>220</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>220</v>
+      <c r="A2" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2116,180 +2157,180 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="15">
+        <v>456789</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="16">
-        <v>456789</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="J2" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="L2" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="H2" s="16" t="s">
+      <c r="M2" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="N2" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" s="16" t="s">
+      <c r="O2" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="P2" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="Q2" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="R2" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="S2" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="O2" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="P2" s="16" t="s">
+      <c r="T2" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="U2" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="V2" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="W2" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="X2" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="Y2" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="Z2" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA2" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="AB2" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="AC2" s="15" t="s">
         <v>126</v>
-      </c>
-      <c r="Y2" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z2" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="AA2" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB2" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="AC2" s="16" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2317,10 +2358,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -2328,13 +2369,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2358,84 +2399,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
-        <v>215</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="D2" s="52">
+      <c r="A2" s="53" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" s="51">
         <v>930</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
-        <v>215</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="D3" s="52">
+      <c r="A3" s="53" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" s="51">
         <v>930</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
-        <v>215</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>232</v>
+      <c r="A4" s="53" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>227</v>
       </c>
       <c r="D4">
         <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
-        <v>215</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>232</v>
+      <c r="A5" s="53" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>227</v>
       </c>
       <c r="D5">
         <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
-        <v>215</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>232</v>
+      <c r="A6" s="53" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>227</v>
       </c>
       <c r="D6">
         <v>456</v>
@@ -2473,10 +2514,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>36</v>
@@ -2485,42 +2526,42 @@
         <v>31</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>205</v>
+        <v>200</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>201</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>205</v>
+      <c r="D2" s="15" t="s">
+        <v>201</v>
       </c>
       <c r="E2" s="4">
         <v>1234587</v>
       </c>
-      <c r="F2" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>149</v>
+      <c r="F2" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2547,16 +2588,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>32</v>
       </c>
       <c r="E1" s="9" t="s">
@@ -2567,19 +2608,19 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>233</v>
-      </c>
-      <c r="B2" s="52" t="s">
-        <v>229</v>
-      </c>
-      <c r="C2" s="52" t="s">
-        <v>229</v>
-      </c>
-      <c r="D2" s="52">
+      <c r="A2" s="49" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" s="51">
         <v>123.45</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="51" t="s">
         <v>37</v>
       </c>
       <c r="F2" s="10">
@@ -2587,19 +2628,19 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
-        <v>233</v>
-      </c>
-      <c r="B3" s="52" t="s">
-        <v>230</v>
-      </c>
-      <c r="C3" s="52" t="s">
-        <v>230</v>
-      </c>
-      <c r="D3" s="52">
+      <c r="A3" s="49" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>225</v>
+      </c>
+      <c r="D3" s="51">
         <v>123.67</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="51" t="s">
         <v>37</v>
       </c>
       <c r="F3" s="10">
@@ -2705,11 +2746,11 @@
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="50" t="s">
-        <v>236</v>
-      </c>
-      <c r="E2" s="50" t="s">
-        <v>236</v>
+      <c r="D2" s="49" t="s">
+        <v>231</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>231</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>43</v>
@@ -2787,21 +2828,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B2" s="4">
         <v>101200453</v>
@@ -2835,31 +2876,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="36" t="s">
+      <c r="B1" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2892,43 +2933,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>160</v>
-      </c>
-      <c r="E1" s="41" t="s">
+      <c r="B1" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="41">
+        <v>100</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>162</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42">
-        <v>100</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>166</v>
       </c>
       <c r="C2" s="4">
         <v>8564</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" s="42" t="s">
         <v>161</v>
-      </c>
-      <c r="E2" s="43" t="s">
-        <v>164</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2954,31 +2995,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>154</v>
+      <c r="A1" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -3016,11 +3057,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>219</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>219</v>
+      <c r="A2" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3051,31 +3092,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>154</v>
+      <c r="A1" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" s="50" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" s="50" t="s">
-        <v>190</v>
+        <v>130</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="49" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3104,31 +3145,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="36" t="s">
+      <c r="B1" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3156,31 +3197,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="36" t="s">
+      <c r="B1" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3215,11 +3256,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
-        <v>219</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>62</v>
+      <c r="A2" s="53" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -3313,11 +3354,11 @@
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="50" t="s">
-        <v>234</v>
-      </c>
-      <c r="E2" s="50" t="s">
-        <v>234</v>
+      <c r="D2" s="49" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>229</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -3385,10 +3426,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>36</v>
@@ -3397,42 +3438,42 @@
         <v>31</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>206</v>
+        <v>200</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>206</v>
+      <c r="D2" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="E2" s="4">
         <v>1234587</v>
       </c>
-      <c r="F2" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>149</v>
+      <c r="F2" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3459,18 +3500,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
-        <v>197</v>
+      <c r="A2" s="46" t="s">
+        <v>193</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3503,7 +3544,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>38</v>
@@ -3511,10 +3552,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C2" s="4">
         <v>8085</v>
@@ -3553,18 +3594,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -3599,10 +3640,10 @@
         <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3610,13 +3651,13 @@
         <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3646,30 +3687,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>228</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>228</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -3724,7 +3765,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3745,8 +3786,8 @@
       <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="50" t="s">
-        <v>218</v>
+      <c r="B2" s="49" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -3773,10 +3814,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3808,10 +3849,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3829,10 +3870,10 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3841,22 +3882,95 @@
     <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>50</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>235</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>236</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="I1" s="56" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="57">
+        <v>987654</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>241</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" s="57">
+        <v>60101</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>244</v>
+      </c>
+      <c r="H2" s="57">
+        <v>6305551234</v>
+      </c>
+      <c r="I2" s="57" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="57">
+        <v>123456</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="F3" s="57">
+        <v>60148</v>
+      </c>
+      <c r="G3" s="57" t="s">
+        <v>244</v>
+      </c>
+      <c r="H3" s="57">
+        <v>6305559876</v>
+      </c>
+      <c r="I3" s="57" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -3957,11 +4071,11 @@
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="50" t="s">
-        <v>235</v>
-      </c>
-      <c r="E2" s="50" t="s">
-        <v>235</v>
+      <c r="D2" s="49" t="s">
+        <v>230</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>230</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>43</v>
@@ -4041,42 +4155,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="49" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>212</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>68</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D2" s="4">
         <v>967.1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="F2" s="55" t="s">
-        <v>214</v>
+        <v>209</v>
+      </c>
+      <c r="F2" s="54" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -4107,21 +4221,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B2" s="4">
         <v>101000187</v>
@@ -4157,43 +4271,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="B1" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="37">
+        <v>100</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="38">
+        <v>241</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="37" t="s">
-        <v>162</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="38">
-        <v>100</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="39">
-        <v>241</v>
-      </c>
-      <c r="D2" s="38" t="s">
+      <c r="F2" s="39" t="s">
         <v>161</v>
-      </c>
-      <c r="E2" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -4222,42 +4336,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>215</v>
-      </c>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="49" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D2" s="4">
         <v>1234.56</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -4288,42 +4402,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="B1" s="37" t="s">
+      <c r="A1" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="D1" s="37" t="s">
+      <c r="C1" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>194</v>
+      <c r="E1" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>227</v>
+      <c r="A2" s="48" t="s">
+        <v>222</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>208</v>
-      </c>
-      <c r="D2" s="46">
+        <v>58</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="45">
         <v>122105155</v>
       </c>
-      <c r="E2" s="46">
+      <c r="E2" s="45">
         <v>123456789</v>
       </c>
-      <c r="F2" s="46">
+      <c r="F2" s="45">
         <v>123456789</v>
       </c>
     </row>
@@ -4354,42 +4468,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>223</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" s="46">
+      <c r="D2" s="45">
         <v>122105155</v>
       </c>
-      <c r="E2" s="46">
+      <c r="E2" s="45">
         <v>123456789</v>
       </c>
-      <c r="F2" s="46">
+      <c r="F2" s="45">
         <v>123456789</v>
       </c>
     </row>
@@ -4415,25 +4529,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>211</v>
+      <c r="A1" s="50" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" s="52" t="s">
+      <c r="A2" s="52" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="50" t="s">
-        <v>219</v>
+      <c r="C2" s="49" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -4456,11 +4570,11 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52">
+      <c r="A2" s="51">
         <v>999999</v>
       </c>
     </row>
@@ -4483,12 +4597,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>217</v>
+      <c r="A1" s="50" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52">
+      <c r="A2" s="51">
         <v>99999</v>
       </c>
     </row>
@@ -4513,7 +4627,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -4521,10 +4635,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -4552,11 +4666,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
-        <v>199</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>196</v>
+      <c r="A2" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -4642,365 +4756,365 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="G1" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="H1" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="I1" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="J1" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="K1" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="L1" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="K1" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="L1" s="32" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="33">
+      <c r="A2" s="32">
         <v>32002</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="K2" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="L2" s="24" t="s">
-        <v>147</v>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="18">
+      <c r="A3" s="24"/>
+      <c r="B3" s="17">
         <v>100</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="17">
         <v>1000</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="L3" s="26" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>150</v>
+      <c r="D4" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>146</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="L4" s="26" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="18" t="s">
-        <v>148</v>
+      <c r="F5" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="L5" s="26" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>148</v>
+        <v>143</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="L6" s="26" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>148</v>
+        <v>143</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="L7" s="26" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>148</v>
+        <v>143</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="L8" s="26" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>148</v>
+        <v>143</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="L9" s="26" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="L9" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="L10" s="26" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="L10" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="L11" s="27" t="s">
-        <v>148</v>
+        <v>143</v>
+      </c>
+      <c r="L11" s="26" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="20">
+      <c r="A12" s="19">
         <v>33343</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="J12" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>147</v>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="25">
+      <c r="A13" s="24">
         <v>33310</v>
       </c>
       <c r="B13" s="4"/>
@@ -5008,29 +5122,29 @@
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>148</v>
+        <v>143</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="L13" s="26" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="L13" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="25">
+      <c r="A14" s="24">
         <v>33558</v>
       </c>
       <c r="B14" s="4"/>
@@ -5038,29 +5152,29 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>148</v>
+        <v>143</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="L14" s="26" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="L14" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="25">
+      <c r="A15" s="24">
         <v>33280</v>
       </c>
       <c r="B15" s="4"/>
@@ -5068,29 +5182,29 @@
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>148</v>
+        <v>143</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="L15" s="26" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="L15" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="25">
+      <c r="A16" s="24">
         <v>33307</v>
       </c>
       <c r="B16" s="4"/>
@@ -5098,55 +5212,55 @@
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="K16" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="L16" s="26" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="K16" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="L16" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28">
+      <c r="A17" s="27">
         <v>8140</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="I17" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="J17" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="K17" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="L17" s="31" t="s">
-        <v>148</v>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="K17" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="L17" s="30" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -5169,8 +5283,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
-        <v>179</v>
+      <c r="A1" s="43" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -5214,24 +5328,24 @@
         <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>219</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>225</v>
+      <c r="A2" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>220</v>
       </c>
       <c r="D2" s="4">
         <v>100</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>224</v>
+      <c r="E2" s="18" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -5272,24 +5386,24 @@
         <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>219</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>231</v>
+      <c r="A2" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>226</v>
       </c>
       <c r="D2" s="4">
         <v>100</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>226</v>
+      <c r="E2" s="18" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated K sprint tests, added Anils code for factor filter
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2D4ADE3D-6EF3-4908-A840-48C46B255E4A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8EF11087-93AC-4F1D-B08C-27CB1CB7B826}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="248">
   <si>
     <t>Username</t>
   </si>
@@ -836,9 +836,6 @@
     <t>TestCompany1</t>
   </si>
   <si>
-    <t>TestCompany2</t>
-  </si>
-  <si>
     <t>123 Main St</t>
   </si>
   <si>
@@ -854,13 +851,10 @@
     <t>John Doe</t>
   </si>
   <si>
-    <t>456 North Ave</t>
-  </si>
-  <si>
-    <t>Lombard</t>
-  </si>
-  <si>
-    <t>Jane Doe</t>
+    <t>Password@5</t>
+  </si>
+  <si>
+    <t>123457</t>
   </si>
   <si>
     <t>w2k\</t>
@@ -1258,10 +1252,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1548,7 +1542,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1567,7 +1561,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B2" s="49"/>
     </row>
@@ -3787,7 +3781,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>58</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3870,10 +3864,10 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3915,62 +3909,33 @@
         <v>238</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57">
-        <v>987654</v>
-      </c>
-      <c r="B2" s="57" t="s">
+    <row r="2" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="58" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="E2" s="58" t="s">
         <v>242</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="F2" s="58">
+        <v>60101</v>
+      </c>
+      <c r="G2" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="F2" s="57">
-        <v>60101</v>
-      </c>
-      <c r="G2" s="57" t="s">
+      <c r="H2" s="58">
+        <v>6305551234</v>
+      </c>
+      <c r="I2" s="58" t="s">
         <v>244</v>
-      </c>
-      <c r="H2" s="57">
-        <v>6305551234</v>
-      </c>
-      <c r="I2" s="57" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57">
-        <v>123456</v>
-      </c>
-      <c r="B3" s="57" t="s">
-        <v>240</v>
-      </c>
-      <c r="C3" s="57" t="s">
-        <v>246</v>
-      </c>
-      <c r="D3" s="57" t="s">
-        <v>247</v>
-      </c>
-      <c r="E3" s="57" t="s">
-        <v>243</v>
-      </c>
-      <c r="F3" s="57">
-        <v>60148</v>
-      </c>
-      <c r="G3" s="57" t="s">
-        <v>244</v>
-      </c>
-      <c r="H3" s="57">
-        <v>6305559876</v>
-      </c>
-      <c r="I3" s="57" t="s">
-        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test data updated for L sprint
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8EF11087-93AC-4F1D-B08C-27CB1CB7B826}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EF6CF690-79B1-431C-A843-E3C028267498}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="253">
   <si>
     <t>Username</t>
   </si>
@@ -343,12 +343,6 @@
     <t>SearchAmount</t>
   </si>
   <si>
-    <t>carrier820@loadpaytest.truckstop.com</t>
-  </si>
-  <si>
-    <t>Carrier123@0909</t>
-  </si>
-  <si>
     <t>CarrierDOT</t>
   </si>
   <si>
@@ -658,18 +652,6 @@
     <t>070818X5</t>
   </si>
   <si>
-    <t>07/05/2018</t>
-  </si>
-  <si>
-    <t>k carrier</t>
-  </si>
-  <si>
-    <t>08/05/2018</t>
-  </si>
-  <si>
-    <t>Password@12</t>
-  </si>
-  <si>
     <t>Password@90</t>
   </si>
   <si>
@@ -739,16 +721,6 @@
     <t xml:space="preserve">Email </t>
   </si>
   <si>
-    <t>jcglaser@yahoo.com</t>
-  </si>
-  <si>
-    <t>ARTHUR J KENYON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-824811 </t>
-  </si>
-  <si>
     <t>carrier@loadpaytest.truckstop.com</t>
   </si>
   <si>
@@ -785,9 +757,6 @@
     <t>CarrierQAnobankaccount@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>AbcCal12@126</t>
-  </si>
-  <si>
     <t>123NJ7671S</t>
   </si>
   <si>
@@ -855,6 +824,51 @@
   </si>
   <si>
     <t>123457</t>
+  </si>
+  <si>
+    <t>gfqacarrier@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>Truckstop@6</t>
+  </si>
+  <si>
+    <t>Calpion@5</t>
+  </si>
+  <si>
+    <t>Truckstop@5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gfqacarrier@loadpaytest.truckstop.com </t>
+  </si>
+  <si>
+    <t>STEWART MOTOR SERVICE INCORPORATED</t>
+  </si>
+  <si>
+    <t>BNP114</t>
+  </si>
+  <si>
+    <t>carrier32@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>JJH4354D434DE</t>
+  </si>
+  <si>
+    <t>09/06/2018</t>
+  </si>
+  <si>
+    <t>080918TTRKP</t>
+  </si>
+  <si>
+    <t>080918PHTQAD12</t>
+  </si>
+  <si>
+    <t>10/01/2018</t>
+  </si>
+  <si>
+    <t>09/11/2018</t>
   </si>
   <si>
     <t>w2k\</t>
@@ -867,7 +881,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -935,6 +949,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Open_sansregular"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1172,7 +1191,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1233,7 +1252,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1247,15 +1265,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1542,16 +1558,16 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="14.75" customWidth="1"/>
     <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1559,11 +1575,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B2" s="49"/>
+        <v>252</v>
+      </c>
+      <c r="B2" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1578,7 +1594,7 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
@@ -1590,7 +1606,7 @@
     <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1598,42 +1614,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="F2" s="4">
         <v>1111111111</v>
@@ -1661,130 +1677,10 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="4">
-        <v>110</v>
-      </c>
-      <c r="E2" s="4">
-        <v>230</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="4">
-        <v>110</v>
-      </c>
-      <c r="E2" s="4">
-        <v>230</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
@@ -1793,38 +1689,157 @@
     <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
+      <c r="A2" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="C2" s="50">
+        <v>911.4</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="57">
+        <v>896472</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="D2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="4">
-        <v>110</v>
-      </c>
-      <c r="E2" s="4">
-        <v>230</v>
+        <v>245</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" s="50">
+        <v>123.67</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>248</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{BEAAE2F7-7F1D-46BF-888C-471B22906C33}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="50">
+        <v>123.67</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>215</v>
+      </c>
+      <c r="E2" s="50">
+        <v>174912</v>
       </c>
     </row>
   </sheetData>
@@ -1841,35 +1856,34 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1" s="55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{4781DA1A-6424-483A-878E-C1124701B26A}"/>
-    <hyperlink ref="B1" r:id="rId2" xr:uid="{1435F2DD-1D47-4254-9ADA-2479914646F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1880,35 +1894,34 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="37.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1" s="55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="B2" s="49" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DA813998-C10E-45EC-AD16-E22F40C0C23F}"/>
-    <hyperlink ref="B1" r:id="rId2" xr:uid="{31EA81E1-CB98-4D4D-B0F6-4724E540AD60}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1922,13 +1935,13 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="37.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1936,11 +1949,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>215</v>
-      </c>
-      <c r="B2" s="49" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1961,7 +1974,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="14.25" customWidth="1"/>
     <col min="2" max="2" width="16.125" customWidth="1"/>
@@ -1980,7 +1993,7 @@
     <col min="17" max="17" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2033,18 +2046,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="4" customFormat="1">
       <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="49" t="s">
-        <v>232</v>
-      </c>
-      <c r="E2" s="49" t="s">
-        <v>232</v>
+      <c r="D2" s="48" t="s">
+        <v>222</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>222</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -2064,7 +2077,7 @@
       <c r="K2" s="5">
         <v>374657342938</v>
       </c>
-      <c r="L2" s="49" t="s">
+      <c r="L2" s="48" t="s">
         <v>26</v>
       </c>
       <c r="M2" s="4" t="s">
@@ -2102,26 +2115,26 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="39.625" customWidth="1"/>
     <col min="2" max="2" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>215</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>215</v>
+    <row r="2" spans="1:2">
+      <c r="A2" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -2141,7 +2154,7 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
@@ -2149,7 +2162,7 @@
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -2157,90 +2170,90 @@
         <v>36</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AB1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>29</v>
@@ -2249,82 +2262,82 @@
         <v>456789</v>
       </c>
       <c r="D2" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="G2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="I2" s="15" t="s">
         <v>107</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>109</v>
       </c>
       <c r="J2" s="15" t="b">
         <v>1</v>
       </c>
       <c r="K2" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="N2" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="O2" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="P2" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="Q2" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="O2" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="P2" s="15" t="s">
+      <c r="R2" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="S2" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="T2" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="U2" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="V2" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="U2" s="15" t="s">
+      <c r="W2" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="X2" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="15" t="s">
+      <c r="Y2" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="X2" s="15" t="s">
+      <c r="Z2" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA2" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="Y2" s="15" t="s">
+      <c r="AB2" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="Z2" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA2" s="15" t="s">
+      <c r="AC2" s="15" t="s">
         <v>124</v>
-      </c>
-      <c r="AB2" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="AC2" s="15" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2343,33 +2356,33 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2386,91 +2399,91 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:4" s="7" customFormat="1">
+      <c r="A1" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="49" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>211</v>
+    <row r="2" spans="1:4">
+      <c r="A2" s="52" t="s">
+        <v>202</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="D2" s="51">
+        <v>217</v>
+      </c>
+      <c r="D2" s="50">
         <v>930</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
-        <v>211</v>
+    <row r="3" spans="1:4">
+      <c r="A3" s="52" t="s">
+        <v>202</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="D3" s="51">
+        <v>217</v>
+      </c>
+      <c r="D3" s="50">
         <v>930</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
-        <v>211</v>
+    <row r="4" spans="1:4">
+      <c r="A4" s="52" t="s">
+        <v>202</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D4">
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
-        <v>211</v>
+    <row r="5" spans="1:4">
+      <c r="A5" s="52" t="s">
+        <v>202</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D5">
         <v>321</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
-        <v>211</v>
+    <row r="6" spans="1:4">
+      <c r="A6" s="52" t="s">
+        <v>202</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D6">
         <v>456</v>
@@ -2497,7 +2510,7 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
@@ -2506,12 +2519,12 @@
     <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>36</v>
@@ -2520,42 +2533,42 @@
         <v>31</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E2" s="4">
         <v>1234587</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2574,24 +2587,24 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="49" t="s">
         <v>32</v>
       </c>
       <c r="E1" s="9" t="s">
@@ -2601,40 +2614,40 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>228</v>
-      </c>
-      <c r="B2" s="51" t="s">
-        <v>224</v>
-      </c>
-      <c r="C2" s="51" t="s">
-        <v>224</v>
-      </c>
-      <c r="D2" s="51">
+    <row r="2" spans="1:6">
+      <c r="A2" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" s="50">
         <v>123.45</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="50" t="s">
         <v>37</v>
       </c>
       <c r="F2" s="10">
         <v>295676689</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
-        <v>228</v>
-      </c>
-      <c r="B3" s="51" t="s">
-        <v>225</v>
-      </c>
-      <c r="C3" s="51" t="s">
-        <v>225</v>
-      </c>
-      <c r="D3" s="51">
+    <row r="3" spans="1:6">
+      <c r="A3" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" s="50">
         <v>123.67</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="50" t="s">
         <v>37</v>
       </c>
       <c r="F3" s="10">
@@ -2658,7 +2671,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
@@ -2667,7 +2680,7 @@
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2732,7 +2745,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>20</v>
@@ -2740,11 +2753,11 @@
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="49" t="s">
-        <v>231</v>
-      </c>
-      <c r="E2" s="49" t="s">
-        <v>231</v>
+      <c r="D2" s="48" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>221</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>43</v>
@@ -2812,7 +2825,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
@@ -2820,7 +2833,7 @@
     <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>50</v>
       </c>
@@ -2834,7 +2847,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
@@ -2861,7 +2874,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="39.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.25" customWidth="1"/>
@@ -2869,32 +2882,32 @@
     <col min="4" max="4" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D1" s="35" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2917,7 +2930,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13.125" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -2926,7 +2939,7 @@
     <col min="5" max="6" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="40" t="s">
         <v>63</v>
       </c>
@@ -2937,33 +2950,33 @@
         <v>60</v>
       </c>
       <c r="D1" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="E1" s="40" t="s">
-        <v>158</v>
-      </c>
       <c r="F1" s="40" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="A2" s="41">
         <v>100</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C2" s="4">
         <v>8564</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F2" s="42" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2980,7 +2993,7 @@
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
@@ -2988,32 +3001,32 @@
     <col min="4" max="4" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="33" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3036,13 +3049,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41.5" customWidth="1"/>
     <col min="2" max="2" width="40.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -3050,12 +3063,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>214</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>214</v>
+    <row r="2" spans="1:2">
+      <c r="A2" s="48" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3074,10 +3087,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
@@ -3085,39 +3098,38 @@
     <col min="4" max="4" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>185</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>186</v>
-      </c>
-      <c r="D2" s="49" t="s">
-        <v>186</v>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="48" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-1100-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{D398D781-8F73-4F96-84B5-2FDA25BC186C}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{5A92F491-77A0-4C6B-B4A3-2BDA0D7E195B}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{4515284A-FFED-4FEB-A06D-C2A7917388C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3131,39 +3143,39 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="38.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D1" s="35" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -3183,39 +3195,39 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="38.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D1" s="35" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3232,16 +3244,16 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="7" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -3249,17 +3261,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>214</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>58</v>
+    <row r="2" spans="1:2">
+      <c r="A2" s="52" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{6E5A2FE4-2254-4B7A-A522-7E92A8AB6074}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{5A879D72-B638-4C26-B6F0-08F56F24285F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3273,7 +3285,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="13.75" customWidth="1"/>
@@ -3288,7 +3300,7 @@
     <col min="17" max="17" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -3341,18 +3353,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="4" customFormat="1">
       <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="49" t="s">
-        <v>229</v>
-      </c>
-      <c r="E2" s="49" t="s">
-        <v>229</v>
+      <c r="D2" s="48" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>219</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -3409,7 +3421,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
@@ -3418,12 +3430,12 @@
     <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>36</v>
@@ -3432,42 +3444,42 @@
         <v>31</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E2" s="4">
         <v>1234587</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3486,26 +3498,26 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.375" customWidth="1"/>
     <col min="2" max="2" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="s">
-        <v>193</v>
+    <row r="2" spans="1:2" ht="16.5">
+      <c r="A2" s="45" t="s">
+        <v>187</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3519,10 +3531,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
@@ -3530,7 +3542,7 @@
     <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -3538,29 +3550,29 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C2" s="4">
+    <row r="2" spans="1:4">
+      <c r="A2" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="50">
         <v>8085</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="50">
         <v>111111111</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{77B6D251-A399-4301-8FE8-814CDA5D5105}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3571,16 +3583,16 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -3591,20 +3603,21 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="48" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{6C7F39C2-C6D1-4CF0-A27A-4AF213811631}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{24D5BAE4-B4A6-407B-A032-E9E9BA5E812A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3615,10 +3628,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.875" customWidth="1"/>
@@ -3626,7 +3639,7 @@
     <col min="4" max="4" width="39.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -3640,24 +3653,24 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>76</v>
+      <c r="C2" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-1A00-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{179992F2-1670-4B17-B082-015BD7D75FE8}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{D59D87A4-DF72-4075-B8A6-4058F3F60BBB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3668,10 +3681,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
@@ -3679,7 +3692,7 @@
     <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>71</v>
       </c>
@@ -3693,26 +3706,26 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>223</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>223</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>77</v>
+    <row r="2" spans="1:4">
+      <c r="A2" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>239</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-1B00-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-1B00-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{7C773533-52AE-4AA5-9B72-6841282D1F98}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{3CE4B82D-0000-4BB3-AF56-92FD2D52C3E6}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{4E515459-F96C-4BB5-953E-9BD98326FF44}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{4EBE52F9-488E-44A2-9CD7-B84F0CFFCF3E}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{8F25B804-3133-46C9-AD4A-72C432BA3392}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3726,13 +3739,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>49</v>
       </c>
@@ -3740,7 +3753,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="4">
         <v>6542988</v>
       </c>
@@ -3762,13 +3775,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
@@ -3776,12 +3789,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="49" t="s">
-        <v>245</v>
+      <c r="B2" s="48" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -3800,13 +3813,13 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>75</v>
       </c>
@@ -3814,7 +3827,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="4">
         <v>100</v>
       </c>
@@ -3835,13 +3848,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>75</v>
       </c>
@@ -3849,7 +3862,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="4">
         <v>500</v>
       </c>
@@ -3870,7 +3883,7 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
@@ -3880,62 +3893,62 @@
     <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="53" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>226</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>227</v>
+      </c>
+      <c r="I1" s="53" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="54" customFormat="1">
+      <c r="A2" s="55" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>230</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>231</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="F2" s="55">
+        <v>60101</v>
+      </c>
+      <c r="G2" s="55" t="s">
         <v>233</v>
       </c>
-      <c r="B1" s="56" t="s">
-        <v>176</v>
-      </c>
-      <c r="C1" s="56" t="s">
+      <c r="H2" s="55">
+        <v>6305551234</v>
+      </c>
+      <c r="I2" s="55" t="s">
         <v>234</v>
-      </c>
-      <c r="D1" s="56" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="56" t="s">
-        <v>235</v>
-      </c>
-      <c r="F1" s="56" t="s">
-        <v>236</v>
-      </c>
-      <c r="G1" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>237</v>
-      </c>
-      <c r="I1" s="56" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
-        <v>246</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>239</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>240</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>241</v>
-      </c>
-      <c r="E2" s="58" t="s">
-        <v>242</v>
-      </c>
-      <c r="F2" s="58">
-        <v>60101</v>
-      </c>
-      <c r="G2" s="58" t="s">
-        <v>243</v>
-      </c>
-      <c r="H2" s="58">
-        <v>6305551234</v>
-      </c>
-      <c r="I2" s="58" t="s">
-        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -3951,7 +3964,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
@@ -3963,7 +3976,7 @@
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -4028,7 +4041,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>47</v>
@@ -4036,11 +4049,11 @@
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="49" t="s">
-        <v>230</v>
-      </c>
-      <c r="E2" s="49" t="s">
-        <v>230</v>
+      <c r="D2" s="48" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>220</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>43</v>
@@ -4105,10 +4118,10 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
@@ -4118,7 +4131,7 @@
     <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -4138,24 +4151,24 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>208</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A2" s="48" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="4">
-        <v>967.1</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="F2" s="54" t="s">
-        <v>210</v>
+      <c r="D2" s="50">
+        <v>100</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>242</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -4176,7 +4189,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
@@ -4184,7 +4197,7 @@
     <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>50</v>
       </c>
@@ -4198,7 +4211,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
@@ -4225,7 +4238,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -4235,7 +4248,7 @@
     <col min="6" max="6" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="36" t="s">
         <v>63</v>
       </c>
@@ -4246,33 +4259,33 @@
         <v>60</v>
       </c>
       <c r="D1" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="E1" s="36" t="s">
-        <v>158</v>
-      </c>
       <c r="F1" s="36" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="37">
         <v>100</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C2" s="38">
         <v>241</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -4289,7 +4302,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="31.625" customWidth="1"/>
     <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
@@ -4299,7 +4312,7 @@
     <col min="6" max="6" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -4307,7 +4320,7 @@
         <v>57</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>63</v>
@@ -4316,27 +4329,27 @@
         <v>60</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>211</v>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="48" t="s">
+        <v>202</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D2" s="4">
         <v>1234.56</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -4356,7 +4369,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.625" customWidth="1"/>
@@ -4366,43 +4379,43 @@
     <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="19.5" customHeight="1">
       <c r="A1" s="36" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
-        <v>222</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A2" s="47" t="s">
+        <v>213</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="45" t="s">
-        <v>204</v>
-      </c>
-      <c r="D2" s="45">
+      <c r="C2" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="44">
         <v>122105155</v>
       </c>
-      <c r="E2" s="45">
+      <c r="E2" s="44">
         <v>123456789</v>
       </c>
-      <c r="F2" s="45">
+      <c r="F2" s="44">
         <v>123456789</v>
       </c>
     </row>
@@ -4422,7 +4435,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
@@ -4432,43 +4445,43 @@
     <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="36" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
-        <v>218</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" customHeight="1">
+      <c r="A2" s="47" t="s">
+        <v>209</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="45" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="45">
+      <c r="C2" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" s="44">
         <v>122105155</v>
       </c>
-      <c r="E2" s="45">
+      <c r="E2" s="44">
         <v>123456789</v>
       </c>
-      <c r="F2" s="45">
+      <c r="F2" s="44">
         <v>123456789</v>
       </c>
     </row>
@@ -4486,33 +4499,33 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="48" t="s">
         <v>205</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>206</v>
-      </c>
-      <c r="C1" s="50" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -4528,18 +4541,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="50">
         <v>999999</v>
       </c>
     </row>
@@ -4556,18 +4569,18 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51">
+    <row r="1" spans="1:1">
+      <c r="A1" s="49" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="50">
         <v>99999</v>
       </c>
     </row>
@@ -4584,26 +4597,26 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -4620,9 +4633,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4630,12 +4643,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>192</v>
+    <row r="2" spans="1:2" ht="16.5">
+      <c r="A2" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -4652,13 +4665,13 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="35.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4666,7 +4679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -4690,7 +4703,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4704,7 +4717,7 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
@@ -4720,45 +4733,45 @@
     <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="16.5" thickBot="1">
       <c r="A1" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="D1" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="E1" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="F1" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="G1" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="H1" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="K1" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="L1" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="K1" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="L1" s="31" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="32">
         <v>32002</v>
       </c>
@@ -4767,28 +4780,28 @@
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
       <c r="F2" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="24"/>
       <c r="B3" s="17">
         <v>100</v>
@@ -4799,256 +4812,256 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="24"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L4" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="24"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L5" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="24"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="24"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L7" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="24"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L8" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="24"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L9" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="24"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L10" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="16.5" thickBot="1">
       <c r="A11" s="24"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L11" s="26" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="19">
         <v>33343</v>
       </c>
@@ -5057,28 +5070,28 @@
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
       <c r="F12" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I12" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="24">
         <v>33310</v>
       </c>
@@ -5087,28 +5100,28 @@
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L13" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="24">
         <v>33558</v>
       </c>
@@ -5117,28 +5130,28 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="24">
         <v>33280</v>
       </c>
@@ -5147,28 +5160,28 @@
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L15" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="24">
         <v>33307</v>
       </c>
@@ -5177,28 +5190,28 @@
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L16" s="25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="16.5" thickBot="1">
       <c r="A17" s="27">
         <v>8140</v>
       </c>
@@ -5207,25 +5220,25 @@
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="F17" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H17" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I17" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J17" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K17" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L17" s="30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -5242,17 +5255,17 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="43" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" s="13">
         <v>1000</v>
       </c>
@@ -5270,7 +5283,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.75" customWidth="1"/>
@@ -5279,7 +5292,7 @@
     <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -5293,24 +5306,24 @@
         <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>214</v>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="48" t="s">
+        <v>205</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D2" s="4">
         <v>100</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -5329,7 +5342,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="37.5" customWidth="1"/>
     <col min="2" max="3" width="15.25" bestFit="1" customWidth="1"/>
@@ -5337,7 +5350,7 @@
     <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -5351,24 +5364,24 @@
         <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>214</v>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="48" t="s">
+        <v>205</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="D2" s="4">
         <v>100</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
N and L sprint updates - 102318
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{788D861A-B4D8-43BD-AAEC-25C414843EB6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FA1D85B1-1C37-42CA-B274-A09263719364}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="256">
   <si>
     <t>Username</t>
   </si>
@@ -850,25 +850,34 @@
     <t>carrier32@loadpaytest.truckstop.com</t>
   </si>
   <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>JJH4354D434DE</t>
-  </si>
-  <si>
-    <t>09/06/2018</t>
-  </si>
-  <si>
-    <t>080918TTRKP</t>
-  </si>
-  <si>
-    <t>080918PHTQAD12</t>
-  </si>
-  <si>
-    <t>10/01/2018</t>
-  </si>
-  <si>
-    <t>09/11/2018</t>
+    <t>Broker Username</t>
+  </si>
+  <si>
+    <t>Broker Password</t>
+  </si>
+  <si>
+    <t>broker20181017160517@loadpaytest.truckstop.com</t>
+  </si>
+  <si>
+    <t>UM20181017161127</t>
+  </si>
+  <si>
+    <t>10/17/2018</t>
+  </si>
+  <si>
+    <t>UM20181017161133</t>
+  </si>
+  <si>
+    <t>NP20181017160936</t>
+  </si>
+  <si>
+    <t>11/17/2018</t>
+  </si>
+  <si>
+    <t>R123RRDAQ322DQ</t>
+  </si>
+  <si>
+    <t>R123RRDAQ323DQ</t>
   </si>
   <si>
     <t>w2k\</t>
@@ -881,7 +890,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -951,7 +960,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="7"/>
       <color rgb="FF333333"/>
       <name val="Open_sansregular"/>
     </font>
@@ -1191,7 +1200,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1271,7 +1280,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1558,16 +1568,16 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.75" customWidth="1"/>
     <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1575,9 +1585,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B2" s="48"/>
     </row>
@@ -1594,7 +1604,7 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
@@ -1606,7 +1616,7 @@
     <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1635,7 +1645,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>162</v>
       </c>
@@ -1674,180 +1684,225 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="15" t="s">
-        <v>245</v>
-      </c>
-      <c r="B2" s="56" t="s">
-        <v>251</v>
-      </c>
-      <c r="C2" s="50">
-        <v>911.4</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>246</v>
-      </c>
-      <c r="E2" s="57">
-        <v>896472</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="57" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" s="50">
+        <v>120.98</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>248</v>
+      </c>
+      <c r="G2" s="58" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{45D34579-C5E1-482B-AD14-15C0A5B6B9DB}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{728B5BD3-41C7-4FF4-8477-A66DCF830B53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="D2:E2"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="B2" s="51" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="57" t="s">
         <v>247</v>
       </c>
-      <c r="C2" s="50">
+      <c r="B2" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" s="50">
         <v>123.67</v>
       </c>
-      <c r="D2" s="57" t="s">
-        <v>248</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>249</v>
+      <c r="F2" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="G2" s="58" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{BEAAE2F7-7F1D-46BF-888C-471B22906C33}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D90855FC-2247-47E7-85DA-99E1D1D05B7F}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{8A5084F2-9BE5-447D-BE63-6BF3FDF16B88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="50" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="57" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="51" t="s">
-        <v>250</v>
-      </c>
-      <c r="C2" s="50">
-        <v>123.67</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>215</v>
+      <c r="D2" s="51" t="s">
+        <v>252</v>
       </c>
       <c r="E2" s="50">
-        <v>174912</v>
+        <v>930</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="G2" s="58" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="jgmbroker1@loadpaytest.truckstop.com" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{BC8E8D55-2693-4593-B635-67CDDE4AE97D}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{3F3C636D-8FEF-4B8C-AEEF-58DB89578FA4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1859,13 +1914,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
         <v>207</v>
       </c>
@@ -1873,7 +1928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>70</v>
       </c>
@@ -1897,13 +1952,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
         <v>207</v>
       </c>
@@ -1911,7 +1966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>208</v>
       </c>
@@ -1935,13 +1990,13 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1949,7 +2004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>206</v>
       </c>
@@ -1974,7 +2029,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.25" customWidth="1"/>
     <col min="2" max="2" width="16.125" customWidth="1"/>
@@ -1993,7 +2048,7 @@
     <col min="17" max="17" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2046,7 +2101,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1">
+    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2115,13 +2170,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.625" customWidth="1"/>
     <col min="2" max="2" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -2129,7 +2184,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>206</v>
       </c>
@@ -2154,7 +2209,7 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
@@ -2162,7 +2217,7 @@
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -2251,7 +2306,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>102</v>
       </c>
@@ -2356,14 +2411,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>190</v>
       </c>
@@ -2374,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>203</v>
       </c>
@@ -2393,19 +2448,19 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1">
+    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
         <v>28</v>
       </c>
@@ -2419,7 +2474,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>202</v>
       </c>
@@ -2433,7 +2488,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
         <v>202</v>
       </c>
@@ -2447,7 +2502,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>202</v>
       </c>
@@ -2457,11 +2512,11 @@
       <c r="C4" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="D4">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" s="50">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>202</v>
       </c>
@@ -2471,11 +2526,11 @@
       <c r="C5" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="D5">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" s="50">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
         <v>202</v>
       </c>
@@ -2485,7 +2540,77 @@
       <c r="C6" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="50">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" s="50">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" s="50">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" s="50">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" s="50">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D11" s="50">
         <v>456</v>
       </c>
     </row>
@@ -2496,9 +2621,14 @@
     <hyperlink ref="A4" r:id="rId3" xr:uid="{EA87CDFC-A308-4C4B-ADBB-77FC9FB1D4AD}"/>
     <hyperlink ref="A5" r:id="rId4" xr:uid="{C76142B8-E5A1-4F5B-88EB-33862AB73FCC}"/>
     <hyperlink ref="A6" r:id="rId5" xr:uid="{013B6E89-69D3-4071-AC99-48B34CDE2EBB}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{09A6CAD9-9342-4F65-918F-471143302B84}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{0A380C31-F6EB-4BDB-BE6A-F749B98B1946}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{8CDD7FB9-12C9-4455-90DC-A90B840DD04A}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{D7F5E6CC-A0F8-4F23-9640-75AC5472D69E}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{95B0F34C-97F1-4D6B-8511-ABD88C5A833B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -2510,7 +2640,7 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
@@ -2519,7 +2649,7 @@
     <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>181</v>
       </c>
@@ -2545,7 +2675,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>194</v>
       </c>
@@ -2581,20 +2711,20 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
         <v>35</v>
       </c>
@@ -2614,7 +2744,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>218</v>
       </c>
@@ -2634,7 +2764,7 @@
         <v>295676689</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>218</v>
       </c>
@@ -2651,6 +2781,46 @@
         <v>37</v>
       </c>
       <c r="F3" s="10">
+        <v>295676689</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>253</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>253</v>
+      </c>
+      <c r="D4" s="50">
+        <v>123.89</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="10">
+        <v>295676689</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" s="50">
+        <v>124</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="10">
         <v>295676689</v>
       </c>
     </row>
@@ -2658,6 +2828,8 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{8AC65AD8-4A8D-4D4F-9C74-FE1190EF53D3}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{DE157CF1-E748-45D1-850E-D0400BA4C740}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{735ACE70-170A-4355-8049-BF7657C35320}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{77462A2A-ADA7-44EA-B914-6B9DCF18C55E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2671,7 +2843,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
@@ -2680,7 +2852,7 @@
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2745,7 +2917,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>20</v>
@@ -2825,7 +2997,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
@@ -2833,7 +3005,7 @@
     <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>50</v>
       </c>
@@ -2847,7 +3019,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
@@ -2874,7 +3046,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.25" customWidth="1"/>
@@ -2882,7 +3054,7 @@
     <col min="4" max="4" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -2896,7 +3068,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>151</v>
       </c>
@@ -2930,7 +3102,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.125" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -2939,7 +3111,7 @@
     <col min="5" max="6" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>63</v>
       </c>
@@ -2959,7 +3131,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="41">
         <v>100</v>
       </c>
@@ -2993,7 +3165,7 @@
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
@@ -3001,7 +3173,7 @@
     <col min="4" max="4" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>145</v>
       </c>
@@ -3015,7 +3187,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>149</v>
       </c>
@@ -3049,13 +3221,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5" customWidth="1"/>
     <col min="2" max="2" width="40.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -3063,7 +3235,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>205</v>
       </c>
@@ -3090,7 +3262,7 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
@@ -3098,7 +3270,7 @@
     <col min="4" max="4" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>145</v>
       </c>
@@ -3112,7 +3284,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>241</v>
       </c>
@@ -3143,14 +3315,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="38.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -3164,7 +3336,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>128</v>
       </c>
@@ -3195,14 +3367,14 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="38.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -3216,7 +3388,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>128</v>
       </c>
@@ -3247,13 +3419,13 @@
       <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -3261,7 +3433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>237</v>
       </c>
@@ -3285,7 +3457,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="13.75" customWidth="1"/>
@@ -3300,7 +3472,7 @@
     <col min="17" max="17" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -3353,7 +3525,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1">
+    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
@@ -3421,7 +3593,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
@@ -3430,7 +3602,7 @@
     <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>181</v>
       </c>
@@ -3456,7 +3628,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>194</v>
       </c>
@@ -3498,13 +3670,13 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.375" customWidth="1"/>
     <col min="2" max="2" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>145</v>
       </c>
@@ -3512,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5">
+    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
         <v>187</v>
       </c>
@@ -3534,7 +3706,7 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
@@ -3542,7 +3714,7 @@
     <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -3556,7 +3728,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>237</v>
       </c>
@@ -3586,13 +3758,13 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -3603,7 +3775,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>237</v>
       </c>
@@ -3631,7 +3803,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.875" customWidth="1"/>
@@ -3639,7 +3811,7 @@
     <col min="4" max="4" width="39.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -3653,7 +3825,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>37</v>
       </c>
@@ -3684,7 +3856,7 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
@@ -3692,7 +3864,7 @@
     <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>71</v>
       </c>
@@ -3706,7 +3878,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>238</v>
       </c>
@@ -3739,13 +3911,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>49</v>
       </c>
@@ -3753,7 +3925,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>6542988</v>
       </c>
@@ -3775,13 +3947,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
@@ -3789,7 +3961,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
@@ -3813,13 +3985,13 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>75</v>
       </c>
@@ -3827,7 +3999,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>100</v>
       </c>
@@ -3848,13 +4020,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>75</v>
       </c>
@@ -3862,7 +4034,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>500</v>
       </c>
@@ -3883,7 +4055,7 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
@@ -3893,7 +4065,7 @@
     <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>223</v>
       </c>
@@ -3922,7 +4094,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="54" customFormat="1">
+    <row r="2" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>236</v>
       </c>
@@ -3964,7 +4136,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
@@ -3976,7 +4148,7 @@
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -4041,7 +4213,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>47</v>
@@ -4121,7 +4293,7 @@
       <selection activeCell="F2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
@@ -4131,7 +4303,7 @@
     <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -4151,7 +4323,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" customHeight="1">
+    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>241</v>
       </c>
@@ -4189,7 +4361,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
@@ -4197,7 +4369,7 @@
     <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>50</v>
       </c>
@@ -4211,7 +4383,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
@@ -4238,7 +4410,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -4248,7 +4420,7 @@
     <col min="6" max="6" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>63</v>
       </c>
@@ -4268,7 +4440,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="37">
         <v>100</v>
       </c>
@@ -4302,7 +4474,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.625" customWidth="1"/>
     <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
@@ -4312,7 +4484,7 @@
     <col min="6" max="6" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -4332,7 +4504,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>202</v>
       </c>
@@ -4369,7 +4541,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.625" customWidth="1"/>
@@ -4379,7 +4551,7 @@
     <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1">
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>181</v>
       </c>
@@ -4399,7 +4571,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>213</v>
       </c>
@@ -4435,7 +4607,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
@@ -4445,7 +4617,7 @@
     <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>181</v>
       </c>
@@ -4465,7 +4637,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>209</v>
       </c>
@@ -4499,14 +4671,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
         <v>199</v>
       </c>
@@ -4517,7 +4689,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>127</v>
       </c>
@@ -4541,17 +4713,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="50">
         <v>999999</v>
       </c>
@@ -4569,17 +4741,17 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="50">
         <v>99999</v>
       </c>
@@ -4597,13 +4769,13 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>145</v>
       </c>
@@ -4611,7 +4783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>189</v>
       </c>
@@ -4633,9 +4805,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4643,7 +4815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5">
+    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
         <v>189</v>
       </c>
@@ -4665,13 +4837,13 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4679,7 +4851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -4703,7 +4875,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4717,7 +4889,7 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
@@ -4733,7 +4905,7 @@
     <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickBot="1">
+    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>129</v>
       </c>
@@ -4771,7 +4943,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32">
         <v>32002</v>
       </c>
@@ -4801,7 +4973,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="17">
         <v>100</v>
@@ -4833,7 +5005,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -4865,7 +5037,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -4893,7 +5065,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -4921,7 +5093,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -4949,7 +5121,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -4977,7 +5149,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -5005,7 +5177,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -5033,7 +5205,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16.5" thickBot="1">
+    <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -5061,7 +5233,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>33343</v>
       </c>
@@ -5091,7 +5263,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
         <v>33310</v>
       </c>
@@ -5121,7 +5293,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="24">
         <v>33558</v>
       </c>
@@ -5151,7 +5323,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="24">
         <v>33280</v>
       </c>
@@ -5181,7 +5353,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="24">
         <v>33307</v>
       </c>
@@ -5211,7 +5383,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16.5" thickBot="1">
+    <row r="17" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27">
         <v>8140</v>
       </c>
@@ -5255,17 +5427,17 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1000</v>
       </c>
@@ -5283,7 +5455,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.75" customWidth="1"/>
@@ -5292,7 +5464,7 @@
     <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -5309,7 +5481,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>205</v>
       </c>
@@ -5342,7 +5514,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5" customWidth="1"/>
     <col min="2" max="3" width="15.25" bestFit="1" customWidth="1"/>
@@ -5350,7 +5522,7 @@
     <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -5367,7 +5539,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>205</v>
       </c>

</xml_diff>

<commit_message>
L sprint updates - 102418
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FA1D85B1-1C37-42CA-B274-A09263719364}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4B3C8694-A5A3-4B67-AE5F-534149448B90}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="257">
   <si>
     <t>Username</t>
   </si>
@@ -868,16 +868,19 @@
     <t>UM20181017161133</t>
   </si>
   <si>
-    <t>NP20181017160936</t>
-  </si>
-  <si>
-    <t>11/17/2018</t>
-  </si>
-  <si>
     <t>R123RRDAQ322DQ</t>
   </si>
   <si>
     <t>R123RRDAQ323DQ</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>11/09/2018</t>
+  </si>
+  <si>
+    <t>NP123456789</t>
   </si>
   <si>
     <t>w2k\</t>
@@ -890,7 +893,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -961,6 +964,11 @@
     </font>
     <font>
       <sz val="7"/>
+      <color rgb="FF333333"/>
+      <name val="Open_sansregular"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FF333333"/>
       <name val="Open_sansregular"/>
     </font>
@@ -1200,7 +1208,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1282,6 +1290,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1571,13 +1580,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="14.75" customWidth="1"/>
     <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1585,9 +1594,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B2" s="48"/>
     </row>
@@ -1604,7 +1613,7 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
@@ -1616,7 +1625,7 @@
     <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1645,7 +1654,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>162</v>
       </c>
@@ -1690,7 +1699,7 @@
       <selection activeCell="C2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
@@ -1701,7 +1710,7 @@
     <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="49" t="s">
         <v>245</v>
       </c>
@@ -1724,7 +1733,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="57" t="s">
         <v>247</v>
       </c>
@@ -1765,7 +1774,7 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
@@ -1775,7 +1784,7 @@
     <col min="6" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="49" t="s">
         <v>245</v>
       </c>
@@ -1798,7 +1807,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="57" t="s">
         <v>247</v>
       </c>
@@ -1836,10 +1845,10 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
@@ -1850,7 +1859,7 @@
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="49" t="s">
         <v>245</v>
       </c>
@@ -1873,7 +1882,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="57" t="s">
         <v>247</v>
       </c>
@@ -1881,19 +1890,19 @@
         <v>26</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>29</v>
+        <v>253</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="E2" s="50">
-        <v>930</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>251</v>
-      </c>
-      <c r="G2" s="58" t="s">
-        <v>251</v>
+        <v>456.78</v>
+      </c>
+      <c r="F2" s="59">
+        <v>789654123</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -1914,13 +1923,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="49" t="s">
         <v>207</v>
       </c>
@@ -1928,7 +1937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="50" t="s">
         <v>70</v>
       </c>
@@ -1952,13 +1961,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="37.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="49" t="s">
         <v>207</v>
       </c>
@@ -1966,7 +1975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="50" t="s">
         <v>208</v>
       </c>
@@ -1990,13 +1999,13 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="37.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2004,7 +2013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="48" t="s">
         <v>206</v>
       </c>
@@ -2029,7 +2038,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="14.25" customWidth="1"/>
     <col min="2" max="2" width="16.125" customWidth="1"/>
@@ -2048,7 +2057,7 @@
     <col min="17" max="17" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2101,7 +2110,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="4" customFormat="1">
       <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2170,13 +2179,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="39.625" customWidth="1"/>
     <col min="2" max="2" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -2184,7 +2193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="48" t="s">
         <v>206</v>
       </c>
@@ -2209,7 +2218,7 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
@@ -2217,7 +2226,7 @@
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -2306,7 +2315,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29">
       <c r="A2" s="2" t="s">
         <v>102</v>
       </c>
@@ -2411,14 +2420,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>190</v>
       </c>
@@ -2429,7 +2438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
         <v>203</v>
       </c>
@@ -2454,13 +2463,13 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="7" customFormat="1">
       <c r="A1" s="49" t="s">
         <v>28</v>
       </c>
@@ -2474,7 +2483,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="52" t="s">
         <v>202</v>
       </c>
@@ -2488,7 +2497,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="52" t="s">
         <v>202</v>
       </c>
@@ -2502,7 +2511,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="52" t="s">
         <v>202</v>
       </c>
@@ -2516,7 +2525,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="52" t="s">
         <v>202</v>
       </c>
@@ -2530,7 +2539,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="52" t="s">
         <v>202</v>
       </c>
@@ -2544,7 +2553,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="52" t="s">
         <v>202</v>
       </c>
@@ -2558,7 +2567,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="52" t="s">
         <v>202</v>
       </c>
@@ -2572,7 +2581,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="52" t="s">
         <v>202</v>
       </c>
@@ -2586,7 +2595,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="52" t="s">
         <v>202</v>
       </c>
@@ -2600,7 +2609,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="52" t="s">
         <v>202</v>
       </c>
@@ -2640,7 +2649,7 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
@@ -2649,7 +2658,7 @@
     <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>181</v>
       </c>
@@ -2675,7 +2684,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>194</v>
       </c>
@@ -2717,14 +2726,14 @@
       <selection activeCell="C3" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="16.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="49" t="s">
         <v>35</v>
       </c>
@@ -2744,7 +2753,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="48" t="s">
         <v>218</v>
       </c>
@@ -2764,7 +2773,7 @@
         <v>295676689</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="48" t="s">
         <v>218</v>
       </c>
@@ -2784,15 +2793,15 @@
         <v>295676689</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="48" t="s">
         <v>218</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D4" s="50">
         <v>123.89</v>
@@ -2804,15 +2813,15 @@
         <v>295676689</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="48" t="s">
         <v>218</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D5" s="50">
         <v>124</v>
@@ -2843,7 +2852,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
@@ -2852,7 +2861,7 @@
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2917,7 +2926,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>20</v>
@@ -2997,7 +3006,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
@@ -3005,7 +3014,7 @@
     <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>50</v>
       </c>
@@ -3019,7 +3028,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
@@ -3046,7 +3055,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="39.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.25" customWidth="1"/>
@@ -3054,7 +3063,7 @@
     <col min="4" max="4" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -3068,7 +3077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>151</v>
       </c>
@@ -3102,7 +3111,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13.125" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -3111,7 +3120,7 @@
     <col min="5" max="6" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="40" t="s">
         <v>63</v>
       </c>
@@ -3131,7 +3140,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="A2" s="41">
         <v>100</v>
       </c>
@@ -3165,7 +3174,7 @@
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
@@ -3173,7 +3182,7 @@
     <col min="4" max="4" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="33" t="s">
         <v>145</v>
       </c>
@@ -3187,7 +3196,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>149</v>
       </c>
@@ -3221,13 +3230,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41.5" customWidth="1"/>
     <col min="2" max="2" width="40.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -3235,7 +3244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="48" t="s">
         <v>205</v>
       </c>
@@ -3262,7 +3271,7 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
@@ -3270,7 +3279,7 @@
     <col min="4" max="4" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="33" t="s">
         <v>145</v>
       </c>
@@ -3284,7 +3293,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="48" t="s">
         <v>241</v>
       </c>
@@ -3315,14 +3324,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="38.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -3336,7 +3345,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>128</v>
       </c>
@@ -3367,14 +3376,14 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="38.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -3388,7 +3397,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>128</v>
       </c>
@@ -3419,13 +3428,13 @@
       <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="7" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -3433,7 +3442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="52" t="s">
         <v>237</v>
       </c>
@@ -3457,7 +3466,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="13.75" customWidth="1"/>
@@ -3472,7 +3481,7 @@
     <col min="17" max="17" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -3525,7 +3534,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="4" customFormat="1">
       <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
@@ -3593,7 +3602,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
@@ -3602,7 +3611,7 @@
     <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>181</v>
       </c>
@@ -3628,7 +3637,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>194</v>
       </c>
@@ -3670,13 +3679,13 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.375" customWidth="1"/>
     <col min="2" max="2" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>145</v>
       </c>
@@ -3684,7 +3693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16.5">
       <c r="A2" s="45" t="s">
         <v>187</v>
       </c>
@@ -3706,7 +3715,7 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
@@ -3714,7 +3723,7 @@
     <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -3728,7 +3737,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="48" t="s">
         <v>237</v>
       </c>
@@ -3758,13 +3767,13 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -3775,7 +3784,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="48" t="s">
         <v>237</v>
       </c>
@@ -3803,7 +3812,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.875" customWidth="1"/>
@@ -3811,7 +3820,7 @@
     <col min="4" max="4" width="39.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -3825,7 +3834,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="50" t="s">
         <v>37</v>
       </c>
@@ -3856,7 +3865,7 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
@@ -3864,7 +3873,7 @@
     <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>71</v>
       </c>
@@ -3878,7 +3887,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="48" t="s">
         <v>238</v>
       </c>
@@ -3911,13 +3920,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>49</v>
       </c>
@@ -3925,7 +3934,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="4">
         <v>6542988</v>
       </c>
@@ -3947,13 +3956,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
@@ -3961,7 +3970,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
@@ -3985,13 +3994,13 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>75</v>
       </c>
@@ -3999,7 +4008,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="4">
         <v>100</v>
       </c>
@@ -4020,13 +4029,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>75</v>
       </c>
@@ -4034,7 +4043,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="4">
         <v>500</v>
       </c>
@@ -4055,7 +4064,7 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
@@ -4065,7 +4074,7 @@
     <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="53" t="s">
         <v>223</v>
       </c>
@@ -4094,7 +4103,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="54" customFormat="1">
       <c r="A2" s="55" t="s">
         <v>236</v>
       </c>
@@ -4136,7 +4145,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
@@ -4148,7 +4157,7 @@
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -4213,7 +4222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>47</v>
@@ -4293,7 +4302,7 @@
       <selection activeCell="F2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
@@ -4303,7 +4312,7 @@
     <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -4323,7 +4332,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="48" t="s">
         <v>241</v>
       </c>
@@ -4361,7 +4370,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
@@ -4369,7 +4378,7 @@
     <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>50</v>
       </c>
@@ -4383,7 +4392,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
@@ -4410,7 +4419,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
@@ -4420,7 +4429,7 @@
     <col min="6" max="6" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="36" t="s">
         <v>63</v>
       </c>
@@ -4440,7 +4449,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="37">
         <v>100</v>
       </c>
@@ -4474,7 +4483,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="31.625" customWidth="1"/>
     <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
@@ -4484,7 +4493,7 @@
     <col min="6" max="6" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -4504,7 +4513,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="48" t="s">
         <v>202</v>
       </c>
@@ -4541,7 +4550,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.625" customWidth="1"/>
@@ -4551,7 +4560,7 @@
     <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="19.5" customHeight="1">
       <c r="A1" s="36" t="s">
         <v>181</v>
       </c>
@@ -4571,7 +4580,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="47" t="s">
         <v>213</v>
       </c>
@@ -4607,7 +4616,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
@@ -4617,7 +4626,7 @@
     <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="36" t="s">
         <v>181</v>
       </c>
@@ -4637,7 +4646,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="A2" s="47" t="s">
         <v>209</v>
       </c>
@@ -4671,14 +4680,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="49" t="s">
         <v>199</v>
       </c>
@@ -4689,7 +4698,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="51" t="s">
         <v>127</v>
       </c>
@@ -4713,17 +4722,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="8" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="50">
         <v>999999</v>
       </c>
@@ -4741,17 +4750,17 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="49" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="50">
         <v>99999</v>
       </c>
@@ -4769,13 +4778,13 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>145</v>
       </c>
@@ -4783,7 +4792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
         <v>189</v>
       </c>
@@ -4805,9 +4814,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4815,7 +4824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16.5">
       <c r="A2" s="45" t="s">
         <v>189</v>
       </c>
@@ -4837,13 +4846,13 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="35.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4851,7 +4860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -4875,7 +4884,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4889,7 +4898,7 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
@@ -4905,7 +4914,7 @@
     <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="16.5" thickBot="1">
       <c r="A1" s="31" t="s">
         <v>129</v>
       </c>
@@ -4943,7 +4952,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="32">
         <v>32002</v>
       </c>
@@ -4973,7 +4982,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="24"/>
       <c r="B3" s="17">
         <v>100</v>
@@ -5005,7 +5014,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="24"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -5037,7 +5046,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="24"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -5065,7 +5074,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="24"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -5093,7 +5102,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="24"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -5121,7 +5130,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="24"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -5149,7 +5158,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="24"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -5177,7 +5186,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="24"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -5205,7 +5214,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="16.5" thickBot="1">
       <c r="A11" s="24"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -5233,7 +5242,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="19">
         <v>33343</v>
       </c>
@@ -5263,7 +5272,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="24">
         <v>33310</v>
       </c>
@@ -5293,7 +5302,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="24">
         <v>33558</v>
       </c>
@@ -5323,7 +5332,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="24">
         <v>33280</v>
       </c>
@@ -5353,7 +5362,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="24">
         <v>33307</v>
       </c>
@@ -5383,7 +5392,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="16.5" thickBot="1">
       <c r="A17" s="27">
         <v>8140</v>
       </c>
@@ -5427,17 +5436,17 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="43" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="13">
         <v>1000</v>
       </c>
@@ -5455,7 +5464,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.75" customWidth="1"/>
@@ -5464,7 +5473,7 @@
     <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -5481,7 +5490,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="48" t="s">
         <v>205</v>
       </c>
@@ -5514,7 +5523,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="37.5" customWidth="1"/>
     <col min="2" max="3" width="15.25" bestFit="1" customWidth="1"/>
@@ -5522,7 +5531,7 @@
     <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -5539,7 +5548,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="48" t="s">
         <v>205</v>
       </c>

</xml_diff>

<commit_message>
J and L Sprint updates - 102818
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4B3C8694-A5A3-4B67-AE5F-534149448B90}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{802D2D12-387E-4140-9B4C-E7B2792ABE8D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="257">
   <si>
     <t>Username</t>
   </si>
@@ -1577,13 +1577,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="14.75" customWidth="1"/>
-    <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.69921875" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1613,16 +1613,16 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1699,15 +1699,15 @@
       <selection activeCell="C2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1774,13 +1774,13 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="45.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.69921875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1848,14 +1848,14 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="45.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.8984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1923,10 +1923,10 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1961,9 +1961,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1999,9 +1999,9 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2038,22 +2038,22 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="14.25" customWidth="1"/>
-    <col min="2" max="2" width="16.125" customWidth="1"/>
-    <col min="3" max="3" width="17.875" customWidth="1"/>
-    <col min="4" max="4" width="35.75" customWidth="1"/>
-    <col min="5" max="5" width="36.375" customWidth="1"/>
-    <col min="6" max="6" width="12.875" customWidth="1"/>
-    <col min="9" max="9" width="11.875" customWidth="1"/>
-    <col min="10" max="10" width="12.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="15.25" customWidth="1"/>
-    <col min="13" max="13" width="14.75" customWidth="1"/>
-    <col min="14" max="14" width="15.875" customWidth="1"/>
-    <col min="15" max="15" width="15.25" customWidth="1"/>
-    <col min="16" max="16" width="16.25" customWidth="1"/>
+    <col min="1" max="1" width="14.19921875" customWidth="1"/>
+    <col min="2" max="2" width="16.09765625" customWidth="1"/>
+    <col min="3" max="3" width="17.8984375" customWidth="1"/>
+    <col min="4" max="4" width="35.69921875" customWidth="1"/>
+    <col min="5" max="5" width="36.3984375" customWidth="1"/>
+    <col min="6" max="6" width="12.8984375" customWidth="1"/>
+    <col min="9" max="9" width="11.8984375" customWidth="1"/>
+    <col min="10" max="10" width="12.09765625" customWidth="1"/>
+    <col min="11" max="11" width="14.3984375" customWidth="1"/>
+    <col min="12" max="12" width="15.19921875" customWidth="1"/>
+    <col min="13" max="13" width="14.69921875" customWidth="1"/>
+    <col min="14" max="14" width="15.8984375" customWidth="1"/>
+    <col min="15" max="15" width="15.19921875" customWidth="1"/>
+    <col min="16" max="16" width="16.19921875" customWidth="1"/>
     <col min="17" max="17" width="27" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2179,10 +2179,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="39.625" customWidth="1"/>
-    <col min="2" max="2" width="44.25" customWidth="1"/>
+    <col min="1" max="1" width="39.59765625" customWidth="1"/>
+    <col min="2" max="2" width="44.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2218,11 +2218,11 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2420,11 +2420,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2463,10 +2463,10 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1">
@@ -2649,13 +2649,13 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2726,11 +2726,11 @@
       <selection activeCell="C3" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2852,12 +2852,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="35.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="35.19921875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3006,12 +3006,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3055,12 +3055,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="39.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.25" customWidth="1"/>
-    <col min="3" max="3" width="20.75" customWidth="1"/>
-    <col min="4" max="4" width="25.25" customWidth="1"/>
+    <col min="1" max="1" width="39.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.19921875" customWidth="1"/>
+    <col min="3" max="3" width="20.69921875" customWidth="1"/>
+    <col min="4" max="4" width="25.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3108,19 +3108,19 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="13.125" customWidth="1"/>
+    <col min="1" max="1" width="13.09765625" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="31.2">
       <c r="A1" s="40" t="s">
         <v>63</v>
       </c>
@@ -3150,8 +3150,8 @@
       <c r="C2" s="4">
         <v>8564</v>
       </c>
-      <c r="D2" s="41" t="s">
-        <v>155</v>
+      <c r="D2" s="41">
+        <v>1000</v>
       </c>
       <c r="E2" s="42" t="s">
         <v>158</v>
@@ -3174,12 +3174,12 @@
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.625" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" customWidth="1"/>
+    <col min="4" max="4" width="17.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3230,10 +3230,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="41.5" customWidth="1"/>
-    <col min="2" max="2" width="40.75" customWidth="1"/>
+    <col min="2" max="2" width="40.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3271,12 +3271,12 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.09765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3324,11 +3324,11 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="38.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3376,11 +3376,11 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="2" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3428,7 +3428,7 @@
       <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
@@ -3466,18 +3466,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="13.75" customWidth="1"/>
-    <col min="3" max="3" width="10.25" customWidth="1"/>
+    <col min="2" max="2" width="13.69921875" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="35.875" customWidth="1"/>
+    <col min="5" max="5" width="35.8984375" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="11" max="12" width="14.625" customWidth="1"/>
+    <col min="11" max="12" width="14.59765625" customWidth="1"/>
     <col min="13" max="13" width="15.5" customWidth="1"/>
-    <col min="15" max="15" width="13.75" customWidth="1"/>
-    <col min="16" max="16" width="12.625" customWidth="1"/>
+    <col min="15" max="15" width="13.69921875" customWidth="1"/>
+    <col min="16" max="16" width="12.59765625" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3602,13 +3602,13 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3679,10 +3679,10 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
+    <col min="2" max="2" width="15.09765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3693,7 +3693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5">
+    <row r="2" spans="1:2" ht="16.8">
       <c r="A2" s="45" t="s">
         <v>187</v>
       </c>
@@ -3715,12 +3715,12 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="41.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3767,10 +3767,10 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3812,12 +3812,12 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="1" max="1" width="9.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.8984375" customWidth="1"/>
     <col min="3" max="3" width="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3865,12 +3865,12 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3920,9 +3920,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3956,10 +3956,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3994,10 +3994,10 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4029,10 +4029,10 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4064,14 +4064,14 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4145,15 +4145,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="34.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="34.09765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.8984375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4302,14 +4302,14 @@
       <selection activeCell="F2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4370,12 +4370,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4419,17 +4419,17 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.09765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.69921875" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="31.2">
       <c r="A1" s="36" t="s">
         <v>63</v>
       </c>
@@ -4483,14 +4483,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="31.625" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.59765625" customWidth="1"/>
+    <col min="2" max="2" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4550,14 +4550,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.625" customWidth="1"/>
-    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" customWidth="1"/>
-    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.09765625" customWidth="1"/>
+    <col min="6" max="6" width="20.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" customHeight="1">
@@ -4616,17 +4616,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="31.2">
       <c r="A1" s="36" t="s">
         <v>181</v>
       </c>
@@ -4680,11 +4680,11 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.69921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4722,9 +4722,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="15.25" customWidth="1"/>
+    <col min="1" max="1" width="15.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -4750,9 +4750,9 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -4778,10 +4778,10 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4814,7 +4814,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
@@ -4824,7 +4824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5">
+    <row r="2" spans="1:2" ht="16.8">
       <c r="A2" s="45" t="s">
         <v>189</v>
       </c>
@@ -4846,10 +4846,10 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="35.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4884,7 +4884,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4898,23 +4898,23 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.09765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickBot="1">
+    <row r="1" spans="1:12" ht="16.2" thickBot="1">
       <c r="A1" s="31" t="s">
         <v>129</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16.5" thickBot="1">
+    <row r="11" spans="1:12" ht="16.2" thickBot="1">
       <c r="A11" s="24"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -5392,7 +5392,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16.5" thickBot="1">
+    <row r="17" spans="1:12" ht="16.2" thickBot="1">
       <c r="A17" s="27">
         <v>8140</v>
       </c>
@@ -5436,9 +5436,9 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -5464,13 +5464,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.75" customWidth="1"/>
-    <col min="3" max="3" width="12.625" customWidth="1"/>
-    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.69921875" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" customWidth="1"/>
+    <col min="4" max="4" width="7.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5523,12 +5523,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="37.5" customWidth="1"/>
-    <col min="2" max="3" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
J sprint updates - 102918
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{802D2D12-387E-4140-9B4C-E7B2792ABE8D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0CB57986-583D-4CC7-8717-64E8C58FBBAB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="257">
   <si>
     <t>Username</t>
   </si>
@@ -1580,10 +1580,10 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="14.69921875" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.75" customWidth="1"/>
+    <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1613,16 +1613,16 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="41.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.09765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1699,15 +1699,15 @@
       <selection activeCell="C2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.09765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1774,13 +1774,13 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="45.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1848,14 +1848,14 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="45.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.09765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1923,10 +1923,10 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1961,9 +1961,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="37.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1999,9 +1999,9 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="37.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2038,22 +2038,22 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="14.19921875" customWidth="1"/>
-    <col min="2" max="2" width="16.09765625" customWidth="1"/>
-    <col min="3" max="3" width="17.8984375" customWidth="1"/>
-    <col min="4" max="4" width="35.69921875" customWidth="1"/>
-    <col min="5" max="5" width="36.3984375" customWidth="1"/>
-    <col min="6" max="6" width="12.8984375" customWidth="1"/>
-    <col min="9" max="9" width="11.8984375" customWidth="1"/>
-    <col min="10" max="10" width="12.09765625" customWidth="1"/>
-    <col min="11" max="11" width="14.3984375" customWidth="1"/>
-    <col min="12" max="12" width="15.19921875" customWidth="1"/>
-    <col min="13" max="13" width="14.69921875" customWidth="1"/>
-    <col min="14" max="14" width="15.8984375" customWidth="1"/>
-    <col min="15" max="15" width="15.19921875" customWidth="1"/>
-    <col min="16" max="16" width="16.19921875" customWidth="1"/>
+    <col min="1" max="1" width="14.25" customWidth="1"/>
+    <col min="2" max="2" width="16.125" customWidth="1"/>
+    <col min="3" max="3" width="17.875" customWidth="1"/>
+    <col min="4" max="4" width="35.75" customWidth="1"/>
+    <col min="5" max="5" width="36.375" customWidth="1"/>
+    <col min="6" max="6" width="12.875" customWidth="1"/>
+    <col min="9" max="9" width="11.875" customWidth="1"/>
+    <col min="10" max="10" width="12.125" customWidth="1"/>
+    <col min="11" max="11" width="14.375" customWidth="1"/>
+    <col min="12" max="12" width="15.25" customWidth="1"/>
+    <col min="13" max="13" width="14.75" customWidth="1"/>
+    <col min="14" max="14" width="15.875" customWidth="1"/>
+    <col min="15" max="15" width="15.25" customWidth="1"/>
+    <col min="16" max="16" width="16.25" customWidth="1"/>
     <col min="17" max="17" width="27" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2179,10 +2179,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="39.59765625" customWidth="1"/>
-    <col min="2" max="2" width="44.19921875" customWidth="1"/>
+    <col min="1" max="1" width="39.625" customWidth="1"/>
+    <col min="2" max="2" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2218,11 +2218,11 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.09765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2420,11 +2420,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2457,16 +2457,16 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1">
@@ -2536,7 +2536,7 @@
         <v>217</v>
       </c>
       <c r="D5" s="50">
-        <v>930</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2550,7 +2550,7 @@
         <v>217</v>
       </c>
       <c r="D6" s="50">
-        <v>930</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2564,62 +2564,6 @@
         <v>217</v>
       </c>
       <c r="D7" s="50">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="52" t="s">
-        <v>202</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="D8" s="50">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="52" t="s">
-        <v>202</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="D9" s="50">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="52" t="s">
-        <v>202</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="D10" s="50">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="52" t="s">
-        <v>202</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="D11" s="50">
         <v>456</v>
       </c>
     </row>
@@ -2628,16 +2572,12 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{6BD736EF-0A9A-4295-8C91-8829EF333F40}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{E95E0960-C996-46E2-9866-0BD7AB7CC179}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{EA87CDFC-A308-4C4B-ADBB-77FC9FB1D4AD}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{C76142B8-E5A1-4F5B-88EB-33862AB73FCC}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{013B6E89-69D3-4071-AC99-48B34CDE2EBB}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{09A6CAD9-9342-4F65-918F-471143302B84}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{0A380C31-F6EB-4BDB-BE6A-F749B98B1946}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{8CDD7FB9-12C9-4455-90DC-A90B840DD04A}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{D7F5E6CC-A0F8-4F23-9640-75AC5472D69E}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{95B0F34C-97F1-4D6B-8511-ABD88C5A833B}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{8CDD7FB9-12C9-4455-90DC-A90B840DD04A}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{D7F5E6CC-A0F8-4F23-9640-75AC5472D69E}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{95B0F34C-97F1-4D6B-8511-ABD88C5A833B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -2649,13 +2589,13 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2726,11 +2666,11 @@
       <selection activeCell="C3" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.69921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2852,12 +2792,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="35.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="35.25" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3006,12 +2946,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3055,12 +2995,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="39.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.19921875" customWidth="1"/>
-    <col min="3" max="3" width="20.69921875" customWidth="1"/>
-    <col min="4" max="4" width="25.19921875" customWidth="1"/>
+    <col min="1" max="1" width="39.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.25" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
+    <col min="4" max="4" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3111,16 +3051,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.09765625" customWidth="1"/>
+    <col min="1" max="1" width="13.125" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="40" t="s">
         <v>63</v>
       </c>
@@ -3174,12 +3114,12 @@
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.59765625" customWidth="1"/>
-    <col min="4" max="4" width="17.8984375" customWidth="1"/>
+    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.625" customWidth="1"/>
+    <col min="4" max="4" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3230,10 +3170,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41.5" customWidth="1"/>
-    <col min="2" max="2" width="40.69921875" customWidth="1"/>
+    <col min="2" max="2" width="40.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3271,12 +3211,12 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.09765625" customWidth="1"/>
+    <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3324,11 +3264,11 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="38.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3376,11 +3316,11 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3428,7 +3368,7 @@
       <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
@@ -3466,18 +3406,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="13.69921875" customWidth="1"/>
-    <col min="3" max="3" width="10.19921875" customWidth="1"/>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="10.25" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="35.8984375" customWidth="1"/>
+    <col min="5" max="5" width="35.875" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="11" max="12" width="14.59765625" customWidth="1"/>
+    <col min="11" max="12" width="14.625" customWidth="1"/>
     <col min="13" max="13" width="15.5" customWidth="1"/>
-    <col min="15" max="15" width="13.69921875" customWidth="1"/>
-    <col min="16" max="16" width="12.59765625" customWidth="1"/>
+    <col min="15" max="15" width="13.75" customWidth="1"/>
+    <col min="16" max="16" width="12.625" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3602,13 +3542,13 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3679,10 +3619,10 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.3984375" customWidth="1"/>
-    <col min="2" max="2" width="15.09765625" customWidth="1"/>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="2" max="2" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3693,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.8">
+    <row r="2" spans="1:2" ht="16.5">
       <c r="A2" s="45" t="s">
         <v>187</v>
       </c>
@@ -3715,12 +3655,12 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="41.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3767,10 +3707,10 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="38.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3812,12 +3752,12 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.8984375" customWidth="1"/>
+    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
     <col min="3" max="3" width="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3865,12 +3805,12 @@
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3920,9 +3860,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3956,10 +3896,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="23.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3994,10 +3934,10 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4029,10 +3969,10 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4064,14 +4004,14 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4145,15 +4085,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="34.09765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4302,14 +4242,14 @@
       <selection activeCell="F2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4370,12 +4310,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4419,17 +4359,17 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.69921875" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="36" t="s">
         <v>63</v>
       </c>
@@ -4483,14 +4423,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="31.59765625" customWidth="1"/>
-    <col min="2" max="2" width="14.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.625" customWidth="1"/>
+    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4550,14 +4490,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.59765625" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.09765625" customWidth="1"/>
-    <col min="6" max="6" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
+    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.125" customWidth="1"/>
+    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" customHeight="1">
@@ -4616,17 +4556,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="36" t="s">
         <v>181</v>
       </c>
@@ -4680,11 +4620,11 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4722,9 +4662,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="15.19921875" customWidth="1"/>
+    <col min="1" max="1" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -4750,9 +4690,9 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -4778,10 +4718,10 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4814,7 +4754,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
@@ -4824,7 +4764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.8">
+    <row r="2" spans="1:2" ht="16.5">
       <c r="A2" s="45" t="s">
         <v>189</v>
       </c>
@@ -4846,10 +4786,10 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="35.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4884,7 +4824,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4898,23 +4838,23 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.2" thickBot="1">
+    <row r="1" spans="1:12" ht="16.5" thickBot="1">
       <c r="A1" s="31" t="s">
         <v>129</v>
       </c>
@@ -5214,7 +5154,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16.2" thickBot="1">
+    <row r="11" spans="1:12" ht="16.5" thickBot="1">
       <c r="A11" s="24"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -5392,7 +5332,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16.2" thickBot="1">
+    <row r="17" spans="1:12" ht="16.5" thickBot="1">
       <c r="A17" s="27">
         <v>8140</v>
       </c>
@@ -5436,9 +5376,9 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -5464,13 +5404,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.69921875" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" customWidth="1"/>
-    <col min="4" max="4" width="7.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5523,12 +5463,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="37.5" customWidth="1"/>
-    <col min="2" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
Regression updates - 103118
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0CB57986-583D-4CC7-8717-64E8C58FBBAB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{51439416-2828-43FB-82C7-2812D15E205A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="257">
   <si>
     <t>Username</t>
   </si>
@@ -1576,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2457,10 +2457,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2508,76 +2508,16 @@
         <v>217</v>
       </c>
       <c r="D3" s="50">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="52" t="s">
-        <v>202</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="D4" s="50">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="52" t="s">
-        <v>202</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="D5" s="50">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="52" t="s">
-        <v>202</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="D6" s="50">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="52" t="s">
-        <v>202</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="D7" s="50">
-        <v>456</v>
+        <v>931</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{6BD736EF-0A9A-4295-8C91-8829EF333F40}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{E95E0960-C996-46E2-9866-0BD7AB7CC179}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{EA87CDFC-A308-4C4B-ADBB-77FC9FB1D4AD}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{8CDD7FB9-12C9-4455-90DC-A90B840DD04A}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{D7F5E6CC-A0F8-4F23-9640-75AC5472D69E}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{95B0F34C-97F1-4D6B-8511-ABD88C5A833B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changes to Admin PayBy Check test Admin Enable les than 14 days Payment Terms Admin Search By payment id
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
+++ b/src/main/java/testdata/LoadPay/LoadPayTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION\SELENIUM\_Project\testing\SeleniumFramework\src\main\java\testdata\LoadPay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YuriiMerviak\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{51439416-2828-43FB-82C7-2812D15E205A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A7B2EB1B-1845-4D03-B241-93B1325646AF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="1000" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22980" windowHeight="8955" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlookLoginData" sheetId="8" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="257">
   <si>
     <t>Username</t>
   </si>
@@ -820,9 +820,6 @@
     <t>John Doe</t>
   </si>
   <si>
-    <t>Password@5</t>
-  </si>
-  <si>
     <t>123457</t>
   </si>
   <si>
@@ -884,6 +881,9 @@
   </si>
   <si>
     <t>w2k\</t>
+  </si>
+  <si>
+    <t>Password@6</t>
   </si>
 </sst>
 </file>
@@ -1576,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1596,7 +1596,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B2" s="48"/>
     </row>
@@ -1712,10 +1712,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="49" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="49" t="s">
         <v>245</v>
-      </c>
-      <c r="B1" s="49" t="s">
-        <v>246</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>174</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="57" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="57" t="s">
         <v>26</v>
@@ -1744,16 +1744,16 @@
         <v>29</v>
       </c>
       <c r="D2" s="56" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E2" s="50">
         <v>120.98</v>
       </c>
       <c r="F2" s="58" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G2" s="58" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -1786,10 +1786,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="49" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="49" t="s">
         <v>245</v>
-      </c>
-      <c r="B1" s="49" t="s">
-        <v>246</v>
       </c>
       <c r="C1" s="49" t="s">
         <v>174</v>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="57" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="57" t="s">
         <v>26</v>
@@ -1818,16 +1818,16 @@
         <v>29</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E2" s="50">
         <v>123.67</v>
       </c>
       <c r="F2" s="58" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G2" s="58" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -1861,10 +1861,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="49" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="49" t="s">
         <v>245</v>
-      </c>
-      <c r="B1" s="49" t="s">
-        <v>246</v>
       </c>
       <c r="C1" s="49" t="s">
         <v>174</v>
@@ -1884,16 +1884,16 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="57" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="57" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="D2" s="51" t="s">
         <v>253</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>254</v>
       </c>
       <c r="E2" s="50">
         <v>456.78</v>
@@ -1902,7 +1902,7 @@
         <v>789654123</v>
       </c>
       <c r="G2" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -1996,7 +1996,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2014,9 +2014,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="48" t="s">
-        <v>206</v>
-      </c>
+      <c r="A2" s="48"/>
       <c r="B2" s="48" t="s">
         <v>58</v>
       </c>
@@ -2459,8 +2457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2678,10 +2676,10 @@
         <v>218</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D4" s="50">
         <v>123.89</v>
@@ -2698,10 +2696,10 @@
         <v>218</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D5" s="50">
         <v>124</v>
@@ -3175,16 +3173,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C2" s="48" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D2" s="48" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -3324,10 +3322,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="52" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -3619,10 +3617,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C2" s="50">
         <v>8085</v>
@@ -3666,10 +3664,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C2" s="48" t="s">
         <v>66</v>
@@ -3722,10 +3720,10 @@
         <v>69</v>
       </c>
       <c r="C2" s="48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D2" s="48" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3769,16 +3767,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2" s="48" t="s">
         <v>238</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="D2" s="48" t="s">
         <v>238</v>
-      </c>
-      <c r="C2" s="48" t="s">
-        <v>239</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -3833,7 +3831,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3855,7 +3853,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>235</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -3985,7 +3983,7 @@
     </row>
     <row r="2" spans="1:9" s="54" customFormat="1">
       <c r="A2" s="55" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B2" s="55" t="s">
         <v>229</v>
@@ -4214,10 +4212,10 @@
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C2" s="50" t="s">
         <v>62</v>
@@ -4226,10 +4224,10 @@
         <v>100</v>
       </c>
       <c r="E2" s="50" t="s">
+        <v>241</v>
+      </c>
+      <c r="F2" s="50" t="s">
         <v>242</v>
-      </c>
-      <c r="F2" s="50" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -4775,7 +4773,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4834,7 +4832,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="32">
-        <v>32002</v>
+        <v>132000</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
@@ -5124,7 +5122,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="19">
-        <v>33343</v>
+        <v>191816</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
@@ -5154,7 +5152,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="24">
-        <v>33310</v>
+        <v>150892</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -5184,7 +5182,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="24">
-        <v>33558</v>
+        <v>214936</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -5214,7 +5212,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="24">
-        <v>33280</v>
+        <v>185836</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -5244,7 +5242,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="24">
-        <v>33307</v>
+        <v>214884</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -5274,7 +5272,7 @@
     </row>
     <row r="17" spans="1:12" ht="16.5" thickBot="1">
       <c r="A17" s="27">
-        <v>8140</v>
+        <v>158786</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>

</xml_diff>